<commit_message>
debug from 20240223 test
</commit_message>
<xml_diff>
--- a/Mould_Numeriacl_Calculation/Mould_Postison_Cal.xlsx
+++ b/Mould_Numeriacl_Calculation/Mould_Postison_Cal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user01\Documents\GitHub\mould\Mould_Numeriacl_Calculation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9499E92-4BE1-4D67-9451-4539D94E5097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{063DD12E-747B-441F-8A35-D11E41B76BE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="37710" windowHeight="21840" tabRatio="638" xr2:uid="{331D296A-DE97-4357-9338-22F5C8F49D08}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1055" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1060" uniqueCount="446">
   <si>
     <t>ジグの長さの半分</t>
     <rPh sb="3" eb="4">
@@ -12268,6 +12268,75 @@
     <t>トップ外削</t>
     <rPh sb="3" eb="5">
       <t>ガイサク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ジグ外幅の半分(G53B0Z方向)</t>
+    <rPh sb="2" eb="3">
+      <t>ガイ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ハバ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>ハンブン</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>ホウコウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ジグ内幅(ボルト締口までG53B0Y方向)</t>
+    <rPh sb="2" eb="3">
+      <t>ウチ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ハバ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>ホウコウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ジグ内幅(ボルト締口までG53B0X方向)</t>
+    <rPh sb="2" eb="3">
+      <t>ウチ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ハバ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>ホウコウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>その他</t>
+    <rPh sb="2" eb="3">
+      <t>タ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>固定用ボルト長X</t>
+    <rPh sb="0" eb="3">
+      <t>コテイヨウ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>チョウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>固定用ボルト長Y</t>
+    <rPh sb="0" eb="3">
+      <t>コテイヨウ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>チョウ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -12589,7 +12658,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -12776,22 +12845,287 @@
     <xf numFmtId="179" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="80">
+  <dxfs count="119">
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -13068,6 +13402,20 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -13660,14 +14008,12 @@
   <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:R182"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S39" sqref="S39"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="3.75" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.75" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.25" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="1.625" style="1" customWidth="1"/>
     <col min="5" max="5" width="4.125" style="3" bestFit="1" customWidth="1"/>
@@ -15639,7 +15985,7 @@
         <v>127</v>
       </c>
       <c r="H54" s="30">
-        <f>IF($C$25&gt;=$C$69-5,$N$82-$N$15, "-")</f>
+        <f>IF($C$25&gt;=$C$71-5,$N$82-$N$15, "-")</f>
         <v>3.5836378510248323</v>
       </c>
       <c r="K54" s="3">
@@ -15676,7 +16022,7 @@
         <v>127</v>
       </c>
       <c r="H55" s="30">
-        <f>IF($C$25&gt;=$C69-4,$N$83-$N$15, "-")</f>
+        <f>IF($C$25&gt;=$C71-4,$N$83-$N$15, "-")</f>
         <v>4.2564608749580657</v>
       </c>
       <c r="K55" s="3">
@@ -15710,7 +16056,7 @@
         <v>127</v>
       </c>
       <c r="H56" s="30">
-        <f>IF($C$25&gt;=$C$69-3,$N$84-$N$15, "-")</f>
+        <f>IF($C$25&gt;=$C$71-3,$N$84-$N$15, "-")</f>
         <v>4.8843832356542407</v>
       </c>
       <c r="K56" s="3">
@@ -15743,7 +16089,7 @@
         <v>127</v>
       </c>
       <c r="H57" s="30">
-        <f>IF($C$25&gt;=$C$69-2,$N$85-$N$15, "-")</f>
+        <f>IF($C$25&gt;=$C$71-2,$N$85-$N$15, "-")</f>
         <v>5.4674144162945595</v>
       </c>
       <c r="K57" s="3">
@@ -15776,7 +16122,7 @@
         <v>127</v>
       </c>
       <c r="H58" s="30" t="str">
-        <f>IF($C$25&gt;=$C69-1,$N$86-$N$15, "-")</f>
+        <f>IF($C$25&gt;=$C71-1,$N$86-$N$15, "-")</f>
         <v>-</v>
       </c>
       <c r="K58" s="3">
@@ -15804,7 +16150,7 @@
         <v>127</v>
       </c>
       <c r="H59" s="30" t="str">
-        <f>IF($C$25&gt;=$C69,$N$87-$N$15, "-")</f>
+        <f>IF($C$25&gt;=$C71,$N$87-$N$15, "-")</f>
         <v>-</v>
       </c>
       <c r="K59" s="3">
@@ -15859,7 +16205,7 @@
         <v>2</v>
       </c>
       <c r="B61" s="14" t="s">
-        <v>0</v>
+        <v>440</v>
       </c>
       <c r="C61" s="19">
         <v>330</v>
@@ -16174,10 +16520,10 @@
     </row>
     <row r="69" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B69" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="C69" s="38">
-        <v>8</v>
+        <v>441</v>
+      </c>
+      <c r="C69" s="19">
+        <v>251.90899999999999</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>349</v>
@@ -16213,6 +16559,12 @@
       </c>
     </row>
     <row r="70" spans="2:14" x14ac:dyDescent="0.4">
+      <c r="B70" s="14" t="s">
+        <v>442</v>
+      </c>
+      <c r="C70" s="19">
+        <v>244.4</v>
+      </c>
       <c r="E70" s="3" t="s">
         <v>306</v>
       </c>
@@ -16243,11 +16595,11 @@
       </c>
     </row>
     <row r="71" spans="2:14" x14ac:dyDescent="0.4">
-      <c r="B71" s="1" t="s">
-        <v>398</v>
-      </c>
-      <c r="C71" s="5">
-        <v>-561.11400000000003</v>
+      <c r="B71" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="C71" s="38">
+        <v>8</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>308</v>
@@ -16280,12 +16632,6 @@
       </c>
     </row>
     <row r="72" spans="2:14" x14ac:dyDescent="0.4">
-      <c r="B72" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="C72" s="5">
-        <v>-648.33199999999999</v>
-      </c>
       <c r="F72" s="10" t="s">
         <v>310</v>
       </c>
@@ -16312,6 +16658,12 @@
       </c>
     </row>
     <row r="73" spans="2:14" x14ac:dyDescent="0.4">
+      <c r="B73" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="C73" s="5">
+        <v>-561.11400000000003</v>
+      </c>
       <c r="E73" s="3" t="s">
         <v>323</v>
       </c>
@@ -16342,6 +16694,12 @@
       </c>
     </row>
     <row r="74" spans="2:14" x14ac:dyDescent="0.4">
+      <c r="B74" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="C74" s="5">
+        <v>-648.33199999999999</v>
+      </c>
       <c r="E74" s="3" t="s">
         <v>323</v>
       </c>
@@ -16551,7 +16909,7 @@
         <v>127</v>
       </c>
       <c r="H81" s="30">
-        <f ca="1">IF($C$25&gt;=$C$69-5,$H$54*$N$113-$C$20*$N$112, "-")</f>
+        <f ca="1">IF($C$25&gt;=$C$71-5,$H$54*$N$113-$C$20*$N$112, "-")</f>
         <v>0.23613623834420849</v>
       </c>
       <c r="K81" s="3">
@@ -16578,7 +16936,7 @@
         <v>127</v>
       </c>
       <c r="H82" s="30">
-        <f ca="1">IF($C$25&gt;=$C$69-4,$H$55*$N$113-($C$20+$C21)*$N$112, "-")</f>
+        <f ca="1">IF($C$25&gt;=$C$71-4,$H$55*$N$113-($C$20+$C21)*$N$112, "-")</f>
         <v>0.16515537313498907</v>
       </c>
       <c r="K82" s="3">
@@ -16606,7 +16964,7 @@
         <v>127</v>
       </c>
       <c r="H83" s="30">
-        <f ca="1">IF($C$25&gt;=$C$69-3,$H$56*$N$113-($C$20+2*$C$21)*$N$112, "-")</f>
+        <f ca="1">IF($C$25&gt;=$C$71-3,$H$56*$N$113-($C$20+2*$C$21)*$N$112, "-")</f>
         <v>4.930486789530697E-2</v>
       </c>
       <c r="K83" s="3">
@@ -16634,7 +16992,7 @@
         <v>127</v>
       </c>
       <c r="H84" s="30">
-        <f ca="1">IF($C$25&gt;=$C$69-2,$H$57*$N$113-($C$20+3*$C$21)*$N$112, "-")</f>
+        <f ca="1">IF($C$25&gt;=$C$71-2,$H$57*$N$113-($C$20+3*$C$21)*$N$112, "-")</f>
         <v>-0.11140580074584783</v>
       </c>
       <c r="K84" s="3">
@@ -16662,7 +17020,7 @@
         <v>127</v>
       </c>
       <c r="H85" s="30" t="str">
-        <f>IF($C$25&gt;=$C$69-1,$H$58*$N$113-($C$20+4*$C$21)*$N$112, "-")</f>
+        <f>IF($C$25&gt;=$C$71-1,$H$58*$N$113-($C$20+4*$C$21)*$N$112, "-")</f>
         <v>-</v>
       </c>
       <c r="K85" s="3">
@@ -16690,7 +17048,7 @@
         <v>127</v>
       </c>
       <c r="H86" s="30" t="str">
-        <f>IF($C$25&gt;=$C$69,$H$59*$N$113-($C$20+5*$C$21)*$N$112, "-")</f>
+        <f>IF($C$25&gt;=$C$71,$H$59*$N$113-($C$20+5*$C$21)*$N$112, "-")</f>
         <v>-</v>
       </c>
       <c r="K86" s="3">
@@ -16771,7 +17129,7 @@
         <v>124</v>
       </c>
       <c r="H89" s="30">
-        <f ca="1">IF($C$25&gt;=$C$69-5,$H$54*$N$112+$C$20*$N$113, "-")</f>
+        <f ca="1">IF($C$25&gt;=$C$71-5,$H$54*$N$112+$C$20*$N$113, "-")</f>
         <v>90.071009208980442</v>
       </c>
       <c r="K89" s="3">
@@ -16798,7 +17156,7 @@
         <v>124</v>
       </c>
       <c r="H90" s="30">
-        <f ca="1">IF($C$25&gt;=$C$69-4,$H$55*$N$112+($C$20+$C$21)*$N$113, "-")</f>
+        <f ca="1">IF($C$25&gt;=$C$71-4,$H$55*$N$112+($C$20+$C$21)*$N$113, "-")</f>
         <v>110.08219739305159</v>
       </c>
       <c r="K90" s="3">
@@ -16826,7 +17184,7 @@
         <v>124</v>
       </c>
       <c r="H91" s="30">
-        <f ca="1">IF($C$25&gt;=$C$69-3,$H$56*$N$112+($C$20+2*$C$21)*$N$113, "-")</f>
+        <f ca="1">IF($C$25&gt;=$C$71-3,$H$56*$N$112+($C$20+2*$C$21)*$N$113, "-")</f>
         <v>130.09171675638208</v>
       </c>
       <c r="K91" s="3">
@@ -16854,7 +17212,7 @@
         <v>124</v>
       </c>
       <c r="H92" s="30">
-        <f ca="1">IF($C$25&gt;=$C$69-2,$H$57*$N$112+($C$20+3*$C$21)*$N$113, "-")</f>
+        <f ca="1">IF($C$25&gt;=$C$71-2,$H$57*$N$112+($C$20+3*$C$21)*$N$113, "-")</f>
         <v>150.09956765143286</v>
       </c>
       <c r="K92" s="3">
@@ -16882,7 +17240,7 @@
         <v>124</v>
       </c>
       <c r="H93" s="30" t="str">
-        <f>IF($C$25&gt;=$C$69-1,$H$58*$N$112+($C$20+4*$C$21)*$N$113, "-")</f>
+        <f>IF($C$25&gt;=$C$71-1,$H$58*$N$112+($C$20+4*$C$21)*$N$113, "-")</f>
         <v>-</v>
       </c>
       <c r="K93" s="3">
@@ -16910,7 +17268,7 @@
         <v>124</v>
       </c>
       <c r="H94" s="30" t="str">
-        <f>IF($C$25&gt;=$C$69-0,$H$59*$N$112+($C$20+5*$C$21)*$N$113, "-")</f>
+        <f>IF($C$25&gt;=$C$71-0,$H$59*$N$112+($C$20+5*$C$21)*$N$113, "-")</f>
         <v>-</v>
       </c>
       <c r="K94" s="3">
@@ -17012,7 +17370,7 @@
         <v>127</v>
       </c>
       <c r="H98" s="30">
-        <f>$C$71-$C66</f>
+        <f>$C$73-$C66</f>
         <v>-11.095000000000027</v>
       </c>
       <c r="I98" s="30">
@@ -17208,6 +17566,11 @@
       </c>
     </row>
     <row r="105" spans="5:14" x14ac:dyDescent="0.4">
+      <c r="F105" s="34" t="s">
+        <v>443</v>
+      </c>
+      <c r="G105" s="28"/>
+      <c r="H105" s="28"/>
       <c r="K105" s="3">
         <f t="shared" si="2"/>
         <v>105</v>
@@ -17224,6 +17587,11 @@
       </c>
     </row>
     <row r="106" spans="5:14" x14ac:dyDescent="0.4">
+      <c r="F106" s="9" t="s">
+        <v>445</v>
+      </c>
+      <c r="G106" s="62"/>
+      <c r="H106" s="13"/>
       <c r="K106" s="3">
         <f t="shared" si="2"/>
         <v>106</v>
@@ -17240,6 +17608,11 @@
       </c>
     </row>
     <row r="107" spans="5:14" x14ac:dyDescent="0.4">
+      <c r="F107" s="9" t="s">
+        <v>444</v>
+      </c>
+      <c r="G107" s="62"/>
+      <c r="H107" s="13"/>
       <c r="K107" s="3">
         <f t="shared" si="2"/>
         <v>107</v>
@@ -18195,196 +18568,196 @@
   </sheetData>
   <phoneticPr fontId="1"/>
   <conditionalFormatting sqref="C3">
-    <cfRule type="expression" dxfId="79" priority="124">
+    <cfRule type="expression" dxfId="77" priority="124">
       <formula>$C$3&gt;2*N163</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4">
-    <cfRule type="expression" dxfId="78" priority="44">
+    <cfRule type="expression" dxfId="76" priority="44">
       <formula>C4&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6">
-    <cfRule type="expression" dxfId="77" priority="20">
+    <cfRule type="expression" dxfId="75" priority="20">
       <formula>$C$6&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="expression" dxfId="76" priority="48">
+    <cfRule type="expression" dxfId="74" priority="48">
       <formula>$C$9&lt;=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10:C11">
-    <cfRule type="expression" dxfId="75" priority="21">
+    <cfRule type="expression" dxfId="73" priority="21">
       <formula>$C$10&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="expression" dxfId="74" priority="99">
+    <cfRule type="expression" dxfId="72" priority="99">
       <formula>OR(C15&lt;=0, C15&gt;Q2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="expression" dxfId="73" priority="43">
+    <cfRule type="expression" dxfId="71" priority="43">
       <formula>C35&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="expression" dxfId="72" priority="58">
+    <cfRule type="expression" dxfId="70" priority="58">
       <formula>OR($C$36&lt;0, $C$36&gt;=$C$9)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="expression" dxfId="71" priority="17">
+    <cfRule type="expression" dxfId="69" priority="17">
       <formula>OR($C$37&lt;0, $C$37&gt;=$C$10)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38">
-    <cfRule type="expression" dxfId="70" priority="121">
+    <cfRule type="expression" dxfId="68" priority="121">
       <formula>OR(C38&lt;0, C38&gt;=C9)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="expression" dxfId="69" priority="128">
+    <cfRule type="expression" dxfId="67" priority="128">
       <formula>OR(C41&lt;0, C41&gt;=C4)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44">
-    <cfRule type="expression" dxfId="68" priority="129">
+    <cfRule type="expression" dxfId="66" priority="129">
       <formula>OR(C44&lt;0, C44&gt;=C4)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="expression" dxfId="67" priority="52">
+    <cfRule type="expression" dxfId="65" priority="52">
       <formula>AND(C61&lt;&gt;330, C61&lt;&gt;270, C61&lt;&gt;250)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="expression" dxfId="66" priority="51">
+    <cfRule type="expression" dxfId="64" priority="51">
       <formula>C62&lt;&gt;40</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C65">
-    <cfRule type="expression" dxfId="65" priority="28">
+    <cfRule type="expression" dxfId="63" priority="28">
       <formula>OR(C65&gt;0, ABS(ABS(C65)-740)&gt;=1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C66">
-    <cfRule type="expression" dxfId="64" priority="41">
+    <cfRule type="expression" dxfId="62" priority="41">
       <formula>OR(C66&gt;0, ABS(ABS(C66)-550)&gt;=1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C67">
-    <cfRule type="expression" dxfId="63" priority="34">
+    <cfRule type="expression" dxfId="61" priority="34">
       <formula>OR(C67&gt;0, ABS(ABS(C67)-1150)&gt;=1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C68">
-    <cfRule type="expression" dxfId="62" priority="40">
+    <cfRule type="expression" dxfId="60" priority="40">
       <formula>OR(ABS(C68)&gt;=0.2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H48">
-    <cfRule type="expression" dxfId="61" priority="24">
+    <cfRule type="expression" dxfId="59" priority="24">
       <formula>OR($H$48&lt;=1, INT($H$48)&lt;&gt;$H$48)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H52">
-    <cfRule type="expression" dxfId="60" priority="16">
+    <cfRule type="expression" dxfId="58" priority="16">
       <formula>ISERROR(INDIRECT($H$52&amp;"!$G$45"))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25">
-    <cfRule type="expression" dxfId="59" priority="237">
-      <formula>OR(C25-QUOTIENT(C25,1)&lt;&gt;0, C25&lt;0, C25&gt;$C$69)</formula>
+    <cfRule type="expression" dxfId="57" priority="237">
+      <formula>OR(C25-QUOTIENT(C25,1)&lt;&gt;0, C25&lt;0, C25&gt;$C$71)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H50">
-    <cfRule type="expression" dxfId="58" priority="12">
+    <cfRule type="expression" dxfId="56" priority="12">
       <formula>OR($H$50&lt;1, INT($H$50)&lt;&gt;$H$50)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H51">
-    <cfRule type="expression" dxfId="57" priority="11">
+    <cfRule type="expression" dxfId="55" priority="11">
       <formula>OR($H$51&lt;0, INT($H$51)&lt;&gt;$H$51)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23">
-    <cfRule type="expression" dxfId="56" priority="255">
+    <cfRule type="expression" dxfId="54" priority="255">
       <formula>OR($C$23&lt;=0, MOD($C$23,$C$22)&lt;&gt;0, $C$23&gt;=#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26">
-    <cfRule type="expression" dxfId="55" priority="263">
+    <cfRule type="expression" dxfId="53" priority="263">
       <formula>OR($C$26&lt;=0, $C$26&gt;=MIN($C$23, $C$24))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N140:N145">
-    <cfRule type="expression" dxfId="54" priority="10">
+    <cfRule type="expression" dxfId="52" priority="10">
       <formula>$H$51&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N146:N153">
-    <cfRule type="expression" dxfId="53" priority="9">
+    <cfRule type="expression" dxfId="51" priority="9">
       <formula>$H$51&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="expression" dxfId="52" priority="275">
+    <cfRule type="expression" dxfId="50" priority="275">
       <formula>OR(C16&lt;=0, C16+C15&gt;Q2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="expression" dxfId="51" priority="4">
+    <cfRule type="expression" dxfId="49" priority="4">
       <formula>G1="X"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="5">
+    <cfRule type="expression" dxfId="48" priority="5">
       <formula>G1="Y"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="6">
+    <cfRule type="expression" dxfId="47" priority="6">
       <formula>G1="Z"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="7">
+    <cfRule type="expression" dxfId="46" priority="7">
       <formula>G1="B"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H81:H96">
-    <cfRule type="expression" dxfId="47" priority="3">
+    <cfRule type="expression" dxfId="45" priority="3">
       <formula>$H$51&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="expression" dxfId="46" priority="279">
+    <cfRule type="expression" dxfId="44" priority="279">
       <formula>OR($C$17&lt;=0, $C$17&gt;=($C$9-#REF!)/2, $C$17&gt;=($C$36-#REF!)/2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H77">
-    <cfRule type="expression" dxfId="45" priority="280">
+    <cfRule type="expression" dxfId="43" priority="280">
       <formula>$H$77&lt;=$C$27/2+$C$28</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27">
-    <cfRule type="expression" dxfId="44" priority="2">
+    <cfRule type="expression" dxfId="42" priority="2">
       <formula>OR($C$27&lt;=0, $C$27&gt;$C$26)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H49">
-    <cfRule type="expression" dxfId="43" priority="1">
+    <cfRule type="expression" dxfId="41" priority="1">
       <formula>OR($H$49&lt;0, INT($H$49)&lt;&gt;$H$49)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="expression" dxfId="42" priority="285">
+    <cfRule type="expression" dxfId="40" priority="285">
       <formula>OR($C$13&gt;=$C$9, $C$13&gt;=$C$42)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="expression" dxfId="41" priority="286">
+    <cfRule type="expression" dxfId="39" priority="286">
       <formula>OR($C$14&gt;=$C$10, $C$14&gt;=$C$42)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation imeMode="disabled" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C60:C69 H79 N140:N153 C49:C52 C55:C58 H54:H72 H81:H96 C3:C32 G1:G1048576" xr:uid="{5A8FA8E9-E7FC-48D2-B40E-E90D3C7D1F03}"/>
+    <dataValidation imeMode="disabled" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H79 N140:N153 C49:C52 C55:C58 H54:H72 H81:H96 C3:C32 C60:C71 G1:G1048576" xr:uid="{5A8FA8E9-E7FC-48D2-B40E-E90D3C7D1F03}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -22693,191 +23066,191 @@
   </sheetData>
   <phoneticPr fontId="1"/>
   <conditionalFormatting sqref="C3">
-    <cfRule type="expression" dxfId="40" priority="29">
+    <cfRule type="expression" dxfId="118" priority="29">
       <formula>$C$3&gt;2*N151</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4">
-    <cfRule type="expression" dxfId="39" priority="22">
+    <cfRule type="expression" dxfId="117" priority="22">
       <formula>C4&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6">
-    <cfRule type="expression" dxfId="38" priority="14">
+    <cfRule type="expression" dxfId="116" priority="14">
       <formula>$C$6&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="expression" dxfId="37" priority="23">
+    <cfRule type="expression" dxfId="115" priority="23">
       <formula>$C$9&lt;=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10:C11">
-    <cfRule type="expression" dxfId="36" priority="15">
+    <cfRule type="expression" dxfId="114" priority="15">
       <formula>$C$10&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="expression" dxfId="35" priority="27">
+    <cfRule type="expression" dxfId="113" priority="27">
       <formula>OR(C15&lt;=0, C15&gt;Q2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="expression" dxfId="34" priority="21">
+    <cfRule type="expression" dxfId="112" priority="21">
       <formula>C35&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="expression" dxfId="33" priority="26">
+    <cfRule type="expression" dxfId="111" priority="26">
       <formula>OR($C$36&lt;0, $C$36&gt;=$C$9)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="expression" dxfId="32" priority="13">
+    <cfRule type="expression" dxfId="110" priority="13">
       <formula>OR($C$37&lt;0, $C$37&gt;=$C$10)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38">
-    <cfRule type="expression" dxfId="31" priority="28">
+    <cfRule type="expression" dxfId="109" priority="28">
       <formula>OR(C38&lt;0, C38&gt;=C9)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C39">
-    <cfRule type="expression" dxfId="30" priority="30">
+    <cfRule type="expression" dxfId="108" priority="30">
       <formula>OR(C39&lt;0, C39&gt;=C4)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="expression" dxfId="29" priority="31">
+    <cfRule type="expression" dxfId="107" priority="31">
       <formula>OR(C42&lt;0, C42&gt;=C4)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="expression" dxfId="28" priority="25">
+    <cfRule type="expression" dxfId="106" priority="25">
       <formula>AND(C59&lt;&gt;330, C59&lt;&gt;270, C59&lt;&gt;250)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="expression" dxfId="27" priority="24">
+    <cfRule type="expression" dxfId="105" priority="24">
       <formula>C60&lt;&gt;40</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C63">
-    <cfRule type="expression" dxfId="26" priority="17">
+    <cfRule type="expression" dxfId="104" priority="17">
       <formula>OR(C63&gt;0, ABS(ABS(C63)-740)&gt;=1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C64">
-    <cfRule type="expression" dxfId="25" priority="20">
+    <cfRule type="expression" dxfId="103" priority="20">
       <formula>OR(C64&gt;0, ABS(ABS(C64)-550)&gt;=1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C65">
-    <cfRule type="expression" dxfId="24" priority="18">
+    <cfRule type="expression" dxfId="102" priority="18">
       <formula>OR(C65&gt;0, ABS(ABS(C65)-1150)&gt;=1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C66">
-    <cfRule type="expression" dxfId="23" priority="19">
+    <cfRule type="expression" dxfId="101" priority="19">
       <formula>OR(ABS(C66)&gt;=0.2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H48">
-    <cfRule type="expression" dxfId="22" priority="16">
+    <cfRule type="expression" dxfId="100" priority="16">
       <formula>OR($H$48&lt;=1, INT($H$48)&lt;&gt;$H$48)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H52">
-    <cfRule type="expression" dxfId="21" priority="12">
+    <cfRule type="expression" dxfId="99" priority="12">
       <formula>ISERROR(INDIRECT($H$52&amp;"!$G$45"))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25">
-    <cfRule type="expression" dxfId="20" priority="32">
+    <cfRule type="expression" dxfId="98" priority="32">
       <formula>OR(C25-QUOTIENT(C25,1)&lt;&gt;0, C25&lt;0, C25&gt;$C$67)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H50">
-    <cfRule type="expression" dxfId="19" priority="11">
+    <cfRule type="expression" dxfId="97" priority="11">
       <formula>OR($H$50&lt;1, INT($H$50)&lt;&gt;$H$50)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H51">
-    <cfRule type="expression" dxfId="18" priority="10">
+    <cfRule type="expression" dxfId="96" priority="10">
       <formula>OR($H$51&lt;0, INT($H$51)&lt;&gt;$H$51)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23">
-    <cfRule type="expression" dxfId="17" priority="33">
+    <cfRule type="expression" dxfId="95" priority="33">
       <formula>OR($C$23&lt;=0, MOD($C$23,$C$22)&lt;&gt;0, $C$23&gt;=#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26">
-    <cfRule type="expression" dxfId="16" priority="34">
+    <cfRule type="expression" dxfId="94" priority="34">
       <formula>OR($C$26&lt;=0, $C$26&gt;=MIN($C$23, $C$24))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N128:N133">
-    <cfRule type="expression" dxfId="15" priority="9">
+    <cfRule type="expression" dxfId="93" priority="9">
       <formula>$H$51&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N134:N141">
-    <cfRule type="expression" dxfId="14" priority="8">
+    <cfRule type="expression" dxfId="92" priority="8">
       <formula>$H$51&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="expression" dxfId="13" priority="35">
+    <cfRule type="expression" dxfId="91" priority="35">
       <formula>OR(C16&lt;=0, C16+C15&gt;Q2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="expression" dxfId="12" priority="4">
+    <cfRule type="expression" dxfId="90" priority="4">
       <formula>G1="X"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="5">
+    <cfRule type="expression" dxfId="89" priority="5">
       <formula>G1="Y"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="6">
+    <cfRule type="expression" dxfId="88" priority="6">
       <formula>G1="Z"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="7">
+    <cfRule type="expression" dxfId="87" priority="7">
       <formula>G1="B"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H81:H96">
-    <cfRule type="expression" dxfId="8" priority="3">
+    <cfRule type="expression" dxfId="86" priority="3">
       <formula>$H$51&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="expression" dxfId="7" priority="36">
+    <cfRule type="expression" dxfId="85" priority="36">
       <formula>OR($C$13&gt;=$C$9, $C$13&gt;=$C$40)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="expression" dxfId="6" priority="37">
+    <cfRule type="expression" dxfId="84" priority="37">
       <formula>OR($C$14&gt;=$C$10, $C$14&gt;=$C$40)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="expression" dxfId="5" priority="38">
+    <cfRule type="expression" dxfId="83" priority="38">
       <formula>OR($C$17&lt;=0, $C$17&gt;=($C$9-#REF!)/2, $C$17&gt;=($C$36-#REF!)/2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H77">
-    <cfRule type="expression" dxfId="4" priority="39">
+    <cfRule type="expression" dxfId="82" priority="39">
       <formula>$H$77&lt;=$C$27/2+$C$28</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27">
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="81" priority="2">
       <formula>OR($C$27&lt;=0, $C$27&gt;$C$26)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H49">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="80" priority="1">
       <formula>OR($H$49&lt;0, INT($H$49)&lt;&gt;$H$49)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -25053,12 +25426,12 @@
   </sheetData>
   <phoneticPr fontId="1"/>
   <conditionalFormatting sqref="B2:D42">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="79" priority="2">
       <formula>$A2&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:N42">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="78" priority="1">
       <formula>$A2&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
debug from 20240228 test
</commit_message>
<xml_diff>
--- a/Mould_Numeriacl_Calculation/Mould_Postison_Cal.xlsx
+++ b/Mould_Numeriacl_Calculation/Mould_Postison_Cal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user01\Documents\GitHub\mould\Mould_Numeriacl_Calculation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6721E62F-4C02-4611-88B3-DCAB02B6F744}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E06768-10F1-405A-9559-32DA4A69262A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="37710" windowHeight="21840" tabRatio="638" activeTab="1" xr2:uid="{331D296A-DE97-4357-9338-22F5C8F49D08}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1095" uniqueCount="445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1098" uniqueCount="450">
   <si>
     <t>受板の長さ</t>
     <rPh sb="0" eb="1">
@@ -12328,6 +12328,208 @@
     <rPh sb="6" eb="7">
       <t>チョウ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ジグ外幅の半分(G53B0Z方向TOP)</t>
+    <rPh sb="2" eb="3">
+      <t>ガイ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ハバ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>ハンブン</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>ホウコウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ジグ外幅の半分(G53B0Z方向BOT)</t>
+    <rPh sb="2" eb="3">
+      <t>ガイ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ハバ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>ハンブン</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>ホウコウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ボトム 内面取 長さ</t>
+    <rPh sb="4" eb="5">
+      <t>ウチ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>メントリ</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>ナガ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ボトム 外面取 長さ</t>
+    <rPh sb="4" eb="5">
+      <t>ソト</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>メントリ</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>ナガ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>sqrt{R</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>c</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>-(f</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>b</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>-C49)</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>}-sqrt(R</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>c</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>-f</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>b</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>)</t>
+    </r>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -12843,6 +13045,20 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -13113,20 +13329,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -18477,10 +18679,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{925B1691-9EED-4AA0-BD13-7D19A44326F8}">
-  <dimension ref="A1:R182"/>
+  <dimension ref="A1:R183"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.4"/>
@@ -18553,12 +18755,12 @@
         <v>58</v>
       </c>
       <c r="Q2" s="10">
-        <f>C4+N166</f>
-        <v>500.00000001278181</v>
+        <f>C4+N167</f>
+        <v>499.92803488790344</v>
       </c>
       <c r="R2" s="10">
         <f>C67+Q2</f>
-        <v>-649.97399998721812</v>
+        <v>-650.0459651120965</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="15" thickTop="1" x14ac:dyDescent="0.4">
@@ -18582,14 +18784,14 @@
       </c>
       <c r="H3" s="30">
         <f>$C$4+$N$13*$N$5</f>
-        <v>500.01603829462465</v>
+        <v>500.0159494817317</v>
       </c>
       <c r="I3" s="30">
         <f>$C$67+H3</f>
-        <v>-649.95796170537528</v>
+        <v>-649.95805051826824</v>
       </c>
       <c r="K3" s="3">
-        <f t="shared" ref="K3:K75" si="0">ROW(K3)</f>
+        <f t="shared" ref="K3:K76" si="0">ROW(K3)</f>
         <v>3</v>
       </c>
       <c r="L3" s="45" t="s">
@@ -18600,18 +18802,18 @@
       </c>
       <c r="N3" s="2">
         <f>ASIN($N$14)</f>
-        <v>1.1203216917671469E-2</v>
+        <v>1.1203226866402047E-2</v>
       </c>
       <c r="P3" s="9" t="s">
         <v>59</v>
       </c>
       <c r="Q3" s="10">
         <f>C4+C5-Q2</f>
-        <v>499.99999998721819</v>
+        <v>500.07196511209656</v>
       </c>
       <c r="R3" s="10">
         <f>C67+Q3</f>
-        <v>-649.97400001278174</v>
+        <v>-649.90203488790337</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.4">
@@ -18635,11 +18837,11 @@
       </c>
       <c r="H4" s="30">
         <f>$C$4+$C$5-$H$3</f>
-        <v>499.98396170537535</v>
+        <v>499.9840505182683</v>
       </c>
       <c r="I4" s="30">
         <f>$C$67+H4</f>
-        <v>-649.99003829462458</v>
+        <v>-649.98994948173163</v>
       </c>
       <c r="K4" s="3">
         <f t="shared" si="0"/>
@@ -18653,14 +18855,14 @@
       </c>
       <c r="N4" s="2">
         <f>DEGREES($N$3)</f>
-        <v>0.64189704635213818</v>
+        <v>0.64189761637241194</v>
       </c>
       <c r="P4" s="9" t="s">
         <v>60</v>
       </c>
       <c r="Q4" s="10">
         <f>Q2-C61</f>
-        <v>170.00000001278181</v>
+        <v>169.70503488790342</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.4">
@@ -18682,7 +18884,7 @@
       </c>
       <c r="H5" s="30">
         <f>$H$3-$C$61</f>
-        <v>170.01603829462465</v>
+        <v>169.79294948173168</v>
       </c>
       <c r="K5" s="3">
         <f t="shared" si="0"/>
@@ -18700,7 +18902,7 @@
       </c>
       <c r="Q5" s="10">
         <f>Q3-C61</f>
-        <v>169.99999998721819</v>
+        <v>169.84896511209655</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.4">
@@ -18719,7 +18921,7 @@
       </c>
       <c r="H6" s="50">
         <f>$H$4-$C$61</f>
-        <v>169.98396170537535</v>
+        <v>169.76105051826829</v>
       </c>
       <c r="K6" s="3">
         <f t="shared" si="0"/>
@@ -18736,8 +18938,8 @@
         <v>28</v>
       </c>
       <c r="Q6" s="18">
-        <f>N161-N162</f>
-        <v>7.1067335242896661</v>
+        <f>N162-N163</f>
+        <v>7.1118522502201813</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.4">
@@ -18769,7 +18971,7 @@
       </c>
       <c r="N7" s="2">
         <f>SQRT($N$8^2-$N$9^2)</f>
-        <v>8724.6943808938086</v>
+        <v>8724.6864545535973</v>
       </c>
       <c r="P7" s="17" t="s">
         <v>73</v>
@@ -18819,12 +19021,12 @@
         <v>62</v>
       </c>
       <c r="Q8" s="10">
-        <f>-C64+(N16+N17)/2+C6/2-N165</f>
-        <v>-8.3385574269177596</v>
+        <f>-C64+(N16+N17)/2+C6/2-N166</f>
+        <v>-8.3314551675721304</v>
       </c>
       <c r="R8" s="10">
         <f t="shared" ref="R8:R14" si="1">$C$66+Q8</f>
-        <v>-558.35755742691777</v>
+        <v>-558.35045516757214</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.4">
@@ -18849,18 +19051,18 @@
       </c>
       <c r="N9" s="2">
         <f>$C$61-$C$62/2</f>
-        <v>310</v>
+        <v>310.22300000000001</v>
       </c>
       <c r="P9" s="9" t="s">
         <v>16</v>
       </c>
       <c r="Q9" s="10">
-        <f>-C64+N15+C6/2-N165</f>
-        <v>-8.337590837638345</v>
+        <f>-C64+N15+C6/2-N166</f>
+        <v>-8.3304885782927158</v>
       </c>
       <c r="R9" s="10">
         <f t="shared" si="1"/>
-        <v>-558.35659083763835</v>
+        <v>-558.34948857829272</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.4">
@@ -18893,12 +19095,12 @@
         <v>63</v>
       </c>
       <c r="Q10" s="10">
-        <f>C64-(N19+N20)/2-C6/2+N165</f>
-        <v>19.565491184843268</v>
+        <f>C64-(N19+N20)/2-C6/2+N166</f>
+        <v>19.558388925497638</v>
       </c>
       <c r="R10" s="10">
         <f t="shared" si="1"/>
-        <v>-530.45350881515674</v>
+        <v>-530.46061107450237</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.4">
@@ -18932,12 +19134,12 @@
         <v>19</v>
       </c>
       <c r="Q11" s="10">
-        <f>C64-N18-C6/2+N165</f>
-        <v>19.56330812012493</v>
+        <f>C64-N18-C6/2+N166</f>
+        <v>19.556205860779301</v>
       </c>
       <c r="R11" s="10">
         <f t="shared" si="1"/>
-        <v>-530.45569187987508</v>
+        <v>-530.4627941392207</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.4">
@@ -18955,11 +19157,11 @@
       </c>
       <c r="H12" s="30">
         <f>$N$21-$N$13*$N$6</f>
-        <v>-11.905406231671805</v>
+        <v>-11.897480389039629</v>
       </c>
       <c r="I12" s="30">
         <f>$C$66+H12</f>
-        <v>-561.92440623167181</v>
+        <v>-561.91648038903963</v>
       </c>
       <c r="K12" s="3">
         <f t="shared" si="0"/>
@@ -18979,7 +19181,7 @@
         <v>71</v>
       </c>
       <c r="Q12" s="10" t="e">
-        <f>C64-(N19+N20)/2-C6/2+N165-#REF!/2-C35+C36/2</f>
+        <f>C64-(N19+N20)/2-C6/2+N166-#REF!/2-C35+C36/2</f>
         <v>#REF!</v>
       </c>
       <c r="R12" s="10" t="e">
@@ -19002,11 +19204,11 @@
       </c>
       <c r="H13" s="30">
         <f>$N$13*$N$6-$N$22</f>
-        <v>23.132339989597313</v>
+        <v>23.124414146965137</v>
       </c>
       <c r="I13" s="30">
         <f>$C$66+H13</f>
-        <v>-526.88666001040269</v>
+        <v>-526.89458585303487</v>
       </c>
       <c r="K13" s="3">
         <f t="shared" si="0"/>
@@ -19020,7 +19222,7 @@
       </c>
       <c r="N13" s="2">
         <f>$C$64+$N$7</f>
-        <v>8926.1943808938086</v>
+        <v>8926.1864545535973</v>
       </c>
       <c r="P13" s="9" t="s">
         <v>66</v>
@@ -19049,11 +19251,11 @@
       </c>
       <c r="H14" s="30">
         <f>$N$15-$N$13*$N$6</f>
-        <v>-11.90443964239239</v>
+        <v>-11.896513799760214</v>
       </c>
       <c r="I14" s="30">
         <f>$C$66+H14</f>
-        <v>-561.9234396423924</v>
+        <v>-561.91551379976022</v>
       </c>
       <c r="K14" s="3">
         <f t="shared" si="0"/>
@@ -19067,13 +19269,13 @@
       </c>
       <c r="N14" s="2">
         <f>$N$12/$N$13</f>
-        <v>1.1202982562652493E-2</v>
+        <v>1.1202992510758734E-2</v>
       </c>
       <c r="P14" s="9" t="s">
         <v>67</v>
       </c>
       <c r="Q14" s="10" t="e">
-        <f>-C64+(N16+N17)/2+C6/2-N165+#REF!/2+C41-C42/2</f>
+        <f>-C64+(N16+N17)/2+C6/2-N166+#REF!/2+C41-C42/2</f>
         <v>#REF!</v>
       </c>
       <c r="R14" s="10" t="e">
@@ -19100,11 +19302,11 @@
       </c>
       <c r="H15" s="30">
         <f>$N$13*$N$6-$N$18</f>
-        <v>23.130156924878975</v>
+        <v>23.122231082246799</v>
       </c>
       <c r="I15" s="30">
         <f>$C$66+H15</f>
-        <v>-526.88884307512103</v>
+        <v>-526.89676891775321</v>
       </c>
       <c r="K15" s="3">
         <f t="shared" si="0"/>
@@ -19197,12 +19399,12 @@
         <v>51</v>
       </c>
       <c r="Q17" s="10">
-        <f>N28-C64+C6/2-N165</f>
-        <v>-7.6307545676227164</v>
+        <f>N28-C64+C6/2-N166</f>
+        <v>-7.6236523082770873</v>
       </c>
       <c r="R17" s="10">
         <f>$C$66+Q17</f>
-        <v>-557.64975456762272</v>
+        <v>-557.64265230827709</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.4">
@@ -19260,7 +19462,7 @@
       </c>
       <c r="H19" s="30">
         <f>-$C$36/2+$C$35-$C$31</f>
-        <v>-76.724999999999994</v>
+        <v>-77.384999999999991</v>
       </c>
       <c r="I19" s="52"/>
       <c r="K19" s="3">
@@ -19281,12 +19483,12 @@
         <v>45</v>
       </c>
       <c r="Q19" s="10">
-        <f>N29-C17-C13/2+N167-N13</f>
-        <v>-7.6318892500185029</v>
+        <f>N29-C17-C13/2+N168-N13</f>
+        <v>-7.6247869906728738</v>
       </c>
       <c r="R19" s="10">
         <f>$C$66+Q19</f>
-        <v>-557.65088925001851</v>
+        <v>-557.64378699067288</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.4">
@@ -19307,12 +19509,12 @@
         <v>126</v>
       </c>
       <c r="H20" s="30">
-        <f ca="1">$H$13-$H$18/2-$C$35+$C$42/2</f>
-        <v>22.287339989597314</v>
+        <f ca="1">$H$13-$N$42-$H$18/2-$C$31-$C$35+$C$42/2</f>
+        <v>22.201087937634938</v>
       </c>
       <c r="I20" s="30">
         <f ca="1">$C$66+H20</f>
-        <v>-527.73166001040272</v>
+        <v>-527.81791206236505</v>
       </c>
       <c r="K20" s="3">
         <f t="shared" si="0"/>
@@ -19333,11 +19535,11 @@
       </c>
       <c r="Q20" s="10">
         <f>Q3-Q16</f>
-        <v>483.9249999872182</v>
+        <v>483.99696511209658</v>
       </c>
       <c r="R20" s="10">
         <f>C67+Q20</f>
-        <v>-666.04900001278179</v>
+        <v>-665.9770348879033</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.4">
@@ -19359,11 +19561,11 @@
       </c>
       <c r="H21" s="30">
         <f ca="1">-$H$20+$C$46</f>
-        <v>-11.287339989597314</v>
+        <v>-11.201087937634938</v>
       </c>
       <c r="I21" s="30">
         <f ca="1">$C$66+H21</f>
-        <v>-561.30633998959729</v>
+        <v>-561.22008793763496</v>
       </c>
       <c r="K21" s="3">
         <f t="shared" si="0"/>
@@ -19472,7 +19674,7 @@
         <v>68</v>
       </c>
       <c r="Q23" s="10">
-        <f ca="1">DEGREES($N$66)</f>
+        <f ca="1">DEGREES($N$67)</f>
         <v>859.43669269623479</v>
       </c>
     </row>
@@ -19494,11 +19696,11 @@
       </c>
       <c r="H24" s="30">
         <f ca="1">-$N$13*$N$6+$N$21+$H$22/2+$C$41-$C$42/2</f>
-        <v>-11.203906231671795</v>
+        <v>-11.195980389039619</v>
       </c>
       <c r="I24" s="30">
         <f ca="1">$C$66+H24</f>
-        <v>-561.2229062316718</v>
+        <v>-561.21498038903962</v>
       </c>
       <c r="K24" s="3">
         <f t="shared" si="0"/>
@@ -19518,8 +19720,8 @@
         <v>69</v>
       </c>
       <c r="Q24" s="10">
-        <f ca="1">Q9*$N$107+Q2*$N$74</f>
-        <v>-70046.624280368822</v>
+        <f ca="1">Q9*$N$108+Q2*$N$75</f>
+        <v>-69983.416521525956</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.4">
@@ -19540,11 +19742,11 @@
       </c>
       <c r="H25" s="30">
         <f>$H$3-$C$43</f>
-        <v>468.01603829462465</v>
+        <v>468.0159494817317</v>
       </c>
       <c r="I25" s="30">
         <f>$C$67+H25</f>
-        <v>-681.95796170537528</v>
+        <v>-681.95805051826824</v>
       </c>
       <c r="K25" s="3">
         <f t="shared" si="0"/>
@@ -19564,8 +19766,8 @@
         <v>70</v>
       </c>
       <c r="Q25" s="10">
-        <f ca="1">-Q$9*$N$74+Q$2*$N$107</f>
-        <v>4500581.5260234261</v>
+        <f ca="1">-Q$9*$N$75+Q$2*$N$108</f>
+        <v>4499933.6971780732</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.4">
@@ -19583,11 +19785,11 @@
       </c>
       <c r="H26" s="30">
         <f>$H$4-$C$38</f>
-        <v>474.98396170537535</v>
+        <v>474.9840505182683</v>
       </c>
       <c r="I26" s="30">
         <f>$C$67+H26</f>
-        <v>-674.99003829462458</v>
+        <v>-674.98994948173163</v>
       </c>
       <c r="K26" s="3">
         <f t="shared" si="0"/>
@@ -19669,11 +19871,11 @@
       </c>
       <c r="H29" s="30">
         <f>$H$3-$C$15</f>
-        <v>487.96603829462464</v>
+        <v>487.96594948173168</v>
       </c>
       <c r="I29" s="30">
         <f>$C$67+H29</f>
-        <v>-662.00796170537524</v>
+        <v>-662.00805051826819</v>
       </c>
       <c r="K29" s="3">
         <f t="shared" si="0"/>
@@ -19703,11 +19905,11 @@
       </c>
       <c r="H30" s="30">
         <f>$H$29-$C$16</f>
-        <v>479.91603829462463</v>
+        <v>479.91594948173167</v>
       </c>
       <c r="I30" s="30">
         <f>$C$67+H30</f>
-        <v>-670.05796170537531</v>
+        <v>-670.05805051826826</v>
       </c>
       <c r="K30" s="3">
         <f t="shared" si="0"/>
@@ -19742,11 +19944,11 @@
       </c>
       <c r="H31" s="30">
         <f>$H$3-$N$23</f>
-        <v>483.94103829462466</v>
+        <v>483.94094948173171</v>
       </c>
       <c r="I31" s="30">
         <f>$C$67+H31</f>
-        <v>-666.03296170537533</v>
+        <v>-666.03305051826828</v>
       </c>
       <c r="K31" s="3">
         <f t="shared" si="0"/>
@@ -19804,11 +20006,11 @@
       </c>
       <c r="H33" s="30">
         <f>$N$28-$N$13*$N$6</f>
-        <v>-11.197603372376761</v>
+        <v>-11.189677529744586</v>
       </c>
       <c r="I33" s="30">
         <f>$C$66+H33</f>
-        <v>-561.21660337237677</v>
+        <v>-561.20867752974459</v>
       </c>
       <c r="K33" s="3">
         <f t="shared" si="0"/>
@@ -19837,11 +20039,11 @@
       </c>
       <c r="H34" s="30">
         <f ca="1">$H$21</f>
-        <v>-11.287339989597314</v>
+        <v>-11.201087937634938</v>
       </c>
       <c r="I34" s="30">
         <f ca="1">$C$66+H34</f>
-        <v>-561.30633998959729</v>
+        <v>-561.22008793763496</v>
       </c>
       <c r="K34" s="3">
         <f t="shared" si="0"/>
@@ -19863,7 +20065,7 @@
         <v>21</v>
       </c>
       <c r="C35" s="33">
-        <v>13.82</v>
+        <v>13.16</v>
       </c>
       <c r="F35" s="10" t="s">
         <v>129</v>
@@ -19873,11 +20075,11 @@
       </c>
       <c r="H35" s="30">
         <f>$N$29-$C$17-$C$13/2-$N$13</f>
-        <v>-11.759084462064493</v>
+        <v>-11.751158121853223</v>
       </c>
       <c r="I35" s="30">
         <f>$C$66+H35</f>
-        <v>-561.7780844620645</v>
+        <v>-561.77015812185323</v>
       </c>
       <c r="K35" s="3">
         <f t="shared" si="0"/>
@@ -19938,11 +20140,11 @@
       </c>
       <c r="H37" s="30">
         <f ca="1">$H$24</f>
-        <v>-11.203906231671795</v>
+        <v>-11.195980389039619</v>
       </c>
       <c r="I37" s="30">
         <f ca="1">$C$66+H37</f>
-        <v>-561.2229062316718</v>
+        <v>-561.21498038903962</v>
       </c>
       <c r="K37" s="3">
         <f>ROW(K37)</f>
@@ -20019,11 +20221,11 @@
       </c>
       <c r="H40" s="30">
         <f>$H$3-$C$55</f>
-        <v>499.01603829462465</v>
+        <v>499.0159494817317</v>
       </c>
       <c r="I40" s="30">
         <f>$C$67+H40</f>
-        <v>-650.95796170537528</v>
+        <v>-650.95805051826824</v>
       </c>
       <c r="K40" s="3">
         <f t="shared" si="0"/>
@@ -20057,11 +20259,11 @@
       </c>
       <c r="H41" s="30">
         <f>$H$3-$C$57</f>
-        <v>499.51603829462465</v>
+        <v>499.5159494817317</v>
       </c>
       <c r="I41" s="30">
         <f>$C$67+H41</f>
-        <v>-650.45796170537528</v>
+        <v>-650.45805051826824</v>
       </c>
       <c r="K41" s="3">
         <f t="shared" si="0"/>
@@ -20093,26 +20295,22 @@
       </c>
       <c r="H42" s="30">
         <f>$H$4-$C$49</f>
-        <v>495.98396170537535</v>
+        <v>495.9840505182683</v>
       </c>
       <c r="I42" s="30">
         <f>$C$67+H42</f>
-        <v>-653.99003829462458</v>
+        <v>-653.98994948173163</v>
       </c>
       <c r="K42" s="3">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
       <c r="L42" s="45" t="s">
-        <v>177</v>
-      </c>
-      <c r="M42" s="54" t="str">
-        <f>IF($C$25&gt;=3, "振分中心-内面溝1列目間距離", "-")</f>
-        <v>振分中心-内面溝1列目間距離</v>
-      </c>
-      <c r="N42" s="44">
-        <f>$C$4-$C$20</f>
-        <v>310</v>
+        <v>449</v>
+      </c>
+      <c r="N42" s="2">
+        <f>N41-N18</f>
+        <v>0.66832620933018916</v>
       </c>
     </row>
     <row r="43" spans="2:16" x14ac:dyDescent="0.4">
@@ -20130,26 +20328,26 @@
       </c>
       <c r="H43" s="30">
         <f>$H$4-$C$51</f>
-        <v>489.98396170537535</v>
+        <v>489.9840505182683</v>
       </c>
       <c r="I43" s="30">
         <f>$C$67+H43</f>
-        <v>-659.99003829462458</v>
+        <v>-659.98994948173163</v>
       </c>
       <c r="K43" s="3">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
       <c r="L43" s="45" t="s">
-        <v>232</v>
+        <v>177</v>
       </c>
       <c r="M43" s="54" t="str">
-        <f>IF($C$25&gt;=4, "振分中心-内面溝2列目間距離", "-")</f>
-        <v>振分中心-内面溝2列目間距離</v>
+        <f>IF($C$25&gt;=3, "振分中心-内面溝1列目間距離", "-")</f>
+        <v>振分中心-内面溝1列目間距離</v>
       </c>
       <c r="N43" s="44">
-        <f>IF($C$25&gt;=4,$N$42-1*$C$21, "-")</f>
-        <v>290</v>
+        <f>$C$4-$C$20</f>
+        <v>310</v>
       </c>
     </row>
     <row r="44" spans="2:16" x14ac:dyDescent="0.4">
@@ -20166,15 +20364,15 @@
         <v>44</v>
       </c>
       <c r="L44" s="45" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M44" s="54" t="str">
-        <f>IF($C$25&gt;=5, "振分中心-内面溝3列目間距離", "-")</f>
-        <v>振分中心-内面溝3列目間距離</v>
+        <f>IF($C$25&gt;=4, "振分中心-内面溝2列目間距離", "-")</f>
+        <v>振分中心-内面溝2列目間距離</v>
       </c>
       <c r="N44" s="44">
-        <f>IF($C$25&gt;=5,$N$42-2*$C$21, "-")</f>
-        <v>270</v>
+        <f>IF($C$25&gt;=4,$N$43-1*$C$21, "-")</f>
+        <v>290</v>
       </c>
     </row>
     <row r="45" spans="2:16" x14ac:dyDescent="0.4">
@@ -20197,15 +20395,15 @@
         <v>45</v>
       </c>
       <c r="L45" s="45" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="M45" s="54" t="str">
-        <f>IF($C$25&gt;=6, "振分中心-内面溝4列目間距離", "-")</f>
-        <v>振分中心-内面溝4列目間距離</v>
+        <f>IF($C$25&gt;=5, "振分中心-内面溝3列目間距離", "-")</f>
+        <v>振分中心-内面溝3列目間距離</v>
       </c>
       <c r="N45" s="44">
-        <f>IF($C$25&gt;=6,$N$42-3*$C$21, "-")</f>
-        <v>250</v>
+        <f>IF($C$25&gt;=5,$N$43-2*$C$21, "-")</f>
+        <v>270</v>
       </c>
     </row>
     <row r="46" spans="2:16" x14ac:dyDescent="0.4">
@@ -20224,15 +20422,15 @@
         <v>46</v>
       </c>
       <c r="L46" s="45" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="M46" s="54" t="str">
-        <f>IF($C$25&gt;=7, "振分中心-内面溝5列目間距離", "-")</f>
-        <v>-</v>
-      </c>
-      <c r="N46" s="44" t="str">
-        <f>IF($C$25&gt;=7,$N$42-4*$C$21, "-")</f>
-        <v>-</v>
+        <f>IF($C$25&gt;=6, "振分中心-内面溝4列目間距離", "-")</f>
+        <v>振分中心-内面溝4列目間距離</v>
+      </c>
+      <c r="N46" s="44">
+        <f>IF($C$25&gt;=6,$N$43-3*$C$21, "-")</f>
+        <v>250</v>
       </c>
     </row>
     <row r="47" spans="2:16" x14ac:dyDescent="0.4">
@@ -20246,14 +20444,14 @@
         <v>47</v>
       </c>
       <c r="L47" s="45" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="M47" s="54" t="str">
-        <f>IF($C$25&gt;=8, "振分中心-内面溝6列目間距離", "-")</f>
+        <f>IF($C$25&gt;=7, "振分中心-内面溝5列目間距離", "-")</f>
         <v>-</v>
       </c>
       <c r="N47" s="44" t="str">
-        <f>IF($C$25&gt;=8,$N$42-5*$C$21, "-")</f>
+        <f>IF($C$25&gt;=7,$N$43-4*$C$21, "-")</f>
         <v>-</v>
       </c>
     </row>
@@ -20279,19 +20477,20 @@
         <v>48</v>
       </c>
       <c r="L48" s="45" t="s">
-        <v>181</v>
-      </c>
-      <c r="M48" s="54" t="s">
-        <v>154</v>
-      </c>
-      <c r="N48" s="44">
-        <f>$N$42-($C$25-2)*$C$21</f>
-        <v>230</v>
+        <v>235</v>
+      </c>
+      <c r="M48" s="54" t="str">
+        <f>IF($C$25&gt;=8, "振分中心-内面溝6列目間距離", "-")</f>
+        <v>-</v>
+      </c>
+      <c r="N48" s="44" t="str">
+        <f>IF($C$25&gt;=8,$N$43-5*$C$21, "-")</f>
+        <v>-</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.4">
       <c r="B49" s="14" t="s">
-        <v>133</v>
+        <v>448</v>
       </c>
       <c r="C49" s="15">
         <v>4</v>
@@ -20314,14 +20513,14 @@
         <v>49</v>
       </c>
       <c r="L49" s="45" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="M49" s="54" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="N49" s="44">
-        <f>$N$42-($C$25-1)*$C$21</f>
-        <v>210</v>
+        <f>$N$43-($C$25-2)*$C$21</f>
+        <v>230</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.4">
@@ -20346,20 +20545,19 @@
         <v>50</v>
       </c>
       <c r="L50" s="45" t="s">
-        <v>178</v>
-      </c>
-      <c r="M50" s="54" t="str">
-        <f>IF($C$25&gt;=3,"λj ≦ q &lt; λj+1 の λj", "-")</f>
-        <v>λj ≦ q &lt; λj+1 の λj</v>
+        <v>180</v>
+      </c>
+      <c r="M50" s="54" t="s">
+        <v>153</v>
       </c>
       <c r="N50" s="44">
-        <f ca="1">IF($C$25&gt;=3,LOOKUP($C$20,INDIRECT($H$52&amp;"!$A:$A")),"-")</f>
-        <v>75</v>
+        <f>$N$43-($C$25-1)*$C$21</f>
+        <v>210</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.4">
       <c r="B51" s="14" t="s">
-        <v>135</v>
+        <v>447</v>
       </c>
       <c r="C51" s="15">
         <v>10</v>
@@ -20379,15 +20577,15 @@
         <v>51</v>
       </c>
       <c r="L51" s="45" t="s">
-        <v>237</v>
+        <v>178</v>
       </c>
       <c r="M51" s="54" t="str">
-        <f>IF($C$25&gt;=4,"λj ≦ q+pz &lt; λj+1 の λj", "-")</f>
-        <v>λj ≦ q+pz &lt; λj+1 の λj</v>
+        <f>IF($C$25&gt;=3,"λj ≦ q &lt; λj+1 の λj", "-")</f>
+        <v>λj ≦ q &lt; λj+1 の λj</v>
       </c>
       <c r="N51" s="44">
-        <f ca="1">IF($C$25&gt;=4,LOOKUP($C$20+$C$21, INDIRECT($H$52&amp;"!$A:$A")),"-")</f>
-        <v>100</v>
+        <f ca="1">IF($C$25&gt;=3,LOOKUP($C$20,INDIRECT($H$52&amp;"!$A:$A")),"-")</f>
+        <v>75</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.4">
@@ -20412,15 +20610,15 @@
         <v>52</v>
       </c>
       <c r="L52" s="45" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="M52" s="54" t="str">
-        <f>IF($C$25&gt;=5,"λj ≦ q+2pz &lt; λj+1 の λj", "-")</f>
-        <v>λj ≦ q+2pz &lt; λj+1 の λj</v>
+        <f>IF($C$25&gt;=4,"λj ≦ q+pz &lt; λj+1 の λj", "-")</f>
+        <v>λj ≦ q+pz &lt; λj+1 の λj</v>
       </c>
       <c r="N52" s="44">
-        <f ca="1">IF($C$25&gt;=5,LOOKUP($C$20+2*$C$21, INDIRECT($H$52&amp;"!$A:$A")),"-")</f>
-        <v>125</v>
+        <f ca="1">IF($C$25&gt;=4,LOOKUP($C$20+$C$21, INDIRECT($H$52&amp;"!$A:$A")),"-")</f>
+        <v>100</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.4">
@@ -20432,15 +20630,15 @@
         <v>53</v>
       </c>
       <c r="L53" s="45" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="M53" s="54" t="str">
-        <f>IF($C$25&gt;=6,"λj ≦ q+3pz &lt; λj+1 の λj", "-")</f>
-        <v>λj ≦ q+3pz &lt; λj+1 の λj</v>
+        <f>IF($C$25&gt;=5,"λj ≦ q+2pz &lt; λj+1 の λj", "-")</f>
+        <v>λj ≦ q+2pz &lt; λj+1 の λj</v>
       </c>
       <c r="N53" s="44">
-        <f ca="1">IF($C$25&gt;=6,LOOKUP($C$20+3*$C$21, INDIRECT($H$52&amp;"!$A:$A")),"-")</f>
-        <v>150</v>
+        <f ca="1">IF($C$25&gt;=5,LOOKUP($C$20+2*$C$21, INDIRECT($H$52&amp;"!$A:$A")),"-")</f>
+        <v>125</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.4">
@@ -20458,7 +20656,7 @@
         <v>126</v>
       </c>
       <c r="H54" s="30">
-        <f>IF($C$25&gt;=$C$71-5,$N$82-$N$15, "-")</f>
+        <f>IF($C$25&gt;=$C$71-5,$N$83-$N$15, "-")</f>
         <v>3.5836378510248323</v>
       </c>
       <c r="K54" s="3">
@@ -20466,15 +20664,15 @@
         <v>54</v>
       </c>
       <c r="L54" s="45" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="M54" s="54" t="str">
-        <f>IF($C$25&gt;=7,"λj ≦ q+4pz &lt; λj+1 の λj", "-")</f>
-        <v>-</v>
-      </c>
-      <c r="N54" s="44" t="str">
-        <f ca="1">IF($C$25&gt;=7,LOOKUP($C$20+4*$C$21, INDIRECT($H$52&amp;"!$A:$A")),"-")</f>
-        <v>-</v>
+        <f>IF($C$25&gt;=6,"λj ≦ q+3pz &lt; λj+1 の λj", "-")</f>
+        <v>λj ≦ q+3pz &lt; λj+1 の λj</v>
+      </c>
+      <c r="N54" s="44">
+        <f ca="1">IF($C$25&gt;=6,LOOKUP($C$20+3*$C$21, INDIRECT($H$52&amp;"!$A:$A")),"-")</f>
+        <v>150</v>
       </c>
     </row>
     <row r="55" spans="1:14" ht="16.5" x14ac:dyDescent="0.4">
@@ -20495,7 +20693,7 @@
         <v>126</v>
       </c>
       <c r="H55" s="30">
-        <f>IF($C$25&gt;=$C71-4,$N$83-$N$15, "-")</f>
+        <f>IF($C$25&gt;=$C71-4,$N$84-$N$15, "-")</f>
         <v>4.2564608749580657</v>
       </c>
       <c r="K55" s="3">
@@ -20503,14 +20701,14 @@
         <v>55</v>
       </c>
       <c r="L55" s="45" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="M55" s="54" t="str">
-        <f>IF($C$25&gt;=8,"λj ≦ q+5pz &lt; λj+1 の λj", "-")</f>
+        <f>IF($C$25&gt;=7,"λj ≦ q+4pz &lt; λj+1 の λj", "-")</f>
         <v>-</v>
       </c>
       <c r="N55" s="44" t="str">
-        <f ca="1">IF($C$25&gt;=8,LOOKUP($C$20+5*$C$21, INDIRECT($H$52&amp;"!$A:$A")),"-")</f>
+        <f ca="1">IF($C$25&gt;=7,LOOKUP($C$20+4*$C$21, INDIRECT($H$52&amp;"!$A:$A")),"-")</f>
         <v>-</v>
       </c>
     </row>
@@ -20529,7 +20727,7 @@
         <v>126</v>
       </c>
       <c r="H56" s="30">
-        <f>IF($C$25&gt;=$C$71-3,$N$84-$N$15, "-")</f>
+        <f>IF($C$25&gt;=$C$71-3,$N$85-$N$15, "-")</f>
         <v>4.8843832356542407</v>
       </c>
       <c r="K56" s="3">
@@ -20537,14 +20735,15 @@
         <v>56</v>
       </c>
       <c r="L56" s="45" t="s">
-        <v>245</v>
-      </c>
-      <c r="M56" s="54" t="s">
-        <v>247</v>
-      </c>
-      <c r="N56" s="2">
-        <f ca="1">LOOKUP($C$20+($C$25-2)*$C$21, INDIRECT($H$52&amp;"!$A:$A"))</f>
-        <v>150</v>
+        <v>243</v>
+      </c>
+      <c r="M56" s="54" t="str">
+        <f>IF($C$25&gt;=8,"λj ≦ q+5pz &lt; λj+1 の λj", "-")</f>
+        <v>-</v>
+      </c>
+      <c r="N56" s="44" t="str">
+        <f ca="1">IF($C$25&gt;=8,LOOKUP($C$20+5*$C$21, INDIRECT($H$52&amp;"!$A:$A")),"-")</f>
+        <v>-</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.4">
@@ -20562,7 +20761,7 @@
         <v>126</v>
       </c>
       <c r="H57" s="30">
-        <f>IF($C$25&gt;=$C$71-2,$N$85-$N$15, "-")</f>
+        <f>IF($C$25&gt;=$C$71-2,$N$86-$N$15, "-")</f>
         <v>5.4674144162945595</v>
       </c>
       <c r="K57" s="3">
@@ -20570,14 +20769,14 @@
         <v>57</v>
       </c>
       <c r="L57" s="45" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="M57" s="54" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="N57" s="2">
-        <f ca="1">LOOKUP($C$20+($C$25-1)*$C$21, INDIRECT($H$52&amp;"!$A:$A"))</f>
-        <v>175</v>
+        <f ca="1">LOOKUP($C$20+($C$25-2)*$C$21, INDIRECT($H$52&amp;"!$A:$A"))</f>
+        <v>150</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.4">
@@ -20595,7 +20794,7 @@
         <v>126</v>
       </c>
       <c r="H58" s="30" t="str">
-        <f>IF($C$25&gt;=$C71-1,$N$86-$N$15, "-")</f>
+        <f>IF($C$25&gt;=$C71-1,$N$87-$N$15, "-")</f>
         <v>-</v>
       </c>
       <c r="K58" s="3">
@@ -20603,15 +20802,14 @@
         <v>58</v>
       </c>
       <c r="L58" s="45" t="s">
-        <v>179</v>
-      </c>
-      <c r="M58" s="54" t="str">
-        <f>IF($C$25&gt;=3,"λj ≦ q &lt; λj+1 の λj+1", "-")</f>
-        <v>λj ≦ q &lt; λj+1 の λj+1</v>
-      </c>
-      <c r="N58" s="2" cm="1">
-        <f t="array" aca="1" ref="N58" ca="1">IF($C$25&gt;=3, INDEX(INDIRECT($H$52&amp;"!$A:$A"), MATCH($N50, INDIRECT($H$52&amp;"!$A:$A"), 0) +1),"-")</f>
-        <v>100</v>
+        <v>244</v>
+      </c>
+      <c r="M58" s="54" t="s">
+        <v>246</v>
+      </c>
+      <c r="N58" s="2">
+        <f ca="1">LOOKUP($C$20+($C$25-1)*$C$21, INDIRECT($H$52&amp;"!$A:$A"))</f>
+        <v>175</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.4">
@@ -20623,7 +20821,7 @@
         <v>126</v>
       </c>
       <c r="H59" s="30" t="str">
-        <f>IF($C$25&gt;=$C71,$N$87-$N$15, "-")</f>
+        <f>IF($C$25&gt;=$C71,$N$88-$N$15, "-")</f>
         <v>-</v>
       </c>
       <c r="K59" s="3">
@@ -20631,15 +20829,15 @@
         <v>59</v>
       </c>
       <c r="L59" s="45" t="s">
-        <v>238</v>
+        <v>179</v>
       </c>
       <c r="M59" s="54" t="str">
-        <f>IF($C$25&gt;=4,"λj ≦ q+pz &lt; λj+1 の λj+1", "-")</f>
-        <v>λj ≦ q+pz &lt; λj+1 の λj+1</v>
-      </c>
-      <c r="N59" s="44" cm="1">
-        <f t="array" aca="1" ref="N59" ca="1">IF($C$25&gt;=4, INDEX(INDIRECT($H$52&amp;"!$A:$A"), MATCH($N51, INDIRECT($H$52&amp;"!$A:$A"), 0) +1),"-")</f>
-        <v>125</v>
+        <f>IF($C$25&gt;=3,"λj ≦ q &lt; λj+1 の λj+1", "-")</f>
+        <v>λj ≦ q &lt; λj+1 の λj+1</v>
+      </c>
+      <c r="N59" s="2" cm="1">
+        <f t="array" aca="1" ref="N59" ca="1">IF($C$25&gt;=3, INDEX(INDIRECT($H$52&amp;"!$A:$A"), MATCH($N51, INDIRECT($H$52&amp;"!$A:$A"), 0) +1),"-")</f>
+        <v>100</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.4">
@@ -20654,7 +20852,7 @@
         <v>126</v>
       </c>
       <c r="H60" s="30">
-        <f>$N$88-$N$15</f>
+        <f>$N$89-$N$15</f>
         <v>6.0055632197072555</v>
       </c>
       <c r="K60" s="3">
@@ -20662,15 +20860,15 @@
         <v>60</v>
       </c>
       <c r="L60" s="45" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="M60" s="54" t="str">
-        <f>IF($C$25&gt;=5,"λj ≦ q+2pz &lt; λj+1 の λj+1", "-")</f>
-        <v>λj ≦ q+2pz &lt; λj+1 の λj+1</v>
+        <f>IF($C$25&gt;=4,"λj ≦ q+pz &lt; λj+1 の λj+1", "-")</f>
+        <v>λj ≦ q+pz &lt; λj+1 の λj+1</v>
       </c>
       <c r="N60" s="44" cm="1">
-        <f t="array" aca="1" ref="N60" ca="1">IF($C$25&gt;=5, INDEX(INDIRECT($H$52&amp;"!$A:$A"), MATCH($N52, INDIRECT($H$52&amp;"!$A:$A"), 0) +1),"-")</f>
-        <v>150</v>
+        <f t="array" aca="1" ref="N60" ca="1">IF($C$25&gt;=4, INDEX(INDIRECT($H$52&amp;"!$A:$A"), MATCH($N52, INDIRECT($H$52&amp;"!$A:$A"), 0) +1),"-")</f>
+        <v>125</v>
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.4">
@@ -20681,7 +20879,8 @@
         <v>439</v>
       </c>
       <c r="C61" s="19">
-        <v>330</v>
+        <f>AVERAGE(C76,C77)</f>
+        <v>330.22300000000001</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>302</v>
@@ -20693,7 +20892,7 @@
         <v>126</v>
       </c>
       <c r="H61" s="30">
-        <f>$N$89-$N$15</f>
+        <f>$N$90-$N$15</f>
         <v>6.4988377690224297</v>
       </c>
       <c r="K61" s="3">
@@ -20701,15 +20900,15 @@
         <v>61</v>
       </c>
       <c r="L61" s="45" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="M61" s="54" t="str">
-        <f>IF($C$25&gt;=6,"λj ≦ q+3pz &lt; λj+1 の λj+1", "-")</f>
-        <v>λj ≦ q+3pz &lt; λj+1 の λj+1</v>
+        <f>IF($C$25&gt;=5,"λj ≦ q+2pz &lt; λj+1 の λj+1", "-")</f>
+        <v>λj ≦ q+2pz &lt; λj+1 の λj+1</v>
       </c>
       <c r="N61" s="44" cm="1">
-        <f t="array" aca="1" ref="N61" ca="1">IF($C$25&gt;=6, INDEX(INDIRECT($H$52&amp;"!$A:$A"), MATCH($N53, INDIRECT($H$52&amp;"!$A:$A"), 0) +1),"-")</f>
-        <v>175</v>
+        <f t="array" aca="1" ref="N61" ca="1">IF($C$25&gt;=5, INDEX(INDIRECT($H$52&amp;"!$A:$A"), MATCH($N53, INDIRECT($H$52&amp;"!$A:$A"), 0) +1),"-")</f>
+        <v>150</v>
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.4">
@@ -20734,26 +20933,26 @@
       </c>
       <c r="H62" s="60">
         <f>IF($C$25&gt;=3,$H$3-$C$20,"-")</f>
-        <v>410.01603829462465</v>
+        <v>410.0159494817317</v>
       </c>
       <c r="I62" s="30">
         <f>IF($C$25&gt;=3,$C$67+H62,"-")</f>
-        <v>-739.95796170537528</v>
+        <v>-739.95805051826824</v>
       </c>
       <c r="K62" s="3">
         <f t="shared" si="0"/>
         <v>62</v>
       </c>
       <c r="L62" s="45" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="M62" s="54" t="str">
-        <f>IF($C$25&gt;=7,"λj ≦ q+4pz &lt; λj+1 の λj+1", "-")</f>
-        <v>-</v>
-      </c>
-      <c r="N62" s="44" t="str" cm="1">
-        <f t="array" aca="1" ref="N62" ca="1">IF($C$25&gt;=7, INDEX(INDIRECT($H$52&amp;"!$A:$A"), MATCH($N54, INDIRECT($H$52&amp;"!$A:$A"), 0) +1),"-")</f>
-        <v>-</v>
+        <f>IF($C$25&gt;=6,"λj ≦ q+3pz &lt; λj+1 の λj+1", "-")</f>
+        <v>λj ≦ q+3pz &lt; λj+1 の λj+1</v>
+      </c>
+      <c r="N62" s="44" cm="1">
+        <f t="array" aca="1" ref="N62" ca="1">IF($C$25&gt;=6, INDEX(INDIRECT($H$52&amp;"!$A:$A"), MATCH($N54, INDIRECT($H$52&amp;"!$A:$A"), 0) +1),"-")</f>
+        <v>175</v>
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.4">
@@ -20778,25 +20977,25 @@
       </c>
       <c r="H63" s="60">
         <f>IF($C$25&gt;=4,$H$3-$C$20-$C$21,"-")</f>
-        <v>390.01603829462465</v>
+        <v>390.0159494817317</v>
       </c>
       <c r="I63" s="30">
         <f>IF($C$25&gt;=4,$C$67+H63,"-")</f>
-        <v>-759.95796170537528</v>
+        <v>-759.95805051826824</v>
       </c>
       <c r="K63" s="3">
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
       <c r="L63" s="45" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="M63" s="54" t="str">
-        <f>IF($C$25&gt;=8,"λj ≦ q+5pz &lt; λj+1 の λj+1", "-")</f>
+        <f>IF($C$25&gt;=7,"λj ≦ q+4pz &lt; λj+1 の λj+1", "-")</f>
         <v>-</v>
       </c>
       <c r="N63" s="44" t="str" cm="1">
-        <f t="array" aca="1" ref="N63" ca="1">IF($C$25&gt;=8, INDEX(INDIRECT($H$52&amp;"!$A:$A"), MATCH($N55, INDIRECT($H$52&amp;"!$A:$A"), 0) +1),"-")</f>
+        <f t="array" aca="1" ref="N63" ca="1">IF($C$25&gt;=7, INDEX(INDIRECT($H$52&amp;"!$A:$A"), MATCH($N55, INDIRECT($H$52&amp;"!$A:$A"), 0) +1),"-")</f>
         <v>-</v>
       </c>
     </row>
@@ -20819,25 +21018,26 @@
       </c>
       <c r="H64" s="60">
         <f>IF($C$25&gt;=5,$H$3-$C$20-2*$C$21,"-")</f>
-        <v>370.01603829462465</v>
+        <v>370.0159494817317</v>
       </c>
       <c r="I64" s="30">
         <f>IF($C$25&gt;=5,$C$67+H64,"-")</f>
-        <v>-779.95796170537528</v>
+        <v>-779.95805051826824</v>
       </c>
       <c r="K64" s="3">
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
       <c r="L64" s="45" t="s">
-        <v>251</v>
-      </c>
-      <c r="M64" s="54" t="s">
-        <v>253</v>
-      </c>
-      <c r="N64" s="44" cm="1">
-        <f t="array" aca="1" ref="N64" ca="1">INDEX(INDIRECT($H$52&amp;"!$A:$A"), MATCH($N56, INDIRECT($H$52&amp;"!$A:$A"), 0) +1)</f>
-        <v>175</v>
+        <v>250</v>
+      </c>
+      <c r="M64" s="54" t="str">
+        <f>IF($C$25&gt;=8,"λj ≦ q+5pz &lt; λj+1 の λj+1", "-")</f>
+        <v>-</v>
+      </c>
+      <c r="N64" s="44" t="str" cm="1">
+        <f t="array" aca="1" ref="N64" ca="1">IF($C$25&gt;=8, INDEX(INDIRECT($H$52&amp;"!$A:$A"), MATCH($N56, INDIRECT($H$52&amp;"!$A:$A"), 0) +1),"-")</f>
+        <v>-</v>
       </c>
     </row>
     <row r="65" spans="2:14" x14ac:dyDescent="0.4">
@@ -20856,25 +21056,25 @@
       </c>
       <c r="H65" s="60">
         <f>IF($C$25&gt;=6,$H$3-$C$20-3*$C$21,"-")</f>
-        <v>350.01603829462465</v>
+        <v>350.0159494817317</v>
       </c>
       <c r="I65" s="30">
         <f>IF($C$25&gt;=6,$C$67+H65,"-")</f>
-        <v>-799.95796170537528</v>
+        <v>-799.95805051826824</v>
       </c>
       <c r="K65" s="3">
         <f t="shared" si="0"/>
         <v>65</v>
       </c>
       <c r="L65" s="45" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="M65" s="54" t="s">
-        <v>147</v>
+        <v>253</v>
       </c>
       <c r="N65" s="44" cm="1">
         <f t="array" aca="1" ref="N65" ca="1">INDEX(INDIRECT($H$52&amp;"!$A:$A"), MATCH($N57, INDIRECT($H$52&amp;"!$A:$A"), 0) +1)</f>
-        <v>200</v>
+        <v>175</v>
       </c>
     </row>
     <row r="66" spans="2:14" x14ac:dyDescent="0.4">
@@ -20904,15 +21104,14 @@
         <v>66</v>
       </c>
       <c r="L66" s="45" t="s">
-        <v>148</v>
-      </c>
-      <c r="M66" s="54" t="str">
-        <f>IF($C$25&gt;=3,"q-λj","")</f>
-        <v>q-λj</v>
-      </c>
-      <c r="N66" s="44">
-        <f ca="1">IF($C$25&gt;=3,$C$20-$N$50, "-")</f>
-        <v>15</v>
+        <v>252</v>
+      </c>
+      <c r="M66" s="54" t="s">
+        <v>147</v>
+      </c>
+      <c r="N66" s="44" cm="1">
+        <f t="array" aca="1" ref="N66" ca="1">INDEX(INDIRECT($H$52&amp;"!$A:$A"), MATCH($N58, INDIRECT($H$52&amp;"!$A:$A"), 0) +1)</f>
+        <v>200</v>
       </c>
     </row>
     <row r="67" spans="2:14" x14ac:dyDescent="0.4">
@@ -20943,15 +21142,15 @@
         <v>67</v>
       </c>
       <c r="L67" s="45" t="s">
-        <v>256</v>
+        <v>148</v>
       </c>
       <c r="M67" s="54" t="str">
-        <f>IF($C$25&gt;=4,"q+pz-λj","")</f>
-        <v>q+pz-λj</v>
+        <f>IF($C$25&gt;=3,"q-λj","")</f>
+        <v>q-λj</v>
       </c>
       <c r="N67" s="44">
-        <f ca="1">IF($C$25&gt;=4,$C$20+$C$21-$N$51, "-")</f>
-        <v>10</v>
+        <f ca="1">IF($C$25&gt;=3,$C$20-$N$51, "-")</f>
+        <v>15</v>
       </c>
     </row>
     <row r="68" spans="2:14" x14ac:dyDescent="0.4">
@@ -20969,26 +21168,26 @@
       </c>
       <c r="H68" s="60">
         <f>$H$3-$C$20-($C$25-2)*$C$21</f>
-        <v>330.01603829462465</v>
+        <v>330.0159494817317</v>
       </c>
       <c r="I68" s="30">
         <f>$C$67+H68</f>
-        <v>-819.95796170537528</v>
+        <v>-819.95805051826824</v>
       </c>
       <c r="K68" s="3">
         <f t="shared" si="0"/>
         <v>68</v>
       </c>
       <c r="L68" s="45" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="M68" s="54" t="str">
-        <f>IF($C$25&gt;=5,"q+2pz-λj","")</f>
-        <v>q+2pz-λj</v>
+        <f>IF($C$25&gt;=4,"q+pz-λj","")</f>
+        <v>q+pz-λj</v>
       </c>
       <c r="N68" s="44">
-        <f ca="1">IF($C$25&gt;=5,$C$20+2*$C$21-$N$52, "-")</f>
-        <v>5</v>
+        <f ca="1">IF($C$25&gt;=4,$C$20+$C$21-$N$52, "-")</f>
+        <v>10</v>
       </c>
     </row>
     <row r="69" spans="2:14" x14ac:dyDescent="0.4">
@@ -21009,26 +21208,26 @@
       </c>
       <c r="H69" s="60">
         <f>$H$3-$C$20-($C$25-1)*$C$21</f>
-        <v>310.01603829462465</v>
+        <v>310.0159494817317</v>
       </c>
       <c r="I69" s="30">
         <f>$C$67+H69</f>
-        <v>-839.95796170537528</v>
+        <v>-839.95805051826824</v>
       </c>
       <c r="K69" s="3">
         <f t="shared" si="0"/>
         <v>69</v>
       </c>
       <c r="L69" s="45" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="M69" s="54" t="str">
-        <f>IF($C$25&gt;=6,"q+3pz-λj","")</f>
-        <v>q+3pz-λj</v>
+        <f>IF($C$25&gt;=5,"q+2pz-λj","")</f>
+        <v>q+2pz-λj</v>
       </c>
       <c r="N69" s="44">
-        <f ca="1">IF($C$25&gt;=6,$C$20+3*$C$21-$N$53, "-")</f>
-        <v>0</v>
+        <f ca="1">IF($C$25&gt;=5,$C$20+2*$C$21-$N$53, "-")</f>
+        <v>5</v>
       </c>
     </row>
     <row r="70" spans="2:14" x14ac:dyDescent="0.4">
@@ -21056,15 +21255,15 @@
         <v>70</v>
       </c>
       <c r="L70" s="45" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="M70" s="54" t="str">
-        <f>IF($C$25&gt;=7,"q+4pz-λj","-")</f>
-        <v>-</v>
-      </c>
-      <c r="N70" s="44" t="str">
-        <f>IF($C$25&gt;=7,$C$20+4*$C$21-$N$54, "-")</f>
-        <v>-</v>
+        <f>IF($C$25&gt;=6,"q+3pz-λj","")</f>
+        <v>q+3pz-λj</v>
+      </c>
+      <c r="N70" s="44">
+        <f ca="1">IF($C$25&gt;=6,$C$20+3*$C$21-$N$54, "-")</f>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="2:14" x14ac:dyDescent="0.4">
@@ -21085,7 +21284,7 @@
         <v>126</v>
       </c>
       <c r="H71" s="30">
-        <f ca="1">IF($C$25&gt;=3,($N$66*$N$98+$N$74*$N$90)/($N$58-$N$50)+$C$31*2,"-")</f>
+        <f ca="1">IF($C$25&gt;=3,($N$67*$N$99+$N$75*$N$91)/($N$59-$N$51)+$C$31*2,"-")</f>
         <v>156.59259999999998</v>
       </c>
       <c r="K71" s="3">
@@ -21093,14 +21292,14 @@
         <v>71</v>
       </c>
       <c r="L71" s="45" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="M71" s="54" t="str">
-        <f>IF($C$25&gt;=8,"q+5pz-λj","-")</f>
+        <f>IF($C$25&gt;=7,"q+4pz-λj","-")</f>
         <v>-</v>
       </c>
       <c r="N71" s="44" t="str">
-        <f>IF($C$25&gt;=8,$C$20+5*$C$21-$N$55, "-")</f>
+        <f>IF($C$25&gt;=7,$C$20+4*$C$21-$N$55, "-")</f>
         <v>-</v>
       </c>
     </row>
@@ -21112,7 +21311,7 @@
         <v>126</v>
       </c>
       <c r="H72" s="30">
-        <f ca="1">($N$73*$N$105+$N$81*$N$97)/($N$65-$N$57)+$C$31*2</f>
+        <f ca="1">($N$74*$N$106+$N$82*$N$98)/($N$66-$N$58)+$C$31*2</f>
         <v>156.16120000000001</v>
       </c>
       <c r="K72" s="3">
@@ -21120,14 +21319,15 @@
         <v>72</v>
       </c>
       <c r="L72" s="45" t="s">
-        <v>261</v>
-      </c>
-      <c r="M72" s="54" t="s">
-        <v>261</v>
-      </c>
-      <c r="N72" s="44">
-        <f ca="1">$C$20+($C$25-2)*$C$21-$N$56</f>
-        <v>20</v>
+        <v>260</v>
+      </c>
+      <c r="M72" s="54" t="str">
+        <f>IF($C$25&gt;=8,"q+5pz-λj","-")</f>
+        <v>-</v>
+      </c>
+      <c r="N72" s="44" t="str">
+        <f>IF($C$25&gt;=8,$C$20+5*$C$21-$N$56, "-")</f>
+        <v>-</v>
       </c>
     </row>
     <row r="73" spans="2:14" x14ac:dyDescent="0.4">
@@ -21147,7 +21347,7 @@
         <v>124</v>
       </c>
       <c r="H73" s="30">
-        <f ca="1">ROUND(DEGREES($N$111),3)</f>
+        <f ca="1">ROUND(DEGREES($N$112),3)</f>
         <v>2.13</v>
       </c>
       <c r="I73" s="5"/>
@@ -21156,14 +21356,14 @@
         <v>73</v>
       </c>
       <c r="L73" s="45" t="s">
-        <v>150</v>
+        <v>261</v>
       </c>
       <c r="M73" s="54" t="s">
-        <v>150</v>
+        <v>261</v>
       </c>
       <c r="N73" s="44">
-        <f ca="1">$C$20+($C$25-1)*$C$21-$N$57</f>
-        <v>15</v>
+        <f ca="1">$C$20+($C$25-2)*$C$21-$N$57</f>
+        <v>20</v>
       </c>
     </row>
     <row r="74" spans="2:14" x14ac:dyDescent="0.4">
@@ -21195,15 +21395,14 @@
         <v>74</v>
       </c>
       <c r="L74" s="45" t="s">
-        <v>149</v>
-      </c>
-      <c r="M74" s="54" t="str">
-        <f>IF($C$25&gt;=3, "λj+1-q", "-")</f>
-        <v>λj+1-q</v>
+        <v>150</v>
+      </c>
+      <c r="M74" s="54" t="s">
+        <v>150</v>
       </c>
       <c r="N74" s="44">
-        <f ca="1">IF($C$25&gt;=3,$N$58-$C$20, "-")</f>
-        <v>10</v>
+        <f ca="1">$C$20+($C$25-1)*$C$21-$N$58</f>
+        <v>15</v>
       </c>
     </row>
     <row r="75" spans="2:14" x14ac:dyDescent="0.4">
@@ -21217,7 +21416,7 @@
         <v>124</v>
       </c>
       <c r="H75" s="56">
-        <f ca="1">DEGREES($N$119)</f>
+        <f ca="1">DEGREES($N$120)</f>
         <v>1.8081075579837422</v>
       </c>
       <c r="K75" s="3">
@@ -21225,18 +21424,24 @@
         <v>75</v>
       </c>
       <c r="L75" s="45" t="s">
-        <v>262</v>
+        <v>149</v>
       </c>
       <c r="M75" s="54" t="str">
-        <f>IF($C$25&gt;=4, "λj+1-q-pz", "-")</f>
-        <v>λj+1-q-pz</v>
+        <f>IF($C$25&gt;=3, "λj+1-q", "-")</f>
+        <v>λj+1-q</v>
       </c>
       <c r="N75" s="44">
-        <f ca="1">IF($C$25&gt;=4,$N$59-$C$20-$C$21, "-")</f>
-        <v>15</v>
+        <f ca="1">IF($C$25&gt;=3,$N$59-$C$20, "-")</f>
+        <v>10</v>
       </c>
     </row>
     <row r="76" spans="2:14" x14ac:dyDescent="0.4">
+      <c r="B76" s="14" t="s">
+        <v>445</v>
+      </c>
+      <c r="C76" s="19">
+        <v>330.26600000000002</v>
+      </c>
       <c r="E76" s="3" t="s">
         <v>323</v>
       </c>
@@ -21255,46 +21460,52 @@
         <v>2.3771075579837424</v>
       </c>
       <c r="K76" s="3">
-        <f t="shared" ref="K76:K166" si="2">ROW(K76)</f>
+        <f t="shared" si="0"/>
         <v>76</v>
       </c>
       <c r="L76" s="45" t="s">
+        <v>262</v>
+      </c>
+      <c r="M76" s="54" t="str">
+        <f>IF($C$25&gt;=4, "λj+1-q-pz", "-")</f>
+        <v>λj+1-q-pz</v>
+      </c>
+      <c r="N76" s="44">
+        <f ca="1">IF($C$25&gt;=4,$N$60-$C$20-$C$21, "-")</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="77" spans="2:14" x14ac:dyDescent="0.4">
+      <c r="B77" s="14" t="s">
+        <v>446</v>
+      </c>
+      <c r="C77" s="19">
+        <v>330.18</v>
+      </c>
+      <c r="F77" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="G77" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="H77" s="30">
+        <f ca="1">MIN($N$123, $N$124)</f>
+        <v>21.495936780292737</v>
+      </c>
+      <c r="K77" s="3">
+        <f t="shared" ref="K77:K167" si="2">ROW(K77)</f>
+        <v>77</v>
+      </c>
+      <c r="L77" s="45" t="s">
         <v>263</v>
       </c>
-      <c r="M76" s="54" t="str">
+      <c r="M77" s="54" t="str">
         <f>IF($C$25&gt;=5, "λj+1-q-2pz", "-")</f>
         <v>λj+1-q-2pz</v>
       </c>
-      <c r="N76" s="44">
-        <f ca="1">IF($C$25&gt;=5,$N$60-$C$20-2*$C$21, "-")</f>
+      <c r="N77" s="44">
+        <f ca="1">IF($C$25&gt;=5,$N$61-$C$20-2*$C$21, "-")</f>
         <v>20</v>
-      </c>
-    </row>
-    <row r="77" spans="2:14" x14ac:dyDescent="0.4">
-      <c r="F77" s="10" t="s">
-        <v>197</v>
-      </c>
-      <c r="G77" s="30" t="s">
-        <v>126</v>
-      </c>
-      <c r="H77" s="30">
-        <f ca="1">MIN($N$122, $N$123)</f>
-        <v>21.495936780292737</v>
-      </c>
-      <c r="K77" s="3">
-        <f t="shared" si="2"/>
-        <v>77</v>
-      </c>
-      <c r="L77" s="45" t="s">
-        <v>264</v>
-      </c>
-      <c r="M77" s="54" t="str">
-        <f>IF($C$25&gt;=6, "λj+1-q-3pz", "-")</f>
-        <v>λj+1-q-3pz</v>
-      </c>
-      <c r="N77" s="44">
-        <f ca="1">IF($C$25&gt;=6,$N$61-$C$20-3*$C$21, "-")</f>
-        <v>25</v>
       </c>
     </row>
     <row r="78" spans="2:14" x14ac:dyDescent="0.4">
@@ -21308,7 +21519,7 @@
         <v>125</v>
       </c>
       <c r="H78" s="30">
-        <f ca="1">($N$66*$N$132+$N$74*$N$124)/($N$58-$N$50)+$C$31*2</f>
+        <f ca="1">($N$67*$N$133+$N$75*$N$125)/($N$59-$N$51)+$C$31*2</f>
         <v>154.57380000000001</v>
       </c>
       <c r="K78" s="3">
@@ -21316,15 +21527,15 @@
         <v>78</v>
       </c>
       <c r="L78" s="45" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="M78" s="54" t="str">
-        <f>IF($C$25&gt;=7, "λj+1-q-4pz", "-")</f>
-        <v>-</v>
-      </c>
-      <c r="N78" s="44" t="str">
-        <f>IF($C$25&gt;=7,$N$62-$C$20-4*$C$21, "-")</f>
-        <v>-</v>
+        <f>IF($C$25&gt;=6, "λj+1-q-3pz", "-")</f>
+        <v>λj+1-q-3pz</v>
+      </c>
+      <c r="N78" s="44">
+        <f ca="1">IF($C$25&gt;=6,$N$62-$C$20-3*$C$21, "-")</f>
+        <v>25</v>
       </c>
     </row>
     <row r="79" spans="2:14" x14ac:dyDescent="0.4">
@@ -21335,7 +21546,7 @@
         <v>125</v>
       </c>
       <c r="H79" s="30">
-        <f ca="1">($N$73*$N$139+$N$81*$N$131)/($N$65-$N$57)+$C$31*2</f>
+        <f ca="1">($N$74*$N$140+$N$82*$N$132)/($N$66-$N$58)+$C$31*2</f>
         <v>154.14839999999998</v>
       </c>
       <c r="K79" s="3">
@@ -21343,14 +21554,14 @@
         <v>79</v>
       </c>
       <c r="L79" s="45" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="M79" s="54" t="str">
-        <f>IF($C$25&gt;=8, "λj+1-q-5pz", "-")</f>
+        <f>IF($C$25&gt;=7, "λj+1-q-4pz", "-")</f>
         <v>-</v>
       </c>
       <c r="N79" s="44" t="str">
-        <f>IF($C$25&gt;=8,$N$63-$C$20-5*$C$21, "-")</f>
+        <f>IF($C$25&gt;=7,$N$63-$C$20-4*$C$21, "-")</f>
         <v>-</v>
       </c>
     </row>
@@ -21363,14 +21574,15 @@
         <v>80</v>
       </c>
       <c r="L80" s="45" t="s">
-        <v>267</v>
-      </c>
-      <c r="M80" s="54" t="s">
-        <v>267</v>
-      </c>
-      <c r="N80" s="2">
-        <f ca="1">$N$64-$C$20-($C$25-2)*$C$21</f>
-        <v>5</v>
+        <v>266</v>
+      </c>
+      <c r="M80" s="54" t="str">
+        <f>IF($C$25&gt;=8, "λj+1-q-5pz", "-")</f>
+        <v>-</v>
+      </c>
+      <c r="N80" s="44" t="str">
+        <f>IF($C$25&gt;=8,$N$64-$C$20-5*$C$21, "-")</f>
+        <v>-</v>
       </c>
     </row>
     <row r="81" spans="6:14" x14ac:dyDescent="0.4">
@@ -21382,7 +21594,7 @@
         <v>126</v>
       </c>
       <c r="H81" s="30">
-        <f ca="1">IF($C$25&gt;=$C$71-5,$H$54*$N$113-$C$20*$N$112, "-")</f>
+        <f ca="1">IF($C$25&gt;=$C$71-5,$H$54*$N$114-$C$20*$N$113, "-")</f>
         <v>0.23613623834420849</v>
       </c>
       <c r="K81" s="3">
@@ -21390,14 +21602,14 @@
         <v>81</v>
       </c>
       <c r="L81" s="45" t="s">
-        <v>182</v>
+        <v>267</v>
       </c>
       <c r="M81" s="54" t="s">
-        <v>182</v>
+        <v>267</v>
       </c>
       <c r="N81" s="2">
-        <f ca="1">$N$65-$C$20-($C$25-1)*$C$21</f>
-        <v>10</v>
+        <f ca="1">$N$65-$C$20-($C$25-2)*$C$21</f>
+        <v>5</v>
       </c>
     </row>
     <row r="82" spans="6:14" x14ac:dyDescent="0.4">
@@ -21409,7 +21621,7 @@
         <v>126</v>
       </c>
       <c r="H82" s="30">
-        <f ca="1">IF($C$25&gt;=$C$71-4,$H$55*$N$113-($C$20+$C21)*$N$112, "-")</f>
+        <f ca="1">IF($C$25&gt;=$C$71-4,$H$55*$N$114-($C$20+$C21)*$N$113, "-")</f>
         <v>0.16515537313498907</v>
       </c>
       <c r="K82" s="3">
@@ -21417,15 +21629,14 @@
         <v>82</v>
       </c>
       <c r="L82" s="45" t="s">
-        <v>270</v>
-      </c>
-      <c r="M82" s="54" t="str">
-        <f>IF($C$25&gt;=3,"1列目湾曲中心X","-")</f>
-        <v>1列目湾曲中心X</v>
-      </c>
-      <c r="N82" s="46">
-        <f>IF($C$25&gt;=3,SQRT($C$3^2-$N$42^2),"-")</f>
-        <v>8917.3132326951491</v>
+        <v>182</v>
+      </c>
+      <c r="M82" s="54" t="s">
+        <v>182</v>
+      </c>
+      <c r="N82" s="2">
+        <f ca="1">$N$66-$C$20-($C$25-1)*$C$21</f>
+        <v>10</v>
       </c>
     </row>
     <row r="83" spans="6:14" x14ac:dyDescent="0.4">
@@ -21437,7 +21648,7 @@
         <v>126</v>
       </c>
       <c r="H83" s="30">
-        <f ca="1">IF($C$25&gt;=$C$71-3,$H$56*$N$113-($C$20+2*$C$21)*$N$112, "-")</f>
+        <f ca="1">IF($C$25&gt;=$C$71-3,$H$56*$N$114-($C$20+2*$C$21)*$N$113, "-")</f>
         <v>4.930486789530697E-2</v>
       </c>
       <c r="K83" s="3">
@@ -21445,15 +21656,15 @@
         <v>83</v>
       </c>
       <c r="L83" s="45" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="M83" s="54" t="str">
-        <f>IF($C$25&gt;=4,"2列目湾曲中心X","-")</f>
-        <v>2列目湾曲中心X</v>
+        <f>IF($C$25&gt;=3,"1列目湾曲中心X","-")</f>
+        <v>1列目湾曲中心X</v>
       </c>
       <c r="N83" s="46">
-        <f>IF($C$25&gt;=4,SQRT($C$3^2-$N$43^2),"-")</f>
-        <v>8917.9860557190823</v>
+        <f>IF($C$25&gt;=3,SQRT($C$3^2-$N$43^2),"-")</f>
+        <v>8917.3132326951491</v>
       </c>
     </row>
     <row r="84" spans="6:14" x14ac:dyDescent="0.4">
@@ -21465,7 +21676,7 @@
         <v>126</v>
       </c>
       <c r="H84" s="30">
-        <f ca="1">IF($C$25&gt;=$C$71-2,$H$57*$N$113-($C$20+3*$C$21)*$N$112, "-")</f>
+        <f ca="1">IF($C$25&gt;=$C$71-2,$H$57*$N$114-($C$20+3*$C$21)*$N$113, "-")</f>
         <v>-0.11140580074584783</v>
       </c>
       <c r="K84" s="3">
@@ -21473,15 +21684,15 @@
         <v>84</v>
       </c>
       <c r="L84" s="45" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="M84" s="54" t="str">
-        <f>IF($C$25&gt;=5,"3列目湾曲中心X","-")</f>
-        <v>3列目湾曲中心X</v>
+        <f>IF($C$25&gt;=4,"2列目湾曲中心X","-")</f>
+        <v>2列目湾曲中心X</v>
       </c>
       <c r="N84" s="46">
-        <f>IF($C$25&gt;=5,SQRT($C$3^2-$N$44^2),"-")</f>
-        <v>8918.6139780797785</v>
+        <f>IF($C$25&gt;=4,SQRT($C$3^2-$N$44^2),"-")</f>
+        <v>8917.9860557190823</v>
       </c>
     </row>
     <row r="85" spans="6:14" x14ac:dyDescent="0.4">
@@ -21493,7 +21704,7 @@
         <v>126</v>
       </c>
       <c r="H85" s="30" t="str">
-        <f>IF($C$25&gt;=$C$71-1,$H$58*$N$113-($C$20+4*$C$21)*$N$112, "-")</f>
+        <f>IF($C$25&gt;=$C$71-1,$H$58*$N$114-($C$20+4*$C$21)*$N$113, "-")</f>
         <v>-</v>
       </c>
       <c r="K85" s="3">
@@ -21501,15 +21712,15 @@
         <v>85</v>
       </c>
       <c r="L85" s="45" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="M85" s="54" t="str">
-        <f>IF($C$25&gt;=6,"4列目湾曲中心X","-")</f>
-        <v>4列目湾曲中心X</v>
+        <f>IF($C$25&gt;=5,"3列目湾曲中心X","-")</f>
+        <v>3列目湾曲中心X</v>
       </c>
       <c r="N85" s="46">
-        <f>IF($C$25&gt;=6,SQRT($C$3^2-$N$45^2),"-")</f>
-        <v>8919.1970092604188</v>
+        <f>IF($C$25&gt;=5,SQRT($C$3^2-$N$45^2),"-")</f>
+        <v>8918.6139780797785</v>
       </c>
     </row>
     <row r="86" spans="6:14" x14ac:dyDescent="0.4">
@@ -21521,7 +21732,7 @@
         <v>126</v>
       </c>
       <c r="H86" s="30" t="str">
-        <f>IF($C$25&gt;=$C$71,$H$59*$N$113-($C$20+5*$C$21)*$N$112, "-")</f>
+        <f>IF($C$25&gt;=$C$71,$H$59*$N$114-($C$20+5*$C$21)*$N$113, "-")</f>
         <v>-</v>
       </c>
       <c r="K86" s="3">
@@ -21529,15 +21740,15 @@
         <v>86</v>
       </c>
       <c r="L86" s="45" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="M86" s="54" t="str">
-        <f>IF($C$25&gt;=7,"5列目湾曲中心X","-")</f>
-        <v>-</v>
-      </c>
-      <c r="N86" s="46" t="str">
-        <f>IF($C$25&gt;=7,SQRT($C$3^2-$N$46^2),"-")</f>
-        <v>-</v>
+        <f>IF($C$25&gt;=6,"4列目湾曲中心X","-")</f>
+        <v>4列目湾曲中心X</v>
+      </c>
+      <c r="N86" s="46">
+        <f>IF($C$25&gt;=6,SQRT($C$3^2-$N$46^2),"-")</f>
+        <v>8919.1970092604188</v>
       </c>
     </row>
     <row r="87" spans="6:14" x14ac:dyDescent="0.4">
@@ -21548,7 +21759,7 @@
         <v>126</v>
       </c>
       <c r="H87" s="30">
-        <f ca="1">$H$60*$N$113-($C$20+($C$25-2)*$C$21)*$N$112</f>
+        <f ca="1">$H$60*$N$114-($C$20+($C$25-2)*$C$21)*$N$113</f>
         <v>-0.31696783604237844</v>
       </c>
       <c r="K87" s="3">
@@ -21556,14 +21767,14 @@
         <v>87</v>
       </c>
       <c r="L87" s="45" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="M87" s="54" t="str">
-        <f>IF($C$25&gt;=8,"6列目湾曲中心X","-")</f>
+        <f>IF($C$25&gt;=7,"5列目湾曲中心X","-")</f>
         <v>-</v>
       </c>
       <c r="N87" s="46" t="str">
-        <f>IF($C$25&gt;=8,SQRT($C$3^2-$N$47^2),"-")</f>
+        <f>IF($C$25&gt;=7,SQRT($C$3^2-$N$47^2),"-")</f>
         <v>-</v>
       </c>
     </row>
@@ -21575,7 +21786,7 @@
         <v>126</v>
       </c>
       <c r="H88" s="30">
-        <f ca="1">$H$61*$N$113-($C$20+($C$25-1)*$C$21)*$N$112</f>
+        <f ca="1">$H$61*$N$114-($C$20+($C$25-1)*$C$21)*$N$113</f>
         <v>-0.56737312047669697</v>
       </c>
       <c r="K88" s="3">
@@ -21583,14 +21794,15 @@
         <v>88</v>
       </c>
       <c r="L88" s="45" t="s">
-        <v>276</v>
-      </c>
-      <c r="M88" s="54" t="s">
-        <v>278</v>
-      </c>
-      <c r="N88" s="47">
-        <f>SQRT($C$3^2-$N$48^2)</f>
-        <v>8919.7351580638315</v>
+        <v>275</v>
+      </c>
+      <c r="M88" s="54" t="str">
+        <f>IF($C$25&gt;=8,"6列目湾曲中心X","-")</f>
+        <v>-</v>
+      </c>
+      <c r="N88" s="46" t="str">
+        <f>IF($C$25&gt;=8,SQRT($C$3^2-$N$48^2),"-")</f>
+        <v>-</v>
       </c>
     </row>
     <row r="89" spans="6:14" x14ac:dyDescent="0.4">
@@ -21602,7 +21814,7 @@
         <v>123</v>
       </c>
       <c r="H89" s="30">
-        <f ca="1">IF($C$25&gt;=$C$71-5,$H$54*$N$112+$C$20*$N$113, "-")</f>
+        <f ca="1">IF($C$25&gt;=$C$71-5,$H$54*$N$113+$C$20*$N$114, "-")</f>
         <v>90.071009208980442</v>
       </c>
       <c r="K89" s="3">
@@ -21610,14 +21822,14 @@
         <v>89</v>
       </c>
       <c r="L89" s="45" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="M89" s="54" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="N89" s="47">
         <f>SQRT($C$3^2-$N$49^2)</f>
-        <v>8920.2284326131467</v>
+        <v>8919.7351580638315</v>
       </c>
     </row>
     <row r="90" spans="6:14" x14ac:dyDescent="0.4">
@@ -21629,7 +21841,7 @@
         <v>123</v>
       </c>
       <c r="H90" s="30">
-        <f ca="1">IF($C$25&gt;=$C$71-4,$H$55*$N$112+($C$20+$C$21)*$N$113, "-")</f>
+        <f ca="1">IF($C$25&gt;=$C$71-4,$H$55*$N$113+($C$20+$C$21)*$N$114, "-")</f>
         <v>110.08219739305159</v>
       </c>
       <c r="K90" s="3">
@@ -21637,15 +21849,14 @@
         <v>90</v>
       </c>
       <c r="L90" s="45" t="s">
-        <v>280</v>
-      </c>
-      <c r="M90" s="54" t="str">
-        <f>IF($C$25&gt;=3,"λj ≦ q &lt; λj+1 の wAj", "-")</f>
-        <v>λj ≦ q &lt; λj+1 の wAj</v>
-      </c>
-      <c r="N90" s="44">
-        <f ca="1">IF($C$25&gt;=3, INDEX(INDIRECT($H$52&amp;"!B:B"), MATCH($N$50, INDIRECT($H$52&amp;"!A:A"), 0)),"-")</f>
-        <v>156.52099999999999</v>
+        <v>277</v>
+      </c>
+      <c r="M90" s="54" t="s">
+        <v>279</v>
+      </c>
+      <c r="N90" s="47">
+        <f>SQRT($C$3^2-$N$50^2)</f>
+        <v>8920.2284326131467</v>
       </c>
     </row>
     <row r="91" spans="6:14" x14ac:dyDescent="0.4">
@@ -21657,7 +21868,7 @@
         <v>123</v>
       </c>
       <c r="H91" s="30">
-        <f ca="1">IF($C$25&gt;=$C$71-3,$H$56*$N$112+($C$20+2*$C$21)*$N$113, "-")</f>
+        <f ca="1">IF($C$25&gt;=$C$71-3,$H$56*$N$113+($C$20+2*$C$21)*$N$114, "-")</f>
         <v>130.09171675638208</v>
       </c>
       <c r="K91" s="3">
@@ -21665,15 +21876,15 @@
         <v>91</v>
       </c>
       <c r="L91" s="45" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="M91" s="54" t="str">
-        <f>IF($C$25&gt;=4,"λj ≦ q+pz &lt; λj+1 の wAj", "-")</f>
-        <v>λj ≦ q+pz &lt; λj+1 の wAj</v>
+        <f>IF($C$25&gt;=3,"λj ≦ q &lt; λj+1 の wAj", "-")</f>
+        <v>λj ≦ q &lt; λj+1 の wAj</v>
       </c>
       <c r="N91" s="44">
-        <f ca="1">IF($C$25&gt;=4, INDEX(INDIRECT($H$52&amp;"!B:B"), MATCH($N$51, INDIRECT($H$52&amp;"!A:A"), 0)),"-")</f>
-        <v>156.40700000000001</v>
+        <f ca="1">IF($C$25&gt;=3, INDEX(INDIRECT($H$52&amp;"!B:B"), MATCH($N$51, INDIRECT($H$52&amp;"!A:A"), 0)),"-")</f>
+        <v>156.52099999999999</v>
       </c>
     </row>
     <row r="92" spans="6:14" x14ac:dyDescent="0.4">
@@ -21685,7 +21896,7 @@
         <v>123</v>
       </c>
       <c r="H92" s="30">
-        <f ca="1">IF($C$25&gt;=$C$71-2,$H$57*$N$112+($C$20+3*$C$21)*$N$113, "-")</f>
+        <f ca="1">IF($C$25&gt;=$C$71-2,$H$57*$N$113+($C$20+3*$C$21)*$N$114, "-")</f>
         <v>150.09956765143286</v>
       </c>
       <c r="K92" s="3">
@@ -21693,15 +21904,15 @@
         <v>92</v>
       </c>
       <c r="L92" s="45" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="M92" s="54" t="str">
-        <f>IF($C$25&gt;=5,"λj ≦ q+2pz &lt; λj+1 の wAj", "-")</f>
-        <v>λj ≦ q+2pz &lt; λj+1 の wAj</v>
+        <f>IF($C$25&gt;=4,"λj ≦ q+pz &lt; λj+1 の wAj", "-")</f>
+        <v>λj ≦ q+pz &lt; λj+1 の wAj</v>
       </c>
       <c r="N92" s="44">
-        <f ca="1">IF($C$25&gt;=5, INDEX(INDIRECT($H$52&amp;"!B:B"), MATCH($N$52, INDIRECT($H$52&amp;"!A:A"), 0)),"-")</f>
-        <v>156.29300000000001</v>
+        <f ca="1">IF($C$25&gt;=4, INDEX(INDIRECT($H$52&amp;"!B:B"), MATCH($N$52, INDIRECT($H$52&amp;"!A:A"), 0)),"-")</f>
+        <v>156.40700000000001</v>
       </c>
     </row>
     <row r="93" spans="6:14" x14ac:dyDescent="0.4">
@@ -21713,7 +21924,7 @@
         <v>123</v>
       </c>
       <c r="H93" s="30" t="str">
-        <f>IF($C$25&gt;=$C$71-1,$H$58*$N$112+($C$20+4*$C$21)*$N$113, "-")</f>
+        <f>IF($C$25&gt;=$C$71-1,$H$58*$N$113+($C$20+4*$C$21)*$N$114, "-")</f>
         <v>-</v>
       </c>
       <c r="K93" s="3">
@@ -21721,15 +21932,15 @@
         <v>93</v>
       </c>
       <c r="L93" s="45" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="M93" s="54" t="str">
-        <f>IF($C$25&gt;=6,"λj ≦ q+3pz &lt; λj+1 の wAj", "-")</f>
-        <v>λj ≦ q+3pz &lt; λj+1 の wAj</v>
+        <f>IF($C$25&gt;=5,"λj ≦ q+2pz &lt; λj+1 の wAj", "-")</f>
+        <v>λj ≦ q+2pz &lt; λj+1 の wAj</v>
       </c>
       <c r="N93" s="44">
-        <f ca="1">IF($C$25&gt;=6, INDEX(INDIRECT($H$52&amp;"!B:B"), MATCH($N$53, INDIRECT($H$52&amp;"!A:A"), 0)),"-")</f>
-        <v>156.179</v>
+        <f ca="1">IF($C$25&gt;=5, INDEX(INDIRECT($H$52&amp;"!B:B"), MATCH($N$53, INDIRECT($H$52&amp;"!A:A"), 0)),"-")</f>
+        <v>156.29300000000001</v>
       </c>
     </row>
     <row r="94" spans="6:14" x14ac:dyDescent="0.4">
@@ -21741,7 +21952,7 @@
         <v>123</v>
       </c>
       <c r="H94" s="30" t="str">
-        <f>IF($C$25&gt;=$C$71-0,$H$59*$N$112+($C$20+5*$C$21)*$N$113, "-")</f>
+        <f>IF($C$25&gt;=$C$71-0,$H$59*$N$113+($C$20+5*$C$21)*$N$114, "-")</f>
         <v>-</v>
       </c>
       <c r="K94" s="3">
@@ -21749,15 +21960,15 @@
         <v>94</v>
       </c>
       <c r="L94" s="45" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="M94" s="54" t="str">
-        <f>IF($C$25&gt;=7,"λj ≦ q+4pz &lt; λj+1 の wAj", "-")</f>
-        <v>-</v>
-      </c>
-      <c r="N94" s="44" t="str">
-        <f ca="1">IF($C$25&gt;=7, INDEX(INDIRECT($H$52&amp;"!B:B"), MATCH($N$54, INDIRECT($H$52&amp;"!A:A"), 0)),"-")</f>
-        <v>-</v>
+        <f>IF($C$25&gt;=6,"λj ≦ q+3pz &lt; λj+1 の wAj", "-")</f>
+        <v>λj ≦ q+3pz &lt; λj+1 の wAj</v>
+      </c>
+      <c r="N94" s="44">
+        <f ca="1">IF($C$25&gt;=6, INDEX(INDIRECT($H$52&amp;"!B:B"), MATCH($N$54, INDIRECT($H$52&amp;"!A:A"), 0)),"-")</f>
+        <v>156.179</v>
       </c>
     </row>
     <row r="95" spans="6:14" x14ac:dyDescent="0.4">
@@ -21768,7 +21979,7 @@
         <v>123</v>
       </c>
       <c r="H95" s="30">
-        <f ca="1">$H$60*$N$112+($C$20+($C$25-2)*$C$21)*$N$113</f>
+        <f ca="1">$H$60*$N$113+($C$20+($C$25-2)*$C$21)*$N$114</f>
         <v>170.10575040537816</v>
       </c>
       <c r="K95" s="3">
@@ -21776,14 +21987,14 @@
         <v>95</v>
       </c>
       <c r="L95" s="45" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="M95" s="54" t="str">
-        <f>IF($C$25&gt;=8,"λj ≦ q+5pz &lt; λj+1 の wAj", "-")</f>
+        <f>IF($C$25&gt;=7,"λj ≦ q+4pz &lt; λj+1 の wAj", "-")</f>
         <v>-</v>
       </c>
       <c r="N95" s="44" t="str">
-        <f ca="1">IF($C$25&gt;=8, INDEX(INDIRECT($H$52&amp;"!B:B"), MATCH($N$55, INDIRECT($H$52&amp;"!A:A"), 0)),"-")</f>
+        <f ca="1">IF($C$25&gt;=7, INDEX(INDIRECT($H$52&amp;"!B:B"), MATCH($N$55, INDIRECT($H$52&amp;"!A:A"), 0)),"-")</f>
         <v>-</v>
       </c>
     </row>
@@ -21795,7 +22006,7 @@
         <v>123</v>
       </c>
       <c r="H96" s="30">
-        <f ca="1">$H$61*$N$112+($C$20+($C$25-1)*$C$21)*$N$113</f>
+        <f ca="1">$H$61*$N$113+($C$20+($C$25-1)*$C$21)*$N$114</f>
         <v>190.11026532013003</v>
       </c>
       <c r="K96" s="3">
@@ -21803,14 +22014,15 @@
         <v>96</v>
       </c>
       <c r="L96" s="45" t="s">
-        <v>286</v>
-      </c>
-      <c r="M96" s="54" t="s">
-        <v>288</v>
-      </c>
-      <c r="N96" s="44">
-        <f ca="1">INDEX(INDIRECT($H$52&amp;"!B:B"), MATCH($N$56, INDIRECT($H$52&amp;"!A:A"), 0))</f>
-        <v>156.179</v>
+        <v>285</v>
+      </c>
+      <c r="M96" s="54" t="str">
+        <f>IF($C$25&gt;=8,"λj ≦ q+5pz &lt; λj+1 の wAj", "-")</f>
+        <v>-</v>
+      </c>
+      <c r="N96" s="44" t="str">
+        <f ca="1">IF($C$25&gt;=8, INDEX(INDIRECT($H$52&amp;"!B:B"), MATCH($N$56, INDIRECT($H$52&amp;"!A:A"), 0)),"-")</f>
+        <v>-</v>
       </c>
     </row>
     <row r="97" spans="5:14" x14ac:dyDescent="0.4">
@@ -21822,14 +22034,14 @@
         <v>97</v>
       </c>
       <c r="L97" s="45" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="M97" s="54" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="N97" s="44">
         <f ca="1">INDEX(INDIRECT($H$52&amp;"!B:B"), MATCH($N$57, INDIRECT($H$52&amp;"!A:A"), 0))</f>
-        <v>156.077</v>
+        <v>156.179</v>
       </c>
     </row>
     <row r="98" spans="5:14" x14ac:dyDescent="0.4">
@@ -21855,15 +22067,14 @@
         <v>98</v>
       </c>
       <c r="L98" s="45" t="s">
-        <v>290</v>
-      </c>
-      <c r="M98" s="54" t="str">
-        <f>IF($C$25&gt;=3,"λj ≦ q &lt; λj+1 の wAj+1", "-")</f>
-        <v>λj ≦ q &lt; λj+1 の wAj+1</v>
+        <v>287</v>
+      </c>
+      <c r="M98" s="54" t="s">
+        <v>289</v>
       </c>
       <c r="N98" s="44">
-        <f ca="1">IF($C$25&gt;=3, INDEX(INDIRECT($H$52&amp;"!B:B"), MATCH($N$58, INDIRECT($H$52&amp;"!A:A"), 0)),"-")</f>
-        <v>156.40700000000001</v>
+        <f ca="1">INDEX(INDIRECT($H$52&amp;"!B:B"), MATCH($N$58, INDIRECT($H$52&amp;"!A:A"), 0))</f>
+        <v>156.077</v>
       </c>
     </row>
     <row r="99" spans="5:14" x14ac:dyDescent="0.4">
@@ -21878,26 +22089,26 @@
       </c>
       <c r="H99" s="30">
         <f>$H$3</f>
-        <v>500.01603829462465</v>
+        <v>500.0159494817317</v>
       </c>
       <c r="I99" s="30">
         <f>$C$67+H99</f>
-        <v>-649.95796170537528</v>
+        <v>-649.95805051826824</v>
       </c>
       <c r="K99" s="3">
         <f t="shared" si="2"/>
         <v>99</v>
       </c>
       <c r="L99" s="45" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="M99" s="54" t="str">
-        <f>IF($C$25&gt;=4,"λj ≦ q+pz &lt; λj+1 の wAj+1", "-")</f>
-        <v>λj ≦ q+pz &lt; λj+1 の wAj+1</v>
+        <f>IF($C$25&gt;=3,"λj ≦ q &lt; λj+1 の wAj+1", "-")</f>
+        <v>λj ≦ q &lt; λj+1 の wAj+1</v>
       </c>
       <c r="N99" s="44">
-        <f ca="1">IF($C$25&gt;=4, INDEX(INDIRECT($H$52&amp;"!B:B"), MATCH($N$59, INDIRECT($H$52&amp;"!A:A"), 0)),"-")</f>
-        <v>156.29300000000001</v>
+        <f ca="1">IF($C$25&gt;=3, INDEX(INDIRECT($H$52&amp;"!B:B"), MATCH($N$59, INDIRECT($H$52&amp;"!A:A"), 0)),"-")</f>
+        <v>156.40700000000001</v>
       </c>
     </row>
     <row r="100" spans="5:14" x14ac:dyDescent="0.4">
@@ -21911,27 +22122,27 @@
         <v>126</v>
       </c>
       <c r="H100" s="30">
-        <f ca="1">$H$98*$N$113+$H$99*$N$112</f>
-        <v>7.4967373522236862</v>
+        <f ca="1">$H$98*$N$114+$H$99*$N$113</f>
+        <v>7.4967340513192653</v>
       </c>
       <c r="I100" s="30">
         <f ca="1">$C$66+H100</f>
-        <v>-542.5222626477763</v>
+        <v>-542.5222659486808</v>
       </c>
       <c r="K100" s="3">
         <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="L100" s="45" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="M100" s="54" t="str">
-        <f>IF($C$25&gt;=5,"λj ≦ q+2pz &lt; λj+1 の wAj+1", "-")</f>
-        <v>λj ≦ q+2pz &lt; λj+1 の wAj+1</v>
+        <f>IF($C$25&gt;=4,"λj ≦ q+pz &lt; λj+1 の wAj+1", "-")</f>
+        <v>λj ≦ q+pz &lt; λj+1 の wAj+1</v>
       </c>
       <c r="N100" s="44">
-        <f ca="1">IF($C$25&gt;=5, INDEX(INDIRECT($H$52&amp;"!B:B"), MATCH($N$60, INDIRECT($H$52&amp;"!A:A"), 0)),"-")</f>
-        <v>156.179</v>
+        <f ca="1">IF($C$25&gt;=4, INDEX(INDIRECT($H$52&amp;"!B:B"), MATCH($N$60, INDIRECT($H$52&amp;"!A:A"), 0)),"-")</f>
+        <v>156.29300000000001</v>
       </c>
     </row>
     <row r="101" spans="5:14" x14ac:dyDescent="0.4">
@@ -21945,27 +22156,27 @@
         <v>123</v>
       </c>
       <c r="H101" s="30">
-        <f ca="1">-$H$98*$N$112+$H$99*$N$113</f>
-        <v>500.08292962860008</v>
+        <f ca="1">-$H$98*$N$113+$H$99*$N$114</f>
+        <v>500.08284087707057</v>
       </c>
       <c r="I101" s="30">
         <f ca="1">$C$67+H101</f>
-        <v>-649.89107037139979</v>
+        <v>-649.89115912292937</v>
       </c>
       <c r="K101" s="3">
         <f t="shared" si="2"/>
         <v>101</v>
       </c>
       <c r="L101" s="45" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="M101" s="54" t="str">
-        <f>IF($C$25&gt;=6,"λj ≦ q+3pz &lt; λj+1 の wAj+1", "-")</f>
-        <v>λj ≦ q+3pz &lt; λj+1 の wAj+1</v>
+        <f>IF($C$25&gt;=5,"λj ≦ q+2pz &lt; λj+1 の wAj+1", "-")</f>
+        <v>λj ≦ q+2pz &lt; λj+1 の wAj+1</v>
       </c>
       <c r="N101" s="44">
-        <f ca="1">IF($C$25&gt;=6, INDEX(INDIRECT($H$52&amp;"!B:B"), MATCH($N$61, INDIRECT($H$52&amp;"!A:A"), 0)),"-")</f>
-        <v>156.077</v>
+        <f ca="1">IF($C$25&gt;=5, INDEX(INDIRECT($H$52&amp;"!B:B"), MATCH($N$61, INDIRECT($H$52&amp;"!A:A"), 0)),"-")</f>
+        <v>156.179</v>
       </c>
     </row>
     <row r="102" spans="5:14" x14ac:dyDescent="0.4">
@@ -21977,22 +22188,22 @@
       </c>
       <c r="H102" s="30">
         <f ca="1">$H$100-$H$98</f>
-        <v>18.591737352223713</v>
+        <v>18.591734051319293</v>
       </c>
       <c r="K102" s="3">
         <f t="shared" si="2"/>
         <v>102</v>
       </c>
       <c r="L102" s="45" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="M102" s="54" t="str">
-        <f>IF($C$25&gt;=7,"λj ≦ q+4pz &lt; λj+1 の wAj+1", "-")</f>
-        <v>-</v>
-      </c>
-      <c r="N102" s="44" t="str">
-        <f ca="1">IF($C$25&gt;=7, INDEX(INDIRECT($H$52&amp;"!B:B"), MATCH($N$62, INDIRECT($H$52&amp;"!A:A"), 0)),"-")</f>
-        <v>-</v>
+        <f>IF($C$25&gt;=6,"λj ≦ q+3pz &lt; λj+1 の wAj+1", "-")</f>
+        <v>λj ≦ q+3pz &lt; λj+1 の wAj+1</v>
+      </c>
+      <c r="N102" s="44">
+        <f ca="1">IF($C$25&gt;=6, INDEX(INDIRECT($H$52&amp;"!B:B"), MATCH($N$62, INDIRECT($H$52&amp;"!A:A"), 0)),"-")</f>
+        <v>156.077</v>
       </c>
     </row>
     <row r="103" spans="5:14" x14ac:dyDescent="0.4">
@@ -22004,21 +22215,21 @@
       </c>
       <c r="H103" s="30">
         <f ca="1">$H$101-$H$99</f>
-        <v>6.6891333975434009E-2</v>
+        <v>6.6891395338871007E-2</v>
       </c>
       <c r="K103" s="3">
         <f t="shared" si="2"/>
         <v>103</v>
       </c>
       <c r="L103" s="45" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="M103" s="54" t="str">
-        <f>IF($C$25&gt;=8,"λj ≦ q+5pz &lt; λj+1 の wAj+1", "-")</f>
+        <f>IF($C$25&gt;=7,"λj ≦ q+4pz &lt; λj+1 の wAj+1", "-")</f>
         <v>-</v>
       </c>
       <c r="N103" s="44" t="str">
-        <f ca="1">IF($C$25&gt;=8, INDEX(INDIRECT($H$52&amp;"!B:B"), MATCH($N$63, INDIRECT($H$52&amp;"!A:A"), 0)),"-")</f>
+        <f ca="1">IF($C$25&gt;=7, INDEX(INDIRECT($H$52&amp;"!B:B"), MATCH($N$63, INDIRECT($H$52&amp;"!A:A"), 0)),"-")</f>
         <v>-</v>
       </c>
     </row>
@@ -22028,14 +22239,15 @@
         <v>104</v>
       </c>
       <c r="L104" s="45" t="s">
-        <v>296</v>
-      </c>
-      <c r="M104" s="54" t="s">
-        <v>298</v>
-      </c>
-      <c r="N104" s="44">
-        <f ca="1">INDEX(INDIRECT($H$52&amp;"!B:B"), MATCH($N$64, INDIRECT($H$52&amp;"!A:A"), 0))</f>
-        <v>156.077</v>
+        <v>295</v>
+      </c>
+      <c r="M104" s="54" t="str">
+        <f>IF($C$25&gt;=8,"λj ≦ q+5pz &lt; λj+1 の wAj+1", "-")</f>
+        <v>-</v>
+      </c>
+      <c r="N104" s="44" t="str">
+        <f ca="1">IF($C$25&gt;=8, INDEX(INDIRECT($H$52&amp;"!B:B"), MATCH($N$64, INDIRECT($H$52&amp;"!A:A"), 0)),"-")</f>
+        <v>-</v>
       </c>
     </row>
     <row r="105" spans="5:14" x14ac:dyDescent="0.4">
@@ -22049,14 +22261,14 @@
         <v>105</v>
       </c>
       <c r="L105" s="45" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="M105" s="54" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="N105" s="44">
         <f ca="1">INDEX(INDIRECT($H$52&amp;"!B:B"), MATCH($N$65, INDIRECT($H$52&amp;"!A:A"), 0))</f>
-        <v>155.98400000000001</v>
+        <v>156.077</v>
       </c>
     </row>
     <row r="106" spans="5:14" x14ac:dyDescent="0.4">
@@ -22070,14 +22282,14 @@
         <v>106</v>
       </c>
       <c r="L106" s="45" t="s">
-        <v>310</v>
+        <v>297</v>
       </c>
       <c r="M106" s="54" t="s">
-        <v>223</v>
-      </c>
-      <c r="N106" s="2">
-        <f ca="1">$C$3+$H$70/2</f>
-        <v>9001.201500000001</v>
+        <v>299</v>
+      </c>
+      <c r="N106" s="44">
+        <f ca="1">INDEX(INDIRECT($H$52&amp;"!B:B"), MATCH($N$66, INDIRECT($H$52&amp;"!A:A"), 0))</f>
+        <v>155.98400000000001</v>
       </c>
     </row>
     <row r="107" spans="5:14" x14ac:dyDescent="0.4">
@@ -22091,14 +22303,14 @@
         <v>107</v>
       </c>
       <c r="L107" s="45" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="M107" s="54" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="N107" s="2">
-        <f ca="1">$C$3+$H$71/2</f>
-        <v>9000.9963000000007</v>
+        <f ca="1">$C$3+$H$70/2</f>
+        <v>9001.201500000001</v>
       </c>
     </row>
     <row r="108" spans="5:14" x14ac:dyDescent="0.4">
@@ -22107,14 +22319,14 @@
         <v>108</v>
       </c>
       <c r="L108" s="45" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="M108" s="54" t="s">
-        <v>195</v>
+        <v>224</v>
       </c>
       <c r="N108" s="2">
-        <f ca="1">SQRT($N$107^2-$N$42^2)</f>
-        <v>8995.6564181061131</v>
+        <f ca="1">$C$3+$H$71/2</f>
+        <v>9000.9963000000007</v>
       </c>
     </row>
     <row r="109" spans="5:14" x14ac:dyDescent="0.4">
@@ -22123,14 +22335,14 @@
         <v>109</v>
       </c>
       <c r="L109" s="45" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="M109" s="54" t="s">
         <v>195</v>
       </c>
       <c r="N109" s="2">
-        <f ca="1">SQRT($N$106^2-$C$4^2)</f>
-        <v>8992.3094054643298</v>
+        <f ca="1">SQRT($N$108^2-$N$43^2)</f>
+        <v>8995.6564181061131</v>
       </c>
     </row>
     <row r="110" spans="5:14" x14ac:dyDescent="0.4">
@@ -22139,14 +22351,14 @@
         <v>110</v>
       </c>
       <c r="L110" s="45" t="s">
-        <v>183</v>
+        <v>315</v>
       </c>
       <c r="M110" s="54" t="s">
-        <v>183</v>
+        <v>195</v>
       </c>
       <c r="N110" s="2">
-        <f ca="1">IF($N$108&gt;$N$109, ($N$108-$N$109)/$C$20, 0)</f>
-        <v>3.7189029353147718E-2</v>
+        <f ca="1">SQRT($N$107^2-$C$4^2)</f>
+        <v>8992.3094054643298</v>
       </c>
     </row>
     <row r="111" spans="5:14" x14ac:dyDescent="0.4">
@@ -22155,14 +22367,14 @@
         <v>111</v>
       </c>
       <c r="L111" s="45" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="M111" s="54" t="s">
-        <v>151</v>
+        <v>183</v>
       </c>
       <c r="N111" s="2">
-        <f ca="1">ATAN($N$110)</f>
-        <v>3.7171899126953054E-2</v>
+        <f ca="1">IF($N$109&gt;$N$110, ($N$109-$N$110)/$C$20, 0)</f>
+        <v>3.7189029353147718E-2</v>
       </c>
     </row>
     <row r="112" spans="5:14" x14ac:dyDescent="0.4">
@@ -22171,14 +22383,14 @@
         <v>112</v>
       </c>
       <c r="L112" s="45" t="s">
-        <v>392</v>
+        <v>184</v>
       </c>
       <c r="M112" s="54" t="s">
-        <v>392</v>
+        <v>151</v>
       </c>
       <c r="N112" s="2">
-        <f ca="1">SIN(RADIANS($H$73))</f>
-        <v>3.7166950783010577E-2</v>
+        <f ca="1">ATAN($N$111)</f>
+        <v>3.7171899126953054E-2</v>
       </c>
     </row>
     <row r="113" spans="11:14" x14ac:dyDescent="0.4">
@@ -22187,14 +22399,14 @@
         <v>113</v>
       </c>
       <c r="L113" s="45" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="M113" s="54" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="N113" s="2">
-        <f ca="1">COS(RADIANS($H$73))</f>
-        <v>0.9993090701927474</v>
+        <f ca="1">SIN(RADIANS($H$73))</f>
+        <v>3.7166950783010577E-2</v>
       </c>
     </row>
     <row r="114" spans="11:14" x14ac:dyDescent="0.4">
@@ -22203,14 +22415,14 @@
         <v>114</v>
       </c>
       <c r="L114" s="45" t="s">
-        <v>312</v>
+        <v>391</v>
       </c>
       <c r="M114" s="54" t="s">
-        <v>144</v>
+        <v>391</v>
       </c>
       <c r="N114" s="2">
-        <f ca="1">$C$3-$H$71/2</f>
-        <v>8844.4037000000008</v>
+        <f ca="1">COS(RADIANS($H$73))</f>
+        <v>0.9993090701927474</v>
       </c>
     </row>
     <row r="115" spans="11:14" x14ac:dyDescent="0.4">
@@ -22219,14 +22431,14 @@
         <v>115</v>
       </c>
       <c r="L115" s="45" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="M115" s="54" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N115" s="2">
-        <f ca="1">$C$3-$H$72/2</f>
-        <v>8844.6194000000014</v>
+        <f ca="1">$C$3-$H$71/2</f>
+        <v>8844.4037000000008</v>
       </c>
     </row>
     <row r="116" spans="11:14" x14ac:dyDescent="0.4">
@@ -22235,14 +22447,14 @@
         <v>116</v>
       </c>
       <c r="L116" s="45" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="M116" s="54" t="s">
-        <v>196</v>
+        <v>145</v>
       </c>
       <c r="N116" s="2">
-        <f ca="1">SQRT($N$115^2-$N$49^2)</f>
-        <v>8842.1260074066122</v>
+        <f ca="1">$C$3-$H$72/2</f>
+        <v>8844.6194000000014</v>
       </c>
     </row>
     <row r="117" spans="11:14" x14ac:dyDescent="0.4">
@@ -22251,14 +22463,14 @@
         <v>117</v>
       </c>
       <c r="L117" s="45" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="M117" s="54" t="s">
         <v>196</v>
       </c>
       <c r="N117" s="2">
-        <f ca="1">SQRT($N$114^2-$N$42^2)</f>
-        <v>8838.9692164060452</v>
+        <f ca="1">SQRT($N$116^2-$N$50^2)</f>
+        <v>8842.1260074066122</v>
       </c>
     </row>
     <row r="118" spans="11:14" x14ac:dyDescent="0.4">
@@ -22267,11 +22479,14 @@
         <v>118</v>
       </c>
       <c r="L118" s="45" t="s">
-        <v>185</v>
+        <v>317</v>
+      </c>
+      <c r="M118" s="54" t="s">
+        <v>196</v>
       </c>
       <c r="N118" s="2">
-        <f ca="1">($N116-$N117)/($N$42-$N$49)</f>
-        <v>3.1567910005669546E-2</v>
+        <f ca="1">SQRT($N$115^2-$N$43^2)</f>
+        <v>8838.9692164060452</v>
       </c>
     </row>
     <row r="119" spans="11:14" x14ac:dyDescent="0.4">
@@ -22280,46 +22495,43 @@
         <v>119</v>
       </c>
       <c r="L119" s="45" t="s">
-        <v>186</v>
-      </c>
-      <c r="M119" s="54" t="s">
-        <v>152</v>
+        <v>185</v>
       </c>
       <c r="N119" s="2">
-        <f ca="1">ATAN($N$118)</f>
-        <v>3.1557430117010586E-2</v>
+        <f ca="1">($N117-$N118)/($N$43-$N$50)</f>
+        <v>3.1567910005669546E-2</v>
       </c>
     </row>
     <row r="120" spans="11:14" x14ac:dyDescent="0.4">
       <c r="K120" s="3">
-        <f>ROW(K120)</f>
+        <f t="shared" si="2"/>
         <v>120</v>
       </c>
       <c r="L120" s="45" t="s">
+        <v>186</v>
+      </c>
+      <c r="M120" s="54" t="s">
+        <v>152</v>
+      </c>
+      <c r="N120" s="2">
+        <f ca="1">ATAN($N$119)</f>
+        <v>3.1557430117010586E-2</v>
+      </c>
+    </row>
+    <row r="121" spans="11:14" x14ac:dyDescent="0.4">
+      <c r="K121" s="3">
+        <f>ROW(K121)</f>
+        <v>121</v>
+      </c>
+      <c r="L121" s="45" t="s">
         <v>188</v>
       </c>
-      <c r="M120" s="54" t="s">
+      <c r="M121" s="54" t="s">
         <v>156</v>
       </c>
-      <c r="N120" s="2">
+      <c r="N121" s="2">
         <f>IF(MOD($C$25, 2)=0, $C$23, $C$24)</f>
         <v>102</v>
-      </c>
-    </row>
-    <row r="121" spans="11:14" x14ac:dyDescent="0.4">
-      <c r="K121" s="3">
-        <f t="shared" si="2"/>
-        <v>121</v>
-      </c>
-      <c r="L121" s="45" t="s">
-        <v>187</v>
-      </c>
-      <c r="M121" s="54" t="s">
-        <v>155</v>
-      </c>
-      <c r="N121" s="2">
-        <f>IF(MOD($C$25, 2)=0, $C$24, $C$23)</f>
-        <v>85</v>
       </c>
     </row>
     <row r="122" spans="11:14" x14ac:dyDescent="0.4">
@@ -22328,14 +22540,14 @@
         <v>122</v>
       </c>
       <c r="L122" s="45" t="s">
-        <v>319</v>
+        <v>187</v>
       </c>
       <c r="M122" s="54" t="s">
-        <v>198</v>
+        <v>155</v>
       </c>
       <c r="N122" s="2">
-        <f ca="1">$H$70/2-$H$60-$N$120/2</f>
-        <v>21.495936780292737</v>
+        <f>IF(MOD($C$25, 2)=0, $C$24, $C$23)</f>
+        <v>85</v>
       </c>
     </row>
     <row r="123" spans="11:14" x14ac:dyDescent="0.4">
@@ -22344,14 +22556,14 @@
         <v>123</v>
       </c>
       <c r="L123" s="45" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="M123" s="54" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="N123" s="2">
-        <f ca="1">$H$70/2-$H$61-$N$121/2</f>
-        <v>29.502662230977563</v>
+        <f ca="1">$H$70/2-$H$60-$N$121/2</f>
+        <v>21.495936780292737</v>
       </c>
     </row>
     <row r="124" spans="11:14" x14ac:dyDescent="0.4">
@@ -22360,15 +22572,14 @@
         <v>124</v>
       </c>
       <c r="L124" s="45" t="s">
-        <v>324</v>
-      </c>
-      <c r="M124" s="54" t="str">
-        <f>IF($C$25&gt;=3,"λj ≦ q &lt; λj+1 の wBj", "-")</f>
-        <v>λj ≦ q &lt; λj+1 の wBj</v>
-      </c>
-      <c r="N124" s="44">
-        <f ca="1">IF($C$25&gt;=3, INDEX(INDIRECT($H$52&amp;"!C:C"), MATCH($N$50, INDIRECT($H$52&amp;"!A:A"), 0)),"-")</f>
-        <v>154.501</v>
+        <v>320</v>
+      </c>
+      <c r="M124" s="54" t="s">
+        <v>199</v>
+      </c>
+      <c r="N124" s="2">
+        <f ca="1">$H$70/2-$H$61-$N$122/2</f>
+        <v>29.502662230977563</v>
       </c>
     </row>
     <row r="125" spans="11:14" x14ac:dyDescent="0.4">
@@ -22377,15 +22588,15 @@
         <v>125</v>
       </c>
       <c r="L125" s="45" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="M125" s="54" t="str">
-        <f>IF($C$25&gt;=4,"λj ≦ q+pz &lt; λj+1 の wBj", "-")</f>
-        <v>λj ≦ q+pz &lt; λj+1 の wBj</v>
+        <f>IF($C$25&gt;=3,"λj ≦ q &lt; λj+1 の wBj", "-")</f>
+        <v>λj ≦ q &lt; λj+1 の wBj</v>
       </c>
       <c r="N125" s="44">
-        <f ca="1">IF($C$25&gt;=4, INDEX(INDIRECT($H$52&amp;"!C:C"), MATCH($N$51, INDIRECT($H$52&amp;"!A:A"), 0)),"-")</f>
-        <v>154.38900000000001</v>
+        <f ca="1">IF($C$25&gt;=3, INDEX(INDIRECT($H$52&amp;"!C:C"), MATCH($N$51, INDIRECT($H$52&amp;"!A:A"), 0)),"-")</f>
+        <v>154.501</v>
       </c>
     </row>
     <row r="126" spans="11:14" x14ac:dyDescent="0.4">
@@ -22394,15 +22605,15 @@
         <v>126</v>
       </c>
       <c r="L126" s="45" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="M126" s="54" t="str">
-        <f>IF($C$25&gt;=5,"λj ≦ q+2pz &lt; λj+1 の wBj", "-")</f>
-        <v>λj ≦ q+2pz &lt; λj+1 の wBj</v>
+        <f>IF($C$25&gt;=4,"λj ≦ q+pz &lt; λj+1 の wBj", "-")</f>
+        <v>λj ≦ q+pz &lt; λj+1 の wBj</v>
       </c>
       <c r="N126" s="44">
-        <f ca="1">IF($C$25&gt;=5, INDEX(INDIRECT($H$52&amp;"!C:C"), MATCH($N$52, INDIRECT($H$52&amp;"!A:A"), 0)),"-")</f>
-        <v>154.27600000000001</v>
+        <f ca="1">IF($C$25&gt;=4, INDEX(INDIRECT($H$52&amp;"!C:C"), MATCH($N$52, INDIRECT($H$52&amp;"!A:A"), 0)),"-")</f>
+        <v>154.38900000000001</v>
       </c>
     </row>
     <row r="127" spans="11:14" x14ac:dyDescent="0.4">
@@ -22411,15 +22622,15 @@
         <v>127</v>
       </c>
       <c r="L127" s="45" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="M127" s="54" t="str">
-        <f>IF($C$25&gt;=6,"λj ≦ q+3pz &lt; λj+1 の wBj", "-")</f>
-        <v>λj ≦ q+3pz &lt; λj+1 の wBj</v>
+        <f>IF($C$25&gt;=5,"λj ≦ q+2pz &lt; λj+1 の wBj", "-")</f>
+        <v>λj ≦ q+2pz &lt; λj+1 の wBj</v>
       </c>
       <c r="N127" s="44">
-        <f ca="1">IF($C$25&gt;=6, INDEX(INDIRECT($H$52&amp;"!C:C"), MATCH($N$53, INDIRECT($H$52&amp;"!A:A"), 0)),"-")</f>
-        <v>154.16399999999999</v>
+        <f ca="1">IF($C$25&gt;=5, INDEX(INDIRECT($H$52&amp;"!C:C"), MATCH($N$53, INDIRECT($H$52&amp;"!A:A"), 0)),"-")</f>
+        <v>154.27600000000001</v>
       </c>
     </row>
     <row r="128" spans="11:14" x14ac:dyDescent="0.4">
@@ -22428,15 +22639,15 @@
         <v>128</v>
       </c>
       <c r="L128" s="45" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="M128" s="54" t="str">
-        <f>IF($C$25&gt;=7,"λj ≦ q+4pz &lt; λj+1 の wBj", "-")</f>
-        <v>-</v>
-      </c>
-      <c r="N128" s="44" t="str">
-        <f ca="1">IF($C$25&gt;=7, INDEX(INDIRECT($H$52&amp;"!C:C"), MATCH($N$54, INDIRECT($H$52&amp;"!A:A"), 0)),"-")</f>
-        <v>-</v>
+        <f>IF($C$25&gt;=6,"λj ≦ q+3pz &lt; λj+1 の wBj", "-")</f>
+        <v>λj ≦ q+3pz &lt; λj+1 の wBj</v>
+      </c>
+      <c r="N128" s="44">
+        <f ca="1">IF($C$25&gt;=6, INDEX(INDIRECT($H$52&amp;"!C:C"), MATCH($N$54, INDIRECT($H$52&amp;"!A:A"), 0)),"-")</f>
+        <v>154.16399999999999</v>
       </c>
     </row>
     <row r="129" spans="11:14" x14ac:dyDescent="0.4">
@@ -22445,14 +22656,14 @@
         <v>129</v>
       </c>
       <c r="L129" s="45" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="M129" s="54" t="str">
-        <f>IF($C$25&gt;=8,"λj ≦ q+5pz &lt; λj+1 の wBj", "-")</f>
+        <f>IF($C$25&gt;=7,"λj ≦ q+4pz &lt; λj+1 の wBj", "-")</f>
         <v>-</v>
       </c>
       <c r="N129" s="44" t="str">
-        <f ca="1">IF($C$25&gt;=8, INDEX(INDIRECT($H$52&amp;"!C:C"), MATCH($N$55, INDIRECT($H$52&amp;"!A:A"), 0)),"-")</f>
+        <f ca="1">IF($C$25&gt;=7, INDEX(INDIRECT($H$52&amp;"!C:C"), MATCH($N$55, INDIRECT($H$52&amp;"!A:A"), 0)),"-")</f>
         <v>-</v>
       </c>
     </row>
@@ -22462,14 +22673,15 @@
         <v>130</v>
       </c>
       <c r="L130" s="45" t="s">
-        <v>330</v>
-      </c>
-      <c r="M130" s="54" t="s">
-        <v>340</v>
-      </c>
-      <c r="N130" s="44">
-        <f ca="1">INDEX(INDIRECT($H$52&amp;"!C:C"), MATCH($N$56, INDIRECT($H$52&amp;"!A:A"), 0))</f>
-        <v>154.16399999999999</v>
+        <v>329</v>
+      </c>
+      <c r="M130" s="54" t="str">
+        <f>IF($C$25&gt;=8,"λj ≦ q+5pz &lt; λj+1 の wBj", "-")</f>
+        <v>-</v>
+      </c>
+      <c r="N130" s="44" t="str">
+        <f ca="1">IF($C$25&gt;=8, INDEX(INDIRECT($H$52&amp;"!C:C"), MATCH($N$56, INDIRECT($H$52&amp;"!A:A"), 0)),"-")</f>
+        <v>-</v>
       </c>
     </row>
     <row r="131" spans="11:14" x14ac:dyDescent="0.4">
@@ -22478,14 +22690,14 @@
         <v>131</v>
       </c>
       <c r="L131" s="45" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="M131" s="54" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="N131" s="44">
         <f ca="1">INDEX(INDIRECT($H$52&amp;"!C:C"), MATCH($N$57, INDIRECT($H$52&amp;"!A:A"), 0))</f>
-        <v>154.06299999999999</v>
+        <v>154.16399999999999</v>
       </c>
     </row>
     <row r="132" spans="11:14" x14ac:dyDescent="0.4">
@@ -22494,15 +22706,14 @@
         <v>132</v>
       </c>
       <c r="L132" s="45" t="s">
-        <v>332</v>
-      </c>
-      <c r="M132" s="54" t="str">
-        <f>IF($C$25&gt;=3,"λj ≦ q &lt; λj+1 の wBj+1", "-")</f>
-        <v>λj ≦ q &lt; λj+1 の wBj+1</v>
+        <v>331</v>
+      </c>
+      <c r="M132" s="54" t="s">
+        <v>341</v>
       </c>
       <c r="N132" s="44">
-        <f ca="1">IF($C$25&gt;=3, INDEX(INDIRECT($H$52&amp;"!C:C"), MATCH($N$58, INDIRECT($H$52&amp;"!A:A"), 0)),"-")</f>
-        <v>154.38900000000001</v>
+        <f ca="1">INDEX(INDIRECT($H$52&amp;"!C:C"), MATCH($N$58, INDIRECT($H$52&amp;"!A:A"), 0))</f>
+        <v>154.06299999999999</v>
       </c>
     </row>
     <row r="133" spans="11:14" x14ac:dyDescent="0.4">
@@ -22511,15 +22722,15 @@
         <v>133</v>
       </c>
       <c r="L133" s="45" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="M133" s="54" t="str">
-        <f>IF($C$25&gt;=4,"λj ≦ q+pz &lt; λj+1 の wBj+1", "-")</f>
-        <v>λj ≦ q+pz &lt; λj+1 の wBj+1</v>
+        <f>IF($C$25&gt;=3,"λj ≦ q &lt; λj+1 の wBj+1", "-")</f>
+        <v>λj ≦ q &lt; λj+1 の wBj+1</v>
       </c>
       <c r="N133" s="44">
-        <f ca="1">IF($C$25&gt;=4, INDEX(INDIRECT($H$52&amp;"!C:C"), MATCH($N$59, INDIRECT($H$52&amp;"!A:A"), 0)),"-")</f>
-        <v>154.27600000000001</v>
+        <f ca="1">IF($C$25&gt;=3, INDEX(INDIRECT($H$52&amp;"!C:C"), MATCH($N$59, INDIRECT($H$52&amp;"!A:A"), 0)),"-")</f>
+        <v>154.38900000000001</v>
       </c>
     </row>
     <row r="134" spans="11:14" x14ac:dyDescent="0.4">
@@ -22528,15 +22739,15 @@
         <v>134</v>
       </c>
       <c r="L134" s="45" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="M134" s="54" t="str">
-        <f>IF($C$25&gt;=5,"λj ≦ q+2pz &lt; λj+1 の wBj+1", "-")</f>
-        <v>λj ≦ q+2pz &lt; λj+1 の wBj+1</v>
+        <f>IF($C$25&gt;=4,"λj ≦ q+pz &lt; λj+1 の wBj+1", "-")</f>
+        <v>λj ≦ q+pz &lt; λj+1 の wBj+1</v>
       </c>
       <c r="N134" s="44">
-        <f ca="1">IF($C$25&gt;=5, INDEX(INDIRECT($H$52&amp;"!C:C"), MATCH($N$60, INDIRECT($H$52&amp;"!A:A"), 0)),"-")</f>
-        <v>154.16399999999999</v>
+        <f ca="1">IF($C$25&gt;=4, INDEX(INDIRECT($H$52&amp;"!C:C"), MATCH($N$60, INDIRECT($H$52&amp;"!A:A"), 0)),"-")</f>
+        <v>154.27600000000001</v>
       </c>
     </row>
     <row r="135" spans="11:14" x14ac:dyDescent="0.4">
@@ -22545,15 +22756,15 @@
         <v>135</v>
       </c>
       <c r="L135" s="45" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="M135" s="54" t="str">
-        <f>IF($C$25&gt;=6,"λj ≦ q+3pz &lt; λj+1 の wBj+1", "-")</f>
-        <v>λj ≦ q+3pz &lt; λj+1 の wBj+1</v>
+        <f>IF($C$25&gt;=5,"λj ≦ q+2pz &lt; λj+1 の wBj+1", "-")</f>
+        <v>λj ≦ q+2pz &lt; λj+1 の wBj+1</v>
       </c>
       <c r="N135" s="44">
-        <f ca="1">IF($C$25&gt;=6, INDEX(INDIRECT($H$52&amp;"!C:C"), MATCH($N$61, INDIRECT($H$52&amp;"!A:A"), 0)),"-")</f>
-        <v>154.06299999999999</v>
+        <f ca="1">IF($C$25&gt;=5, INDEX(INDIRECT($H$52&amp;"!C:C"), MATCH($N$61, INDIRECT($H$52&amp;"!A:A"), 0)),"-")</f>
+        <v>154.16399999999999</v>
       </c>
     </row>
     <row r="136" spans="11:14" x14ac:dyDescent="0.4">
@@ -22562,15 +22773,15 @@
         <v>136</v>
       </c>
       <c r="L136" s="45" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="M136" s="54" t="str">
-        <f>IF($C$25&gt;=7,"λj ≦ q+4pz &lt; λj+1 の wBj+1", "-")</f>
-        <v>-</v>
-      </c>
-      <c r="N136" s="44" t="str">
-        <f ca="1">IF($C$25&gt;=7, INDEX(INDIRECT($H$52&amp;"!C:C"), MATCH($N$62, INDIRECT($H$52&amp;"!A:A"), 0)),"-")</f>
-        <v>-</v>
+        <f>IF($C$25&gt;=6,"λj ≦ q+3pz &lt; λj+1 の wBj+1", "-")</f>
+        <v>λj ≦ q+3pz &lt; λj+1 の wBj+1</v>
+      </c>
+      <c r="N136" s="44">
+        <f ca="1">IF($C$25&gt;=6, INDEX(INDIRECT($H$52&amp;"!C:C"), MATCH($N$62, INDIRECT($H$52&amp;"!A:A"), 0)),"-")</f>
+        <v>154.06299999999999</v>
       </c>
     </row>
     <row r="137" spans="11:14" x14ac:dyDescent="0.4">
@@ -22579,14 +22790,14 @@
         <v>137</v>
       </c>
       <c r="L137" s="45" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="M137" s="54" t="str">
-        <f>IF($C$25&gt;=8,"λj ≦ q+5pz &lt; λj+1 の wBj+1", "-")</f>
+        <f>IF($C$25&gt;=7,"λj ≦ q+4pz &lt; λj+1 の wBj+1", "-")</f>
         <v>-</v>
       </c>
       <c r="N137" s="44" t="str">
-        <f ca="1">IF($C$25&gt;=8, INDEX(INDIRECT($H$52&amp;"!C:C"), MATCH($N$63, INDIRECT($H$52&amp;"!A:A"), 0)),"-")</f>
+        <f ca="1">IF($C$25&gt;=7, INDEX(INDIRECT($H$52&amp;"!C:C"), MATCH($N$63, INDIRECT($H$52&amp;"!A:A"), 0)),"-")</f>
         <v>-</v>
       </c>
     </row>
@@ -22596,14 +22807,15 @@
         <v>138</v>
       </c>
       <c r="L138" s="45" t="s">
-        <v>338</v>
-      </c>
-      <c r="M138" s="54" t="s">
-        <v>342</v>
-      </c>
-      <c r="N138" s="2">
-        <f ca="1">INDEX(INDIRECT($H$52&amp;"!C:C"), MATCH($N$64, INDIRECT($H$52&amp;"!A:A"), 0))</f>
-        <v>154.06299999999999</v>
+        <v>337</v>
+      </c>
+      <c r="M138" s="54" t="str">
+        <f>IF($C$25&gt;=8,"λj ≦ q+5pz &lt; λj+1 の wBj+1", "-")</f>
+        <v>-</v>
+      </c>
+      <c r="N138" s="44" t="str">
+        <f ca="1">IF($C$25&gt;=8, INDEX(INDIRECT($H$52&amp;"!C:C"), MATCH($N$64, INDIRECT($H$52&amp;"!A:A"), 0)),"-")</f>
+        <v>-</v>
       </c>
     </row>
     <row r="139" spans="11:14" x14ac:dyDescent="0.4">
@@ -22612,14 +22824,14 @@
         <v>139</v>
       </c>
       <c r="L139" s="45" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="M139" s="54" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="N139" s="2">
         <f ca="1">INDEX(INDIRECT($H$52&amp;"!C:C"), MATCH($N$65, INDIRECT($H$52&amp;"!A:A"), 0))</f>
-        <v>153.97200000000001</v>
+        <v>154.06299999999999</v>
       </c>
     </row>
     <row r="140" spans="11:14" x14ac:dyDescent="0.4">
@@ -22628,15 +22840,14 @@
         <v>140</v>
       </c>
       <c r="L140" s="45" t="s">
-        <v>360</v>
-      </c>
-      <c r="M140" s="55" t="str">
-        <f>IF($C$25&gt;=4,"2列目AC内径（水平・めっき含・概算）","-")</f>
-        <v>2列目AC内径（水平・めっき含・概算）</v>
-      </c>
-      <c r="N140" s="44">
-        <f ca="1">IF($C$25&gt;=4,($N$67*$N$99+$N$75*$N$91)/($N$59-$N$51)+$C$31*2,"-")</f>
-        <v>156.50139999999999</v>
+        <v>339</v>
+      </c>
+      <c r="M140" s="54" t="s">
+        <v>343</v>
+      </c>
+      <c r="N140" s="2">
+        <f ca="1">INDEX(INDIRECT($H$52&amp;"!C:C"), MATCH($N$66, INDIRECT($H$52&amp;"!A:A"), 0))</f>
+        <v>153.97200000000001</v>
       </c>
     </row>
     <row r="141" spans="11:14" x14ac:dyDescent="0.4">
@@ -22645,15 +22856,15 @@
         <v>141</v>
       </c>
       <c r="L141" s="45" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="M141" s="55" t="str">
-        <f>IF($C$25&gt;=5,"3列目AC内径（水平・めっき含・概算）","-")</f>
-        <v>3列目AC内径（水平・めっき含・概算）</v>
+        <f>IF($C$25&gt;=4,"2列目AC内径（水平・めっき含・概算）","-")</f>
+        <v>2列目AC内径（水平・めっき含・概算）</v>
       </c>
       <c r="N141" s="44">
-        <f ca="1">IF($C$25&gt;=5,($N$68*$N$100+$N$76*$N$92)/($N$60-$N$52)+$C$31*2,"-")</f>
-        <v>156.4102</v>
+        <f ca="1">IF($C$25&gt;=4,($N$68*$N$100+$N$76*$N$92)/($N$60-$N$52)+$C$31*2,"-")</f>
+        <v>156.50139999999999</v>
       </c>
     </row>
     <row r="142" spans="11:14" x14ac:dyDescent="0.4">
@@ -22662,15 +22873,15 @@
         <v>142</v>
       </c>
       <c r="L142" s="45" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="M142" s="55" t="str">
-        <f>IF($C$25&gt;=6,"4列目AC内径（水平・めっき含・概算）","-")</f>
-        <v>4列目AC内径（水平・めっき含・概算）</v>
+        <f>IF($C$25&gt;=5,"3列目AC内径（水平・めっき含・概算）","-")</f>
+        <v>3列目AC内径（水平・めっき含・概算）</v>
       </c>
       <c r="N142" s="44">
-        <f ca="1">IF($C$25&gt;=6,($N$69*$N$101+$N$77*$N$93)/($N$61-$N$53)+$C$31*2,"-")</f>
-        <v>156.31899999999999</v>
+        <f ca="1">IF($C$25&gt;=5,($N$69*$N$101+$N$77*$N$93)/($N$61-$N$53)+$C$31*2,"-")</f>
+        <v>156.4102</v>
       </c>
     </row>
     <row r="143" spans="11:14" x14ac:dyDescent="0.4">
@@ -22679,15 +22890,15 @@
         <v>143</v>
       </c>
       <c r="L143" s="45" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="M143" s="55" t="str">
-        <f>IF($C$25&gt;=7,"5列目AC内径（水平・めっき含・概算）","-")</f>
-        <v>-</v>
-      </c>
-      <c r="N143" s="44" t="str">
-        <f>IF($C$25&gt;=7,($N$70*$N$102+$N$78*$N$94)/($N$62-$N$54)+$C$31*2,"-")</f>
-        <v>-</v>
+        <f>IF($C$25&gt;=6,"4列目AC内径（水平・めっき含・概算）","-")</f>
+        <v>4列目AC内径（水平・めっき含・概算）</v>
+      </c>
+      <c r="N143" s="44">
+        <f ca="1">IF($C$25&gt;=6,($N$70*$N$102+$N$78*$N$94)/($N$62-$N$54)+$C$31*2,"-")</f>
+        <v>156.31899999999999</v>
       </c>
     </row>
     <row r="144" spans="11:14" x14ac:dyDescent="0.4">
@@ -22696,14 +22907,14 @@
         <v>144</v>
       </c>
       <c r="L144" s="45" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="M144" s="55" t="str">
-        <f>IF($C$25&gt;=8,"6列目AC内径（水平・めっき含・概算）","-")</f>
+        <f>IF($C$25&gt;=7,"5列目AC内径（水平・めっき含・概算）","-")</f>
         <v>-</v>
       </c>
       <c r="N144" s="44" t="str">
-        <f>IF($C$25&gt;=8,($N$71*$N$103+$N$79*$N$95)/($N$63-$N$55)+$C$31*2,"-")</f>
+        <f>IF($C$25&gt;=7,($N$71*$N$103+$N$79*$N$95)/($N$63-$N$55)+$C$31*2,"-")</f>
         <v>-</v>
       </c>
     </row>
@@ -22713,14 +22924,15 @@
         <v>145</v>
       </c>
       <c r="L145" s="45" t="s">
-        <v>365</v>
-      </c>
-      <c r="M145" s="55" t="s">
-        <v>350</v>
-      </c>
-      <c r="N145" s="2">
-        <f ca="1">($N$72*$N$104+$N$80*$N$96)/($N$64-$N$56)+$C$31*2</f>
-        <v>156.23739999999998</v>
+        <v>364</v>
+      </c>
+      <c r="M145" s="55" t="str">
+        <f>IF($C$25&gt;=8,"6列目AC内径（水平・めっき含・概算）","-")</f>
+        <v>-</v>
+      </c>
+      <c r="N145" s="44" t="str">
+        <f>IF($C$25&gt;=8,($N$72*$N$104+$N$80*$N$96)/($N$64-$N$56)+$C$31*2,"-")</f>
+        <v>-</v>
       </c>
     </row>
     <row r="146" spans="11:14" x14ac:dyDescent="0.4">
@@ -22729,14 +22941,14 @@
         <v>146</v>
       </c>
       <c r="L146" s="45" t="s">
-        <v>306</v>
+        <v>365</v>
       </c>
       <c r="M146" s="55" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="N146" s="2">
-        <f ca="1">INDEX(INDIRECT($H$52&amp;"!C:C"), MATCH(0, INDIRECT($H$52&amp;"!A:A"), 0))+$C$31*2</f>
-        <v>154.97899999999998</v>
+        <f ca="1">($N$73*$N$105+$N$81*$N$97)/($N$65-$N$57)+$C$31*2</f>
+        <v>156.23739999999998</v>
       </c>
     </row>
     <row r="147" spans="11:14" x14ac:dyDescent="0.4">
@@ -22745,15 +22957,14 @@
         <v>147</v>
       </c>
       <c r="L147" s="45" t="s">
-        <v>349</v>
-      </c>
-      <c r="M147" s="55" t="str">
-        <f>IF($C$25&gt;=3,"1列目 BD内径（めっき含・概算）","-")</f>
-        <v>1列目 BD内径（めっき含・概算）</v>
-      </c>
-      <c r="N147" s="44">
-        <f ca="1">IF($C$25&gt;=3,($N$66*$N$132+$N$74*$N$124)/($N$58-$N$50)+$C$31*2,"-")</f>
-        <v>154.57380000000001</v>
+        <v>306</v>
+      </c>
+      <c r="M147" s="55" t="s">
+        <v>352</v>
+      </c>
+      <c r="N147" s="2">
+        <f ca="1">INDEX(INDIRECT($H$52&amp;"!C:C"), MATCH(0, INDIRECT($H$52&amp;"!A:A"), 0))+$C$31*2</f>
+        <v>154.97899999999998</v>
       </c>
     </row>
     <row r="148" spans="11:14" x14ac:dyDescent="0.4">
@@ -22762,15 +22973,15 @@
         <v>148</v>
       </c>
       <c r="L148" s="45" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="M148" s="55" t="str">
-        <f>IF($C$25&gt;=4,"2列目 BD内径（めっき含・概算）","-")</f>
-        <v>2列目 BD内径（めっき含・概算）</v>
+        <f>IF($C$25&gt;=3,"1列目 BD内径（めっき含・概算）","-")</f>
+        <v>1列目 BD内径（めっき含・概算）</v>
       </c>
       <c r="N148" s="44">
-        <f ca="1">IF($C$25&gt;=4,($N$67*$N$133+$N$75*$N$125)/($N$59-$N$51)+$C$31*2,"-")</f>
-        <v>154.4838</v>
+        <f ca="1">IF($C$25&gt;=3,($N$67*$N$133+$N$75*$N$125)/($N$59-$N$51)+$C$31*2,"-")</f>
+        <v>154.57380000000001</v>
       </c>
     </row>
     <row r="149" spans="11:14" x14ac:dyDescent="0.4">
@@ -22779,15 +22990,15 @@
         <v>149</v>
       </c>
       <c r="L149" s="45" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="M149" s="55" t="str">
-        <f>IF($C$25&gt;=5,"3列目 BD内径（めっき含・概算）","-")</f>
-        <v>3列目 BD内径（めっき含・概算）</v>
+        <f>IF($C$25&gt;=4,"2列目 BD内径（めっき含・概算）","-")</f>
+        <v>2列目 BD内径（めっき含・概算）</v>
       </c>
       <c r="N149" s="44">
-        <f ca="1">IF($C$25&gt;=5,($N$68*$N$134+$N$76*$N$126)/($N$60-$N$52)+$C$31*2,"-")</f>
-        <v>154.39359999999999</v>
+        <f ca="1">IF($C$25&gt;=4,($N$68*$N$134+$N$76*$N$126)/($N$60-$N$52)+$C$31*2,"-")</f>
+        <v>154.4838</v>
       </c>
     </row>
     <row r="150" spans="11:14" x14ac:dyDescent="0.4">
@@ -22796,15 +23007,15 @@
         <v>150</v>
       </c>
       <c r="L150" s="45" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="M150" s="55" t="str">
-        <f>IF($C$25&gt;=6,"4列目 BD内径（めっき含・概算）","-")</f>
-        <v>4列目 BD内径（めっき含・概算）</v>
+        <f>IF($C$25&gt;=5,"3列目 BD内径（めっき含・概算）","-")</f>
+        <v>3列目 BD内径（めっき含・概算）</v>
       </c>
       <c r="N150" s="44">
-        <f ca="1">IF($C$25&gt;=6,($N$69*$N$135+$N$77*$N$127)/($N$61-$N$53)+$C$31*2,"-")</f>
-        <v>154.30399999999997</v>
+        <f ca="1">IF($C$25&gt;=5,($N$69*$N$135+$N$77*$N$127)/($N$61-$N$53)+$C$31*2,"-")</f>
+        <v>154.39359999999999</v>
       </c>
     </row>
     <row r="151" spans="11:14" x14ac:dyDescent="0.4">
@@ -22813,15 +23024,15 @@
         <v>151</v>
       </c>
       <c r="L151" s="45" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="M151" s="55" t="str">
-        <f>IF($C$25&gt;=7,"5列目 BD内径（めっき含・概算）","-")</f>
-        <v>-</v>
-      </c>
-      <c r="N151" s="44" t="str">
-        <f>IF($C$25&gt;=7,($N$70*$N$136+$N$78*$N$128)/($N$62-$N$54)+$C$31*2,"-")</f>
-        <v>-</v>
+        <f>IF($C$25&gt;=6,"4列目 BD内径（めっき含・概算）","-")</f>
+        <v>4列目 BD内径（めっき含・概算）</v>
+      </c>
+      <c r="N151" s="44">
+        <f ca="1">IF($C$25&gt;=6,($N$70*$N$136+$N$78*$N$128)/($N$62-$N$54)+$C$31*2,"-")</f>
+        <v>154.30399999999997</v>
       </c>
     </row>
     <row r="152" spans="11:14" x14ac:dyDescent="0.4">
@@ -22830,14 +23041,14 @@
         <v>152</v>
       </c>
       <c r="L152" s="45" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="M152" s="55" t="str">
-        <f>IF($C$25&gt;=8,"6列目 BD内径（めっき含・概算）","-")</f>
+        <f>IF($C$25&gt;=7,"5列目 BD内径（めっき含・概算）","-")</f>
         <v>-</v>
       </c>
       <c r="N152" s="44" t="str">
-        <f>IF($C$25&gt;=8,($N$71*$N$137+$N$79*$N$129)/($N$63-$N$55)+$C$31*2,"-")</f>
+        <f>IF($C$25&gt;=7,($N$71*$N$137+$N$79*$N$129)/($N$63-$N$55)+$C$31*2,"-")</f>
         <v>-</v>
       </c>
     </row>
@@ -22847,14 +23058,15 @@
         <v>153</v>
       </c>
       <c r="L153" s="45" t="s">
-        <v>359</v>
-      </c>
-      <c r="M153" s="55" t="s">
-        <v>353</v>
-      </c>
-      <c r="N153" s="2">
-        <f ca="1">($N$72*$N$138+$N$80*$N$130)/($N$64-$N$56)+$C$31*2</f>
-        <v>154.22319999999999</v>
+        <v>358</v>
+      </c>
+      <c r="M153" s="55" t="str">
+        <f>IF($C$25&gt;=8,"6列目 BD内径（めっき含・概算）","-")</f>
+        <v>-</v>
+      </c>
+      <c r="N153" s="44" t="str">
+        <f>IF($C$25&gt;=8,($N$72*$N$138+$N$80*$N$130)/($N$64-$N$56)+$C$31*2,"-")</f>
+        <v>-</v>
       </c>
     </row>
     <row r="154" spans="11:14" x14ac:dyDescent="0.4">
@@ -22862,6 +23074,16 @@
         <f t="shared" si="2"/>
         <v>154</v>
       </c>
+      <c r="L154" s="45" t="s">
+        <v>359</v>
+      </c>
+      <c r="M154" s="55" t="s">
+        <v>353</v>
+      </c>
+      <c r="N154" s="2">
+        <f ca="1">($N$73*$N$139+$N$81*$N$131)/($N$65-$N$57)+$C$31*2</f>
+        <v>154.22319999999999</v>
+      </c>
     </row>
     <row r="155" spans="11:14" x14ac:dyDescent="0.4">
       <c r="K155" s="3">
@@ -22880,13 +23102,6 @@
         <f t="shared" si="2"/>
         <v>157</v>
       </c>
-      <c r="L157" s="45" t="s">
-        <v>189</v>
-      </c>
-      <c r="N157" s="2">
-        <f>C6^2+(2*N9)^2</f>
-        <v>384450.50566139817</v>
-      </c>
     </row>
     <row r="158" spans="11:14" x14ac:dyDescent="0.4">
       <c r="K158" s="3">
@@ -22894,14 +23109,11 @@
         <v>158</v>
       </c>
       <c r="L158" s="45" t="s">
-        <v>190</v>
-      </c>
-      <c r="M158" s="54" t="s">
-        <v>29</v>
+        <v>189</v>
       </c>
       <c r="N158" s="2">
-        <f>SQRT(N157)</f>
-        <v>620.04072903430961</v>
+        <f>C6^2+(2*N9)^2</f>
+        <v>385003.74457739823</v>
       </c>
     </row>
     <row r="159" spans="11:14" x14ac:dyDescent="0.4">
@@ -22910,14 +23122,14 @@
         <v>159</v>
       </c>
       <c r="L159" s="45" t="s">
-        <v>64</v>
+        <v>190</v>
       </c>
       <c r="M159" s="54" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N159" s="2">
-        <f>2*N9/N158</f>
-        <v>0.99993431232433228</v>
+        <f>SQRT(N158)</f>
+        <v>620.4866997586638</v>
       </c>
     </row>
     <row r="160" spans="11:14" x14ac:dyDescent="0.4">
@@ -22926,14 +23138,14 @@
         <v>160</v>
       </c>
       <c r="L160" s="45" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M160" s="54" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N160" s="2">
-        <f>C6/N158</f>
-        <v>1.1461720484501746E-2</v>
+        <f>2*N9/N159</f>
+        <v>0.99993440671866196</v>
       </c>
     </row>
     <row r="161" spans="11:14" x14ac:dyDescent="0.4">
@@ -22942,11 +23154,14 @@
         <v>161</v>
       </c>
       <c r="L161" s="45" t="s">
-        <v>191</v>
+        <v>65</v>
+      </c>
+      <c r="M161" s="54" t="s">
+        <v>31</v>
       </c>
       <c r="N161" s="2">
-        <f>SQRT(N8^2-(N9-N12)^2)</f>
-        <v>8727.6739192066525</v>
+        <f>C6/N159</f>
+        <v>1.1453482448474855E-2</v>
       </c>
     </row>
     <row r="162" spans="11:14" x14ac:dyDescent="0.4">
@@ -22955,11 +23170,11 @@
         <v>162</v>
       </c>
       <c r="L162" s="45" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="N162" s="2">
-        <f>SQRT(N8^2-(N9+N12)^2)</f>
-        <v>8720.5671856823628</v>
+        <f>SQRT(N8^2-(N9-N12)^2)</f>
+        <v>8727.6685506652357</v>
       </c>
     </row>
     <row r="163" spans="11:14" x14ac:dyDescent="0.4">
@@ -22968,11 +23183,11 @@
         <v>163</v>
       </c>
       <c r="L163" s="45" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="N163" s="2">
-        <f>N12*N9</f>
-        <v>31000</v>
+        <f>SQRT(N8^2-(N9+N12)^2)</f>
+        <v>8720.5566984150155</v>
       </c>
     </row>
     <row r="164" spans="11:14" x14ac:dyDescent="0.4">
@@ -22981,11 +23196,11 @@
         <v>164</v>
       </c>
       <c r="L164" s="45" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="N164" s="2">
-        <f>SQRT(N8^2-N157/4)</f>
-        <v>8724.693657291622</v>
+        <f>N12*N9</f>
+        <v>31022.300000000003</v>
       </c>
     </row>
     <row r="165" spans="11:14" x14ac:dyDescent="0.4">
@@ -22994,11 +23209,11 @@
         <v>165</v>
       </c>
       <c r="L165" s="45" t="s">
-        <v>75</v>
+        <v>194</v>
       </c>
       <c r="N165" s="2">
-        <f>N164*N159</f>
-        <v>8724.1205524443612</v>
+        <f>SQRT(N8^2-N158/4)</f>
+        <v>8724.6857309507523</v>
       </c>
     </row>
     <row r="166" spans="11:14" x14ac:dyDescent="0.4">
@@ -23007,230 +23222,243 @@
         <v>166</v>
       </c>
       <c r="L166" s="45" t="s">
-        <v>76</v>
-      </c>
-      <c r="M166" s="54" t="s">
-        <v>27</v>
+        <v>75</v>
       </c>
       <c r="N166" s="2">
-        <f>N164*N160</f>
-        <v>100.00000001278184</v>
+        <f>N165*N160</f>
+        <v>8724.1134501850156</v>
       </c>
     </row>
     <row r="167" spans="11:14" x14ac:dyDescent="0.4">
       <c r="K167" s="3">
-        <f t="shared" ref="K167" si="3">ROW(K167)</f>
+        <f t="shared" si="2"/>
         <v>167</v>
       </c>
       <c r="L167" s="45" t="s">
+        <v>76</v>
+      </c>
+      <c r="M167" s="54" t="s">
+        <v>27</v>
+      </c>
+      <c r="N167" s="2">
+        <f>N165*N161</f>
+        <v>99.928034887903451</v>
+      </c>
+    </row>
+    <row r="168" spans="11:14" x14ac:dyDescent="0.4">
+      <c r="K168" s="3">
+        <f t="shared" ref="K168" si="3">ROW(K168)</f>
+        <v>168</v>
+      </c>
+      <c r="L168" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="M167" s="54" t="s">
+      <c r="M168" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="N167" s="2">
-        <f>C6/2+N7-N165</f>
-        <v>4.12719521204599</v>
-      </c>
-    </row>
-    <row r="182" spans="12:14" x14ac:dyDescent="0.4">
-      <c r="L182" s="54"/>
-      <c r="M182" s="55"/>
-      <c r="N182" s="1"/>
+      <c r="N168" s="2">
+        <f>C6/2+N7-N166</f>
+        <v>4.126371131180349</v>
+      </c>
+    </row>
+    <row r="183" spans="12:14" x14ac:dyDescent="0.4">
+      <c r="L183" s="54"/>
+      <c r="M183" s="55"/>
+      <c r="N183" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <conditionalFormatting sqref="C3">
-    <cfRule type="expression" dxfId="38" priority="29">
-      <formula>$C$3&gt;2*N163</formula>
+    <cfRule type="expression" dxfId="40" priority="30">
+      <formula>$C$3&gt;2*N164</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4">
-    <cfRule type="expression" dxfId="37" priority="22">
+    <cfRule type="expression" dxfId="39" priority="23">
       <formula>C4&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6">
-    <cfRule type="expression" dxfId="36" priority="14">
+    <cfRule type="expression" dxfId="38" priority="15">
       <formula>$C$6&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="expression" dxfId="35" priority="23">
+    <cfRule type="expression" dxfId="37" priority="24">
       <formula>$C$9&lt;=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10:C11">
-    <cfRule type="expression" dxfId="34" priority="15">
+    <cfRule type="expression" dxfId="36" priority="16">
       <formula>$C$10&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="expression" dxfId="33" priority="27">
+    <cfRule type="expression" dxfId="35" priority="28">
       <formula>OR(C15&lt;=0, C15&gt;Q2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="expression" dxfId="32" priority="21">
+    <cfRule type="expression" dxfId="34" priority="22">
       <formula>C35&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="expression" dxfId="31" priority="26">
+    <cfRule type="expression" dxfId="33" priority="27">
       <formula>OR($C$36&lt;0, $C$36&gt;=$C$9)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="expression" dxfId="30" priority="13">
+    <cfRule type="expression" dxfId="32" priority="14">
       <formula>OR($C$37&lt;0, $C$37&gt;=$C$10)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38">
-    <cfRule type="expression" dxfId="29" priority="28">
+    <cfRule type="expression" dxfId="31" priority="29">
       <formula>OR(C38&lt;0, C38&gt;=C9)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="expression" dxfId="28" priority="30">
+    <cfRule type="expression" dxfId="30" priority="31">
       <formula>OR(C41&lt;0, C41&gt;=C4)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44">
-    <cfRule type="expression" dxfId="27" priority="31">
+    <cfRule type="expression" dxfId="29" priority="32">
       <formula>OR(C44&lt;0, C44&gt;=C4)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="expression" dxfId="26" priority="25">
-      <formula>AND(C61&lt;&gt;330, C61&lt;&gt;270, C61&lt;&gt;250)</formula>
+    <cfRule type="expression" dxfId="28" priority="26">
+      <formula>AND(C61&lt;&gt;330.223, C61&lt;&gt;270, C61&lt;&gt;250)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="expression" dxfId="25" priority="24">
+    <cfRule type="expression" dxfId="27" priority="25">
       <formula>C62&lt;&gt;40</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C65">
-    <cfRule type="expression" dxfId="24" priority="17">
+    <cfRule type="expression" dxfId="26" priority="18">
       <formula>OR(C65&gt;0, ABS(ABS(C65)-740)&gt;=1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C66">
-    <cfRule type="expression" dxfId="23" priority="20">
+    <cfRule type="expression" dxfId="25" priority="21">
       <formula>OR(C66&gt;0, ABS(ABS(C66)-550)&gt;=1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C67">
-    <cfRule type="expression" dxfId="22" priority="18">
+    <cfRule type="expression" dxfId="24" priority="19">
       <formula>OR(C67&gt;0, ABS(ABS(C67)-1150)&gt;=1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C68">
-    <cfRule type="expression" dxfId="21" priority="19">
+    <cfRule type="expression" dxfId="23" priority="20">
       <formula>OR(ABS(C68)&gt;=0.2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H48">
-    <cfRule type="expression" dxfId="20" priority="16">
+    <cfRule type="expression" dxfId="22" priority="17">
       <formula>OR($H$48&lt;=1, INT($H$48)&lt;&gt;$H$48)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H52">
-    <cfRule type="expression" dxfId="19" priority="12">
+    <cfRule type="expression" dxfId="21" priority="13">
       <formula>ISERROR(INDIRECT($H$52&amp;"!$G$45"))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25">
-    <cfRule type="expression" dxfId="18" priority="32">
+    <cfRule type="expression" dxfId="20" priority="33">
       <formula>OR(C25-QUOTIENT(C25,1)&lt;&gt;0, C25&lt;0, C25&gt;$C$71)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H50">
-    <cfRule type="expression" dxfId="17" priority="11">
+    <cfRule type="expression" dxfId="19" priority="12">
       <formula>OR($H$50&lt;1, INT($H$50)&lt;&gt;$H$50)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H51">
-    <cfRule type="expression" dxfId="16" priority="10">
+    <cfRule type="expression" dxfId="18" priority="11">
       <formula>OR($H$51&lt;0, INT($H$51)&lt;&gt;$H$51)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23">
-    <cfRule type="expression" dxfId="15" priority="33">
+    <cfRule type="expression" dxfId="17" priority="34">
       <formula>OR($C$23&lt;=0, MOD($C$23,$C$22)&lt;&gt;0, $C$23&gt;=#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26">
-    <cfRule type="expression" dxfId="14" priority="34">
+    <cfRule type="expression" dxfId="16" priority="35">
       <formula>OR($C$26&lt;=0, $C$26&gt;=MIN($C$23, $C$24))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N140:N145">
-    <cfRule type="expression" dxfId="13" priority="9">
+  <conditionalFormatting sqref="N141:N146">
+    <cfRule type="expression" dxfId="15" priority="10">
       <formula>$H$51&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N146:N153">
-    <cfRule type="expression" dxfId="12" priority="8">
+  <conditionalFormatting sqref="N147:N154">
+    <cfRule type="expression" dxfId="14" priority="9">
       <formula>$H$51&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="expression" dxfId="11" priority="35">
+    <cfRule type="expression" dxfId="13" priority="36">
       <formula>OR(C16&lt;=0, C16+C15&gt;Q2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="expression" dxfId="10" priority="4">
+    <cfRule type="expression" dxfId="12" priority="5">
       <formula>G1="X"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="5">
+    <cfRule type="expression" dxfId="11" priority="6">
       <formula>G1="Y"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="6">
+    <cfRule type="expression" dxfId="10" priority="7">
       <formula>G1="Z"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="7">
+    <cfRule type="expression" dxfId="9" priority="8">
       <formula>G1="B"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H81:H96">
-    <cfRule type="expression" dxfId="6" priority="3">
+    <cfRule type="expression" dxfId="8" priority="4">
       <formula>$H$51&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="expression" dxfId="5" priority="36">
+    <cfRule type="expression" dxfId="7" priority="37">
       <formula>OR($C$17&lt;=0, $C$17&gt;=($C$9-#REF!)/2, $C$17&gt;=($C$36-#REF!)/2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H77">
-    <cfRule type="expression" dxfId="4" priority="37">
+    <cfRule type="expression" dxfId="6" priority="38">
       <formula>$H$77&lt;=$C$27/2+$C$28</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27">
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="5" priority="3">
       <formula>OR($C$27&lt;=0, $C$27&gt;$C$26)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H49">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="4" priority="2">
       <formula>OR($H$49&lt;0, INT($H$49)&lt;&gt;$H$49)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="expression" dxfId="1" priority="38">
+    <cfRule type="expression" dxfId="3" priority="39">
       <formula>OR($C$13&gt;=$C$9, $C$13&gt;=$C$42)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="expression" dxfId="0" priority="39">
+    <cfRule type="expression" dxfId="2" priority="40">
       <formula>OR($C$14&gt;=$C$10, $C$14&gt;=$C$42)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation imeMode="disabled" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H79 N140:N153 C49:C52 C55:C58 H54:H72 H81:H96 C3:C32 C60:C71 G1:G1048576" xr:uid="{976C4B3D-D3CF-4864-8086-225C218A19F1}"/>
+    <dataValidation imeMode="disabled" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H79 N141:N154 C49:C52 C55:C58 H54:H72 H81:H96 C3:C32 C60:C71 G1:G1048576 C76:C77" xr:uid="{976C4B3D-D3CF-4864-8086-225C218A19F1}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -25401,12 +25629,12 @@
   </sheetData>
   <phoneticPr fontId="1"/>
   <conditionalFormatting sqref="B2:D42">
-    <cfRule type="expression" dxfId="40" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>$A2&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:N42">
-    <cfRule type="expression" dxfId="39" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>$A2&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
debug from 20240229 test
</commit_message>
<xml_diff>
--- a/Mould_Numeriacl_Calculation/Mould_Postison_Cal.xlsx
+++ b/Mould_Numeriacl_Calculation/Mould_Postison_Cal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user01\Documents\GitHub\mould\Mould_Numeriacl_Calculation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E06768-10F1-405A-9559-32DA4A69262A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE3A986-FAFC-427D-BD67-24CABC036C3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="37710" windowHeight="21840" tabRatio="638" activeTab="1" xr2:uid="{331D296A-DE97-4357-9338-22F5C8F49D08}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" tabRatio="638" activeTab="1" xr2:uid="{331D296A-DE97-4357-9338-22F5C8F49D08}"/>
   </bookViews>
   <sheets>
     <sheet name="position_1916" sheetId="17" r:id="rId1"/>
@@ -18682,7 +18682,7 @@
   <dimension ref="A1:R183"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.4"/>
@@ -18756,11 +18756,11 @@
       </c>
       <c r="Q2" s="10">
         <f>C4+N167</f>
-        <v>499.92803488790344</v>
+        <v>479.92803488790344</v>
       </c>
       <c r="R2" s="10">
         <f>C67+Q2</f>
-        <v>-650.0459651120965</v>
+        <v>-670.0459651120965</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="15" thickTop="1" x14ac:dyDescent="0.4">
@@ -18784,11 +18784,11 @@
       </c>
       <c r="H3" s="30">
         <f>$C$4+$N$13*$N$5</f>
-        <v>500.0159494817317</v>
+        <v>480.0159494817317</v>
       </c>
       <c r="I3" s="30">
         <f>$C$67+H3</f>
-        <v>-649.95805051826824</v>
+        <v>-669.95805051826824</v>
       </c>
       <c r="K3" s="3">
         <f t="shared" ref="K3:K76" si="0">ROW(K3)</f>
@@ -18809,11 +18809,11 @@
       </c>
       <c r="Q3" s="10">
         <f>C4+C5-Q2</f>
-        <v>500.07196511209656</v>
+        <v>480.07196511209656</v>
       </c>
       <c r="R3" s="10">
         <f>C67+Q3</f>
-        <v>-649.90203488790337</v>
+        <v>-669.90203488790337</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.4">
@@ -18824,7 +18824,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="15">
-        <v>400</v>
+        <v>380</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>230</v>
@@ -18837,11 +18837,11 @@
       </c>
       <c r="H4" s="30">
         <f>$C$4+$C$5-$H$3</f>
-        <v>499.9840505182683</v>
+        <v>479.9840505182683</v>
       </c>
       <c r="I4" s="30">
         <f>$C$67+H4</f>
-        <v>-649.98994948173163</v>
+        <v>-669.98994948173163</v>
       </c>
       <c r="K4" s="3">
         <f t="shared" si="0"/>
@@ -18862,7 +18862,7 @@
       </c>
       <c r="Q4" s="10">
         <f>Q2-C61</f>
-        <v>169.70503488790342</v>
+        <v>149.70503488790342</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.4">
@@ -18873,7 +18873,7 @@
         <v>8</v>
       </c>
       <c r="C5" s="15">
-        <v>600</v>
+        <v>580</v>
       </c>
       <c r="D5" s="2"/>
       <c r="F5" s="9" t="s">
@@ -18884,7 +18884,7 @@
       </c>
       <c r="H5" s="30">
         <f>$H$3-$C$61</f>
-        <v>169.79294948173168</v>
+        <v>149.79294948173168</v>
       </c>
       <c r="K5" s="3">
         <f t="shared" si="0"/>
@@ -18902,7 +18902,7 @@
       </c>
       <c r="Q5" s="10">
         <f>Q3-C61</f>
-        <v>169.84896511209655</v>
+        <v>149.84896511209655</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.4">
@@ -18921,7 +18921,7 @@
       </c>
       <c r="H6" s="50">
         <f>$H$4-$C$61</f>
-        <v>169.76105051826829</v>
+        <v>149.76105051826829</v>
       </c>
       <c r="K6" s="3">
         <f t="shared" si="0"/>
@@ -19022,11 +19022,11 @@
       </c>
       <c r="Q8" s="10">
         <f>-C64+(N16+N17)/2+C6/2-N166</f>
-        <v>-8.3314551675721304</v>
+        <v>-7.4563490253094642</v>
       </c>
       <c r="R8" s="10">
         <f t="shared" ref="R8:R14" si="1">$C$66+Q8</f>
-        <v>-558.35045516757214</v>
+        <v>-557.47534902530947</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.4">
@@ -19058,11 +19058,11 @@
       </c>
       <c r="Q9" s="10">
         <f>-C64+N15+C6/2-N166</f>
-        <v>-8.3304885782927158</v>
+        <v>-7.4554769353744632</v>
       </c>
       <c r="R9" s="10">
         <f t="shared" si="1"/>
-        <v>-558.34948857829272</v>
+        <v>-557.47447693537447</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.4">
@@ -19096,11 +19096,11 @@
       </c>
       <c r="Q10" s="10">
         <f>C64-(N19+N20)/2-C6/2+N166</f>
-        <v>19.558388925497638</v>
+        <v>18.232873764451142</v>
       </c>
       <c r="R10" s="10">
         <f t="shared" si="1"/>
-        <v>-530.46061107450237</v>
+        <v>-531.78612623554886</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.4">
@@ -19135,11 +19135,11 @@
       </c>
       <c r="Q11" s="10">
         <f>C64-N18-C6/2+N166</f>
-        <v>19.556205860779301</v>
+        <v>18.230834722731743</v>
       </c>
       <c r="R11" s="10">
         <f t="shared" si="1"/>
-        <v>-530.4627941392207</v>
+        <v>-531.78816527726826</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.4">
@@ -19157,11 +19157,11 @@
       </c>
       <c r="H12" s="30">
         <f>$N$21-$N$13*$N$6</f>
-        <v>-11.897480389039629</v>
+        <v>-11.022374246776963</v>
       </c>
       <c r="I12" s="30">
         <f>$C$66+H12</f>
-        <v>-561.91648038903963</v>
+        <v>-561.04137424677697</v>
       </c>
       <c r="K12" s="3">
         <f t="shared" si="0"/>
@@ -19204,11 +19204,11 @@
       </c>
       <c r="H13" s="30">
         <f>$N$13*$N$6-$N$22</f>
-        <v>23.124414146965137</v>
+        <v>21.79889898591864</v>
       </c>
       <c r="I13" s="30">
         <f>$C$66+H13</f>
-        <v>-526.89458585303487</v>
+        <v>-528.22010101408137</v>
       </c>
       <c r="K13" s="3">
         <f t="shared" si="0"/>
@@ -19251,11 +19251,11 @@
       </c>
       <c r="H14" s="30">
         <f>$N$15-$N$13*$N$6</f>
-        <v>-11.896513799760214</v>
+        <v>-11.021502156841962</v>
       </c>
       <c r="I14" s="30">
         <f>$C$66+H14</f>
-        <v>-561.91551379976022</v>
+        <v>-561.04050215684197</v>
       </c>
       <c r="K14" s="3">
         <f t="shared" si="0"/>
@@ -19302,11 +19302,11 @@
       </c>
       <c r="H15" s="30">
         <f>$N$13*$N$6-$N$18</f>
-        <v>23.122231082246799</v>
+        <v>21.796859944199241</v>
       </c>
       <c r="I15" s="30">
         <f>$C$66+H15</f>
-        <v>-526.89676891775321</v>
+        <v>-528.22214005580076</v>
       </c>
       <c r="K15" s="3">
         <f t="shared" si="0"/>
@@ -19320,14 +19320,14 @@
       </c>
       <c r="N15" s="2">
         <f>SQRT($C$3^2-$C$4^2)</f>
-        <v>8913.7295948441242</v>
+        <v>8914.6046064870425</v>
       </c>
       <c r="P15" s="10" t="s">
         <v>48</v>
       </c>
       <c r="Q15" s="10">
         <f>N28-N15</f>
-        <v>0.70683627001562854</v>
+        <v>0.67070526721727219</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.4">
@@ -19355,7 +19355,7 @@
       </c>
       <c r="N16" s="2">
         <f>SQRT($N$11^2-$C$4^2)</f>
-        <v>9006.321726431941</v>
+        <v>9007.1877431304838</v>
       </c>
       <c r="P16" s="10" t="s">
         <v>49</v>
@@ -19393,18 +19393,18 @@
       </c>
       <c r="N17" s="2">
         <f>SQRT($N$10^2-$C$4^2)</f>
-        <v>8821.1355300777468</v>
+        <v>8822.019725663733</v>
       </c>
       <c r="P17" s="10" t="s">
         <v>51</v>
       </c>
       <c r="Q17" s="10">
         <f>N28-C64+C6/2-N166</f>
-        <v>-7.6236523082770873</v>
+        <v>-6.784771668157191</v>
       </c>
       <c r="R17" s="10">
         <f>$C$66+Q17</f>
-        <v>-557.64265230827709</v>
+        <v>-556.8037716681572</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.4">
@@ -19434,7 +19434,7 @@
       </c>
       <c r="N18" s="2">
         <f>SQRT($C$3^2-$C$5^2)</f>
-        <v>8902.5038775616376</v>
+        <v>8903.8292486996852</v>
       </c>
       <c r="P18" s="10" t="s">
         <v>46</v>
@@ -19477,18 +19477,18 @@
       </c>
       <c r="N19" s="2">
         <f>SQRT($N$11^2-$C$5^2)</f>
-        <v>8995.2115617143772</v>
+        <v>8996.5232751324565</v>
       </c>
       <c r="P19" s="10" t="s">
         <v>45</v>
       </c>
       <c r="Q19" s="10">
         <f>N29-C17-C13/2+N168-N13</f>
-        <v>-7.6247869906728738</v>
+        <v>-6.7945285634559696</v>
       </c>
       <c r="R19" s="10">
         <f>$C$66+Q19</f>
-        <v>-557.64378699067288</v>
+        <v>-556.81352856345598</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.4">
@@ -19510,11 +19510,11 @@
       </c>
       <c r="H20" s="30">
         <f ca="1">$H$13-$N$42-$H$18/2-$C$31-$C$35+$C$42/2</f>
-        <v>22.201087937634938</v>
+        <v>20.898132840539901</v>
       </c>
       <c r="I20" s="30">
         <f ca="1">$C$66+H20</f>
-        <v>-527.81791206236505</v>
+        <v>-529.12086715946009</v>
       </c>
       <c r="K20" s="3">
         <f t="shared" si="0"/>
@@ -19528,18 +19528,18 @@
       </c>
       <c r="N20" s="2">
         <f>SQRT($N$10^2-$C$5^2)</f>
-        <v>8809.7918272794614</v>
+        <v>8811.131144183475</v>
       </c>
       <c r="P20" s="10" t="s">
         <v>47</v>
       </c>
       <c r="Q20" s="10">
         <f>Q3-Q16</f>
-        <v>483.99696511209658</v>
+        <v>463.99696511209658</v>
       </c>
       <c r="R20" s="10">
         <f>C67+Q20</f>
-        <v>-665.9770348879033</v>
+        <v>-685.9770348879033</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.4">
@@ -19561,11 +19561,11 @@
       </c>
       <c r="H21" s="30">
         <f ca="1">-$H$20+$C$46</f>
-        <v>-11.201087937634938</v>
+        <v>-9.8981328405399012</v>
       </c>
       <c r="I21" s="30">
         <f ca="1">$C$66+H21</f>
-        <v>-561.22008793763496</v>
+        <v>-559.91713284053992</v>
       </c>
       <c r="K21" s="3">
         <f t="shared" si="0"/>
@@ -19579,7 +19579,7 @@
       </c>
       <c r="N21" s="2">
         <f>($N$16+$N$17)/2</f>
-        <v>8913.7286282548448</v>
+        <v>8914.6037343971075</v>
       </c>
       <c r="P21" s="10" t="s">
         <v>56</v>
@@ -19625,7 +19625,7 @@
       </c>
       <c r="N22" s="2">
         <f>($N$19+$N$20)/2</f>
-        <v>8902.5016944969193</v>
+        <v>8903.8272096579658</v>
       </c>
       <c r="P22" s="10" t="s">
         <v>57</v>
@@ -19696,11 +19696,11 @@
       </c>
       <c r="H24" s="30">
         <f ca="1">-$N$13*$N$6+$N$21+$H$22/2+$C$41-$C$42/2</f>
-        <v>-11.195980389039619</v>
+        <v>-10.320874246776953</v>
       </c>
       <c r="I24" s="30">
         <f ca="1">$C$66+H24</f>
-        <v>-561.21498038903962</v>
+        <v>-560.33987424677696</v>
       </c>
       <c r="K24" s="3">
         <f t="shared" si="0"/>
@@ -19714,14 +19714,14 @@
       </c>
       <c r="N24" s="2">
         <f>$C$4-$N$23</f>
-        <v>383.92500000000001</v>
+        <v>363.92500000000001</v>
       </c>
       <c r="P24" s="10" t="s">
         <v>69</v>
       </c>
       <c r="Q24" s="10">
         <f ca="1">Q9*$N$108+Q2*$N$75</f>
-        <v>-69983.416521525956</v>
+        <v>-62307.439961161843</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.4">
@@ -19742,11 +19742,11 @@
       </c>
       <c r="H25" s="30">
         <f>$H$3-$C$43</f>
-        <v>468.0159494817317</v>
+        <v>448.0159494817317</v>
       </c>
       <c r="I25" s="30">
         <f>$C$67+H25</f>
-        <v>-681.95805051826824</v>
+        <v>-701.95805051826824</v>
       </c>
       <c r="K25" s="3">
         <f t="shared" si="0"/>
@@ -19767,7 +19767,7 @@
       </c>
       <c r="Q25" s="10">
         <f ca="1">-Q$9*$N$75+Q$2*$N$108</f>
-        <v>4499933.6971780732</v>
+        <v>4319905.021061644</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.4">
@@ -19785,11 +19785,11 @@
       </c>
       <c r="H26" s="30">
         <f>$H$4-$C$38</f>
-        <v>474.9840505182683</v>
+        <v>454.9840505182683</v>
       </c>
       <c r="I26" s="30">
         <f>$C$67+H26</f>
-        <v>-674.98994948173163</v>
+        <v>-694.98994948173163</v>
       </c>
       <c r="K26" s="3">
         <f t="shared" si="0"/>
@@ -19803,7 +19803,7 @@
       </c>
       <c r="N26" s="2">
         <f>$C$4-$N$25</f>
-        <v>379.9</v>
+        <v>359.9</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.4">
@@ -19827,7 +19827,7 @@
       </c>
       <c r="N27" s="2">
         <f>$C$4-$C$15</f>
-        <v>387.95</v>
+        <v>367.95</v>
       </c>
       <c r="P27" s="2"/>
     </row>
@@ -19856,7 +19856,7 @@
       </c>
       <c r="N28" s="2">
         <f>SQRT($C$3^2-$N$24^2)</f>
-        <v>8914.4364311141399</v>
+        <v>8915.2753117542597</v>
       </c>
       <c r="P28" s="2"/>
     </row>
@@ -19871,11 +19871,11 @@
       </c>
       <c r="H29" s="30">
         <f>$H$3-$C$15</f>
-        <v>487.96594948173168</v>
+        <v>467.96594948173168</v>
       </c>
       <c r="I29" s="30">
         <f>$C$67+H29</f>
-        <v>-662.00805051826819</v>
+        <v>-682.00805051826819</v>
       </c>
       <c r="K29" s="3">
         <f t="shared" si="0"/>
@@ -19889,7 +19889,7 @@
       </c>
       <c r="N29" s="2">
         <f>SQRT($N$11^2-$N$24^2)</f>
-        <v>9007.0212964317452</v>
+        <v>9007.8515548589621</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.4">
@@ -19905,11 +19905,11 @@
       </c>
       <c r="H30" s="30">
         <f>$H$29-$C$16</f>
-        <v>479.91594948173167</v>
+        <v>459.91594948173167</v>
       </c>
       <c r="I30" s="30">
         <f>$C$67+H30</f>
-        <v>-670.05805051826826</v>
+        <v>-690.05805051826826</v>
       </c>
       <c r="K30" s="3">
         <f t="shared" si="0"/>
@@ -19923,7 +19923,7 @@
       </c>
       <c r="N30" s="2">
         <f>SQRT($N$10^2-$N$24^2)</f>
-        <v>8821.8497852987166</v>
+        <v>8822.6974692763324</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.4">
@@ -19944,11 +19944,11 @@
       </c>
       <c r="H31" s="30">
         <f>$H$3-$N$23</f>
-        <v>483.94094948173171</v>
+        <v>463.94094948173171</v>
       </c>
       <c r="I31" s="30">
         <f>$C$67+H31</f>
-        <v>-666.03305051826828</v>
+        <v>-686.03305051826828</v>
       </c>
       <c r="K31" s="3">
         <f t="shared" si="0"/>
@@ -19962,7 +19962,7 @@
       </c>
       <c r="N31" s="2">
         <f>SQRT($N$11^2-$N$26^2)</f>
-        <v>9007.1919614272683</v>
+        <v>9008.0132676412068</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.4">
@@ -19980,7 +19980,7 @@
       </c>
       <c r="H32" s="30">
         <f>$N$28-$N$15</f>
-        <v>0.70683627001562854</v>
+        <v>0.67070526721727219</v>
       </c>
       <c r="K32" s="3">
         <f t="shared" si="0"/>
@@ -19994,7 +19994,7 @@
       </c>
       <c r="N32" s="2">
         <f>SQRT($N$11^2-$N$27^2)</f>
-        <v>9006.8488295019142</v>
+        <v>9007.6880406406181</v>
       </c>
     </row>
     <row r="33" spans="2:16" x14ac:dyDescent="0.4">
@@ -20006,11 +20006,11 @@
       </c>
       <c r="H33" s="30">
         <f>$N$28-$N$13*$N$6</f>
-        <v>-11.189677529744586</v>
+        <v>-10.350796889624689</v>
       </c>
       <c r="I33" s="30">
         <f>$C$66+H33</f>
-        <v>-561.20867752974459</v>
+        <v>-560.36979688962469</v>
       </c>
       <c r="K33" s="3">
         <f t="shared" si="0"/>
@@ -20024,7 +20024,7 @@
       </c>
       <c r="N33" s="2">
         <f>($N$31-$N$32)/$C$16</f>
-        <v>4.262508389491932E-2</v>
+        <v>4.040086963834922E-2</v>
       </c>
     </row>
     <row r="34" spans="2:16" x14ac:dyDescent="0.4">
@@ -20039,11 +20039,11 @@
       </c>
       <c r="H34" s="30">
         <f ca="1">$H$21</f>
-        <v>-11.201087937634938</v>
+        <v>-9.8981328405399012</v>
       </c>
       <c r="I34" s="30">
         <f ca="1">$C$66+H34</f>
-        <v>-561.22008793763496</v>
+        <v>-559.91713284053992</v>
       </c>
       <c r="K34" s="3">
         <f t="shared" si="0"/>
@@ -20057,7 +20057,7 @@
       </c>
       <c r="N34" s="2">
         <f>SIN(ATAN($N$33))</f>
-        <v>4.2586413871470295E-2</v>
+        <v>4.0367938185526558E-2</v>
       </c>
     </row>
     <row r="35" spans="2:16" x14ac:dyDescent="0.4">
@@ -20075,11 +20075,11 @@
       </c>
       <c r="H35" s="30">
         <f>$N$29-$C$17-$C$13/2-$N$13</f>
-        <v>-11.751158121853223</v>
+        <v>-10.920899694636319</v>
       </c>
       <c r="I35" s="30">
         <f>$C$66+H35</f>
-        <v>-561.77015812185323</v>
+        <v>-560.93989969463632</v>
       </c>
       <c r="K35" s="3">
         <f t="shared" si="0"/>
@@ -20093,7 +20093,7 @@
       </c>
       <c r="N35" s="2">
         <f>COS(ATAN($N$33))</f>
-        <v>0.99909278715921468</v>
+        <v>0.99918488257511662</v>
       </c>
     </row>
     <row r="36" spans="2:16" x14ac:dyDescent="0.4">
@@ -20122,7 +20122,7 @@
       </c>
       <c r="N36" s="2">
         <f>2*$N$35/(1+$N$35^2)</f>
-        <v>0.99999958810892742</v>
+        <v>0.99999966752089275</v>
       </c>
     </row>
     <row r="37" spans="2:16" x14ac:dyDescent="0.4">
@@ -20140,11 +20140,11 @@
       </c>
       <c r="H37" s="30">
         <f ca="1">$H$24</f>
-        <v>-11.195980389039619</v>
+        <v>-10.320874246776953</v>
       </c>
       <c r="I37" s="30">
         <f ca="1">$C$66+H37</f>
-        <v>-561.21498038903962</v>
+        <v>-560.33987424677696</v>
       </c>
       <c r="K37" s="3">
         <f>ROW(K37)</f>
@@ -20158,7 +20158,7 @@
       </c>
       <c r="N37" s="2">
         <f>$N$29-$N$32</f>
-        <v>0.1724669298309891</v>
+        <v>0.1635142183440621</v>
       </c>
     </row>
     <row r="38" spans="2:16" x14ac:dyDescent="0.4">
@@ -20181,7 +20181,7 @@
       </c>
       <c r="N38" s="2">
         <f>$C$16*$N$34/2</f>
-        <v>0.17141031583266794</v>
+        <v>0.16248095119674441</v>
       </c>
     </row>
     <row r="39" spans="2:16" x14ac:dyDescent="0.4">
@@ -20205,7 +20205,7 @@
       </c>
       <c r="N39" s="2">
         <f>$N$36*($C$17-$N$38)+$N$37</f>
-        <v>6.1370541572370785</v>
+        <v>6.1370312810770375</v>
       </c>
     </row>
     <row r="40" spans="2:16" x14ac:dyDescent="0.4">
@@ -20221,11 +20221,11 @@
       </c>
       <c r="H40" s="30">
         <f>$H$3-$C$55</f>
-        <v>499.0159494817317</v>
+        <v>479.0159494817317</v>
       </c>
       <c r="I40" s="30">
         <f>$C$67+H40</f>
-        <v>-650.95805051826824</v>
+        <v>-670.95805051826824</v>
       </c>
       <c r="K40" s="3">
         <f t="shared" si="0"/>
@@ -20239,7 +20239,7 @@
       </c>
       <c r="N40" s="2">
         <f>$C$5-$C$51</f>
-        <v>590</v>
+        <v>570</v>
       </c>
       <c r="P40" s="2"/>
     </row>
@@ -20259,11 +20259,11 @@
       </c>
       <c r="H41" s="30">
         <f>$H$3-$C$57</f>
-        <v>499.5159494817317</v>
+        <v>479.5159494817317</v>
       </c>
       <c r="I41" s="30">
         <f>$C$67+H41</f>
-        <v>-650.45805051826824</v>
+        <v>-670.45805051826824</v>
       </c>
       <c r="K41" s="3">
         <f t="shared" si="0"/>
@@ -20277,7 +20277,7 @@
       </c>
       <c r="N41" s="2">
         <f>SQRT($C$3^2-$N$40^2)</f>
-        <v>8903.1722037709678</v>
+        <v>8904.4750148450639</v>
       </c>
     </row>
     <row r="42" spans="2:16" x14ac:dyDescent="0.4">
@@ -20295,11 +20295,11 @@
       </c>
       <c r="H42" s="30">
         <f>$H$4-$C$49</f>
-        <v>495.9840505182683</v>
+        <v>475.9840505182683</v>
       </c>
       <c r="I42" s="30">
         <f>$C$67+H42</f>
-        <v>-653.98994948173163</v>
+        <v>-673.98994948173163</v>
       </c>
       <c r="K42" s="3">
         <f t="shared" si="0"/>
@@ -20310,7 +20310,7 @@
       </c>
       <c r="N42" s="2">
         <f>N41-N18</f>
-        <v>0.66832620933018916</v>
+        <v>0.64576614537872956</v>
       </c>
     </row>
     <row r="43" spans="2:16" x14ac:dyDescent="0.4">
@@ -20328,11 +20328,11 @@
       </c>
       <c r="H43" s="30">
         <f>$H$4-$C$51</f>
-        <v>489.9840505182683</v>
+        <v>469.9840505182683</v>
       </c>
       <c r="I43" s="30">
         <f>$C$67+H43</f>
-        <v>-659.98994948173163</v>
+        <v>-679.98994948173163</v>
       </c>
       <c r="K43" s="3">
         <f t="shared" si="0"/>
@@ -20347,7 +20347,7 @@
       </c>
       <c r="N43" s="44">
         <f>$C$4-$C$20</f>
-        <v>310</v>
+        <v>290</v>
       </c>
     </row>
     <row r="44" spans="2:16" x14ac:dyDescent="0.4">
@@ -20372,7 +20372,7 @@
       </c>
       <c r="N44" s="44">
         <f>IF($C$25&gt;=4,$N$43-1*$C$21, "-")</f>
-        <v>290</v>
+        <v>270</v>
       </c>
     </row>
     <row r="45" spans="2:16" x14ac:dyDescent="0.4">
@@ -20387,7 +20387,7 @@
       </c>
       <c r="H45" s="30">
         <f>$N$41-$N$18</f>
-        <v>0.66832620933018916</v>
+        <v>0.64576614537872956</v>
       </c>
       <c r="I45" s="51"/>
       <c r="K45" s="3">
@@ -20403,7 +20403,7 @@
       </c>
       <c r="N45" s="44">
         <f>IF($C$25&gt;=5,$N$43-2*$C$21, "-")</f>
-        <v>270</v>
+        <v>250</v>
       </c>
     </row>
     <row r="46" spans="2:16" x14ac:dyDescent="0.4">
@@ -20430,7 +20430,7 @@
       </c>
       <c r="N46" s="44">
         <f>IF($C$25&gt;=6,$N$43-3*$C$21, "-")</f>
-        <v>250</v>
+        <v>230</v>
       </c>
     </row>
     <row r="47" spans="2:16" x14ac:dyDescent="0.4">
@@ -20520,7 +20520,7 @@
       </c>
       <c r="N49" s="44">
         <f>$N$43-($C$25-2)*$C$21</f>
-        <v>230</v>
+        <v>210</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.4">
@@ -20552,7 +20552,7 @@
       </c>
       <c r="N50" s="44">
         <f>$N$43-($C$25-1)*$C$21</f>
-        <v>210</v>
+        <v>190</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.4">
@@ -20657,7 +20657,7 @@
       </c>
       <c r="H54" s="30">
         <f>IF($C$25&gt;=$C$71-5,$N$83-$N$15, "-")</f>
-        <v>3.5836378510248323</v>
+        <v>3.3814492320398131</v>
       </c>
       <c r="K54" s="3">
         <f t="shared" si="0"/>
@@ -20694,7 +20694,7 @@
       </c>
       <c r="H55" s="30">
         <f>IF($C$25&gt;=$C71-4,$N$84-$N$15, "-")</f>
-        <v>4.2564608749580657</v>
+        <v>4.0093715927359881</v>
       </c>
       <c r="K55" s="3">
         <f t="shared" si="0"/>
@@ -20728,7 +20728,7 @@
       </c>
       <c r="H56" s="30">
         <f>IF($C$25&gt;=$C$71-3,$N$85-$N$15, "-")</f>
-        <v>4.8843832356542407</v>
+        <v>4.5924027733763069</v>
       </c>
       <c r="K56" s="3">
         <f t="shared" si="0"/>
@@ -20762,7 +20762,7 @@
       </c>
       <c r="H57" s="30">
         <f>IF($C$25&gt;=$C$71-2,$N$86-$N$15, "-")</f>
-        <v>5.4674144162945595</v>
+        <v>5.1305515767890029</v>
       </c>
       <c r="K57" s="3">
         <f t="shared" si="0"/>
@@ -20853,7 +20853,7 @@
       </c>
       <c r="H60" s="30">
         <f>$N$89-$N$15</f>
-        <v>6.0055632197072555</v>
+        <v>5.6238261261041771</v>
       </c>
       <c r="K60" s="3">
         <f t="shared" si="0"/>
@@ -20893,7 +20893,7 @@
       </c>
       <c r="H61" s="30">
         <f>$N$90-$N$15</f>
-        <v>6.4988377690224297</v>
+        <v>6.0722338653758925</v>
       </c>
       <c r="K61" s="3">
         <f t="shared" si="0"/>
@@ -20933,11 +20933,11 @@
       </c>
       <c r="H62" s="60">
         <f>IF($C$25&gt;=3,$H$3-$C$20,"-")</f>
-        <v>410.0159494817317</v>
+        <v>390.0159494817317</v>
       </c>
       <c r="I62" s="30">
         <f>IF($C$25&gt;=3,$C$67+H62,"-")</f>
-        <v>-739.95805051826824</v>
+        <v>-759.95805051826824</v>
       </c>
       <c r="K62" s="3">
         <f t="shared" si="0"/>
@@ -20977,11 +20977,11 @@
       </c>
       <c r="H63" s="60">
         <f>IF($C$25&gt;=4,$H$3-$C$20-$C$21,"-")</f>
-        <v>390.0159494817317</v>
+        <v>370.0159494817317</v>
       </c>
       <c r="I63" s="30">
         <f>IF($C$25&gt;=4,$C$67+H63,"-")</f>
-        <v>-759.95805051826824</v>
+        <v>-779.95805051826824</v>
       </c>
       <c r="K63" s="3">
         <f t="shared" si="0"/>
@@ -21018,11 +21018,11 @@
       </c>
       <c r="H64" s="60">
         <f>IF($C$25&gt;=5,$H$3-$C$20-2*$C$21,"-")</f>
-        <v>370.0159494817317</v>
+        <v>350.0159494817317</v>
       </c>
       <c r="I64" s="30">
         <f>IF($C$25&gt;=5,$C$67+H64,"-")</f>
-        <v>-779.95805051826824</v>
+        <v>-799.95805051826824</v>
       </c>
       <c r="K64" s="3">
         <f t="shared" si="0"/>
@@ -21056,11 +21056,11 @@
       </c>
       <c r="H65" s="60">
         <f>IF($C$25&gt;=6,$H$3-$C$20-3*$C$21,"-")</f>
-        <v>350.0159494817317</v>
+        <v>330.0159494817317</v>
       </c>
       <c r="I65" s="30">
         <f>IF($C$25&gt;=6,$C$67+H65,"-")</f>
-        <v>-799.95805051826824</v>
+        <v>-819.95805051826824</v>
       </c>
       <c r="K65" s="3">
         <f t="shared" si="0"/>
@@ -21168,11 +21168,11 @@
       </c>
       <c r="H68" s="60">
         <f>$H$3-$C$20-($C$25-2)*$C$21</f>
-        <v>330.0159494817317</v>
+        <v>310.0159494817317</v>
       </c>
       <c r="I68" s="30">
         <f>$C$67+H68</f>
-        <v>-819.95805051826824</v>
+        <v>-839.95805051826824</v>
       </c>
       <c r="K68" s="3">
         <f t="shared" si="0"/>
@@ -21208,11 +21208,11 @@
       </c>
       <c r="H69" s="60">
         <f>$H$3-$C$20-($C$25-1)*$C$21</f>
-        <v>310.0159494817317</v>
+        <v>290.0159494817317</v>
       </c>
       <c r="I69" s="30">
         <f>$C$67+H69</f>
-        <v>-839.95805051826824</v>
+        <v>-859.95805051826824</v>
       </c>
       <c r="K69" s="3">
         <f t="shared" si="0"/>
@@ -21348,7 +21348,7 @@
       </c>
       <c r="H73" s="30">
         <f ca="1">ROUND(DEGREES($N$112),3)</f>
-        <v>2.13</v>
+        <v>2.0019999999999998</v>
       </c>
       <c r="I73" s="5"/>
       <c r="K73" s="3">
@@ -21384,11 +21384,11 @@
       </c>
       <c r="H74" s="30">
         <f ca="1">$H$7+$H$73</f>
-        <v>2.7719999999999998</v>
+        <v>2.6439999999999997</v>
       </c>
       <c r="I74" s="30">
         <f ca="1">-$C$68+$H$74</f>
-        <v>2.6989999999999998</v>
+        <v>2.5709999999999997</v>
       </c>
       <c r="K74" s="3">
         <f t="shared" si="0"/>
@@ -21417,7 +21417,7 @@
       </c>
       <c r="H75" s="56">
         <f ca="1">DEGREES($N$120)</f>
-        <v>1.8081075579837422</v>
+        <v>1.6784998296714242</v>
       </c>
       <c r="K75" s="3">
         <f t="shared" si="0"/>
@@ -21453,11 +21453,11 @@
       </c>
       <c r="H76" s="56">
         <f ca="1">$H$7+$H$75</f>
-        <v>2.4501075579837424</v>
+        <v>2.3204998296714243</v>
       </c>
       <c r="I76" s="56">
         <f ca="1">-$C$68+$H$76</f>
-        <v>2.3771075579837424</v>
+        <v>2.2474998296714244</v>
       </c>
       <c r="K76" s="3">
         <f t="shared" si="0"/>
@@ -21490,7 +21490,7 @@
       </c>
       <c r="H77" s="30">
         <f ca="1">MIN($N$123, $N$124)</f>
-        <v>21.495936780292737</v>
+        <v>21.877673873895816</v>
       </c>
       <c r="K77" s="3">
         <f t="shared" ref="K77:K167" si="2">ROW(K77)</f>
@@ -21595,7 +21595,7 @@
       </c>
       <c r="H81" s="30">
         <f ca="1">IF($C$25&gt;=$C$71-5,$H$54*$N$114-$C$20*$N$113, "-")</f>
-        <v>0.23613623834420849</v>
+        <v>0.23529084292472469</v>
       </c>
       <c r="K81" s="3">
         <f t="shared" si="2"/>
@@ -21622,7 +21622,7 @@
       </c>
       <c r="H82" s="30">
         <f ca="1">IF($C$25&gt;=$C$71-4,$H$55*$N$114-($C$20+$C21)*$N$113, "-")</f>
-        <v>0.16515537313498907</v>
+        <v>0.16414228491088156</v>
       </c>
       <c r="K82" s="3">
         <f t="shared" si="2"/>
@@ -21649,7 +21649,7 @@
       </c>
       <c r="H83" s="30">
         <f ca="1">IF($C$25&gt;=$C$71-3,$H$56*$N$114-($C$20+2*$C$21)*$N$113, "-")</f>
-        <v>4.930486789530697E-2</v>
+        <v>4.8129948049920657E-2</v>
       </c>
       <c r="K83" s="3">
         <f t="shared" si="2"/>
@@ -21664,7 +21664,7 @@
       </c>
       <c r="N83" s="46">
         <f>IF($C$25&gt;=3,SQRT($C$3^2-$N$43^2),"-")</f>
-        <v>8917.3132326951491</v>
+        <v>8917.9860557190823</v>
       </c>
     </row>
     <row r="84" spans="6:14" x14ac:dyDescent="0.4">
@@ -21677,7 +21677,7 @@
       </c>
       <c r="H84" s="30">
         <f ca="1">IF($C$25&gt;=$C$71-2,$H$57*$N$114-($C$20+3*$C$21)*$N$113, "-")</f>
-        <v>-0.11140580074584783</v>
+        <v>-0.11273737020309937</v>
       </c>
       <c r="K84" s="3">
         <f t="shared" si="2"/>
@@ -21692,7 +21692,7 @@
       </c>
       <c r="N84" s="46">
         <f>IF($C$25&gt;=4,SQRT($C$3^2-$N$44^2),"-")</f>
-        <v>8917.9860557190823</v>
+        <v>8918.6139780797785</v>
       </c>
     </row>
     <row r="85" spans="6:14" x14ac:dyDescent="0.4">
@@ -21720,7 +21720,7 @@
       </c>
       <c r="N85" s="46">
         <f>IF($C$25&gt;=5,SQRT($C$3^2-$N$45^2),"-")</f>
-        <v>8918.6139780797785</v>
+        <v>8919.1970092604188</v>
       </c>
     </row>
     <row r="86" spans="6:14" x14ac:dyDescent="0.4">
@@ -21748,7 +21748,7 @@
       </c>
       <c r="N86" s="46">
         <f>IF($C$25&gt;=6,SQRT($C$3^2-$N$46^2),"-")</f>
-        <v>8919.1970092604188</v>
+        <v>8919.7351580638315</v>
       </c>
     </row>
     <row r="87" spans="6:14" x14ac:dyDescent="0.4">
@@ -21760,7 +21760,7 @@
       </c>
       <c r="H87" s="30">
         <f ca="1">$H$60*$N$114-($C$20+($C$25-2)*$C$21)*$N$113</f>
-        <v>-0.31696783604237844</v>
+        <v>-0.31845155167636996</v>
       </c>
       <c r="K87" s="3">
         <f t="shared" si="2"/>
@@ -21787,7 +21787,7 @@
       </c>
       <c r="H88" s="30">
         <f ca="1">$H$61*$N$114-($C$20+($C$25-1)*$C$21)*$N$113</f>
-        <v>-0.56737312047669697</v>
+        <v>-0.56900515685961839</v>
       </c>
       <c r="K88" s="3">
         <f t="shared" si="2"/>
@@ -21815,7 +21815,7 @@
       </c>
       <c r="H89" s="30">
         <f ca="1">IF($C$25&gt;=$C$71-5,$H$54*$N$113+$C$20*$N$114, "-")</f>
-        <v>90.071009208980442</v>
+        <v>90.063193576111303</v>
       </c>
       <c r="K89" s="3">
         <f t="shared" si="2"/>
@@ -21829,7 +21829,7 @@
       </c>
       <c r="N89" s="47">
         <f>SQRT($C$3^2-$N$49^2)</f>
-        <v>8919.7351580638315</v>
+        <v>8920.2284326131467</v>
       </c>
     </row>
     <row r="90" spans="6:14" x14ac:dyDescent="0.4">
@@ -21842,7 +21842,7 @@
       </c>
       <c r="H90" s="30">
         <f ca="1">IF($C$25&gt;=$C$71-4,$H$55*$N$113+($C$20+$C$21)*$N$114, "-")</f>
-        <v>110.08219739305159</v>
+        <v>110.07292181948721</v>
       </c>
       <c r="K90" s="3">
         <f t="shared" si="2"/>
@@ -21856,7 +21856,7 @@
       </c>
       <c r="N90" s="47">
         <f>SQRT($C$3^2-$N$50^2)</f>
-        <v>8920.2284326131467</v>
+        <v>8920.6768403524184</v>
       </c>
     </row>
     <row r="91" spans="6:14" x14ac:dyDescent="0.4">
@@ -21869,7 +21869,7 @@
       </c>
       <c r="H91" s="30">
         <f ca="1">IF($C$25&gt;=$C$71-3,$H$56*$N$113+($C$20+2*$C$21)*$N$114, "-")</f>
-        <v>130.09171675638208</v>
+        <v>130.08108181723048</v>
       </c>
       <c r="K91" s="3">
         <f t="shared" si="2"/>
@@ -21897,7 +21897,7 @@
       </c>
       <c r="H92" s="30">
         <f ca="1">IF($C$25&gt;=$C$71-2,$H$57*$N$113+($C$20+3*$C$21)*$N$114, "-")</f>
-        <v>150.09956765143286</v>
+        <v>150.08767387686254</v>
       </c>
       <c r="K92" s="3">
         <f t="shared" si="2"/>
@@ -21980,7 +21980,7 @@
       </c>
       <c r="H95" s="30">
         <f ca="1">$H$60*$N$113+($C$20+($C$25-2)*$C$21)*$N$114</f>
-        <v>170.10575040537816</v>
+        <v>170.09269828215989</v>
       </c>
       <c r="K95" s="3">
         <f t="shared" si="2"/>
@@ -22007,7 +22007,7 @@
       </c>
       <c r="H96" s="30">
         <f ca="1">$H$61*$N$113+($C$20+($C$25-1)*$C$21)*$N$114</f>
-        <v>190.11026532013003</v>
+        <v>190.09615529317597</v>
       </c>
       <c r="K96" s="3">
         <f t="shared" si="2"/>
@@ -22089,11 +22089,11 @@
       </c>
       <c r="H99" s="30">
         <f>$H$3</f>
-        <v>500.0159494817317</v>
+        <v>480.0159494817317</v>
       </c>
       <c r="I99" s="30">
         <f>$C$67+H99</f>
-        <v>-649.95805051826824</v>
+        <v>-669.95805051826824</v>
       </c>
       <c r="K99" s="3">
         <f t="shared" si="2"/>
@@ -22123,11 +22123,11 @@
       </c>
       <c r="H100" s="30">
         <f ca="1">$H$98*$N$114+$H$99*$N$113</f>
-        <v>7.4967340513192653</v>
+        <v>5.6808328434610509</v>
       </c>
       <c r="I100" s="30">
         <f ca="1">$C$66+H100</f>
-        <v>-542.5222659486808</v>
+        <v>-544.33816715653893</v>
       </c>
       <c r="K100" s="3">
         <f t="shared" si="2"/>
@@ -22157,11 +22157,11 @@
       </c>
       <c r="H101" s="30">
         <f ca="1">-$H$98*$N$113+$H$99*$N$114</f>
-        <v>500.08284087707057</v>
+        <v>480.1105486448439</v>
       </c>
       <c r="I101" s="30">
         <f ca="1">$C$67+H101</f>
-        <v>-649.89115912292937</v>
+        <v>-669.86345135515603</v>
       </c>
       <c r="K101" s="3">
         <f t="shared" si="2"/>
@@ -22188,7 +22188,7 @@
       </c>
       <c r="H102" s="30">
         <f ca="1">$H$100-$H$98</f>
-        <v>18.591734051319293</v>
+        <v>16.775832843461078</v>
       </c>
       <c r="K102" s="3">
         <f t="shared" si="2"/>
@@ -22215,7 +22215,7 @@
       </c>
       <c r="H103" s="30">
         <f ca="1">$H$101-$H$99</f>
-        <v>6.6891395338871007E-2</v>
+        <v>9.4599163112206952E-2</v>
       </c>
       <c r="K103" s="3">
         <f t="shared" si="2"/>
@@ -22342,7 +22342,7 @@
       </c>
       <c r="N109" s="2">
         <f ca="1">SQRT($N$108^2-$N$43^2)</f>
-        <v>8995.6564181061131</v>
+        <v>8996.3233819496345</v>
       </c>
     </row>
     <row r="110" spans="5:14" x14ac:dyDescent="0.4">
@@ -22358,7 +22358,7 @@
       </c>
       <c r="N110" s="2">
         <f ca="1">SQRT($N$107^2-$C$4^2)</f>
-        <v>8992.3094054643298</v>
+        <v>8993.1767715086226</v>
       </c>
     </row>
     <row r="111" spans="5:14" x14ac:dyDescent="0.4">
@@ -22374,7 +22374,7 @@
       </c>
       <c r="N111" s="2">
         <f ca="1">IF($N$109&gt;$N$110, ($N$109-$N$110)/$C$20, 0)</f>
-        <v>3.7189029353147718E-2</v>
+        <v>3.4962338233466048E-2</v>
       </c>
     </row>
     <row r="112" spans="5:14" x14ac:dyDescent="0.4">
@@ -22390,7 +22390,7 @@
       </c>
       <c r="N112" s="2">
         <f ca="1">ATAN($N$111)</f>
-        <v>3.7171899126953054E-2</v>
+        <v>3.4948103091703542E-2</v>
       </c>
     </row>
     <row r="113" spans="11:14" x14ac:dyDescent="0.4">
@@ -22406,7 +22406,7 @@
       </c>
       <c r="N113" s="2">
         <f ca="1">SIN(RADIANS($H$73))</f>
-        <v>3.7166950783010577E-2</v>
+        <v>3.4934382002123322E-2</v>
       </c>
     </row>
     <row r="114" spans="11:14" x14ac:dyDescent="0.4">
@@ -22422,7 +22422,7 @@
       </c>
       <c r="N114" s="2">
         <f ca="1">COS(RADIANS($H$73))</f>
-        <v>0.9993090701927474</v>
+        <v>0.99938960818798273</v>
       </c>
     </row>
     <row r="115" spans="11:14" x14ac:dyDescent="0.4">
@@ -22470,7 +22470,7 @@
       </c>
       <c r="N117" s="2">
         <f ca="1">SQRT($N$116^2-$N$50^2)</f>
-        <v>8842.1260074066122</v>
+        <v>8842.5783757259615</v>
       </c>
     </row>
     <row r="118" spans="11:14" x14ac:dyDescent="0.4">
@@ -22486,7 +22486,7 @@
       </c>
       <c r="N118" s="2">
         <f ca="1">SQRT($N$115^2-$N$43^2)</f>
-        <v>8838.9692164060452</v>
+        <v>8839.6480025266683</v>
       </c>
     </row>
     <row r="119" spans="11:14" x14ac:dyDescent="0.4">
@@ -22499,7 +22499,7 @@
       </c>
       <c r="N119" s="2">
         <f ca="1">($N117-$N118)/($N$43-$N$50)</f>
-        <v>3.1567910005669546E-2</v>
+        <v>2.9303731992931716E-2</v>
       </c>
     </row>
     <row r="120" spans="11:14" x14ac:dyDescent="0.4">
@@ -22515,7 +22515,7 @@
       </c>
       <c r="N120" s="2">
         <f ca="1">ATAN($N$119)</f>
-        <v>3.1557430117010586E-2</v>
+        <v>2.9295348521930362E-2</v>
       </c>
     </row>
     <row r="121" spans="11:14" x14ac:dyDescent="0.4">
@@ -22563,7 +22563,7 @@
       </c>
       <c r="N123" s="2">
         <f ca="1">$H$70/2-$H$60-$N$121/2</f>
-        <v>21.495936780292737</v>
+        <v>21.877673873895816</v>
       </c>
     </row>
     <row r="124" spans="11:14" x14ac:dyDescent="0.4">
@@ -22579,7 +22579,7 @@
       </c>
       <c r="N124" s="2">
         <f ca="1">$H$70/2-$H$61-$N$122/2</f>
-        <v>29.502662230977563</v>
+        <v>29.9292661346241</v>
       </c>
     </row>
     <row r="125" spans="11:14" x14ac:dyDescent="0.4">

</xml_diff>